<commit_message>
Updates for Slideshow version 3.11.0
</commit_message>
<xml_diff>
--- a/backend/localization.xlsx
+++ b/backend/localization.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mimac\Documents\NetBeansProjects\slideshow-localization\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{684E40FC-5A66-4E9B-A7C7-5F06CEB63C7D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B869A0F6-B067-4875-BE1B-DD72CD749040}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3764" yWindow="3764" windowWidth="36784" windowHeight="14642" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-10479" yWindow="4691" windowWidth="20987" windowHeight="14642" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="properties" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4186" uniqueCount="4008">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4263" uniqueCount="4085">
   <si>
     <t>keys</t>
   </si>
@@ -10499,9 +10499,6 @@
     <t>Visita https://slideshow.digital/documentation per suggerimenti su come utilizzare più funzioni di Slideshow.</t>
   </si>
   <si>
-    <t>Odwiedź https://slideshow.digital/documentation, aby uzyskać wskazówki, jak korzystać z większej liczby funkcji pokazu slajdów.</t>
-  </si>
-  <si>
     <t>Tipy ako využiť viac funkcií Slideshow môžete nájsť na https://slideshow.digital/documentation.</t>
   </si>
   <si>
@@ -12072,6 +12069,240 @@
   </si>
   <si>
     <t>user</t>
+  </si>
+  <si>
+    <t>weather_text</t>
+  </si>
+  <si>
+    <t>weather_text_help</t>
+  </si>
+  <si>
+    <t>Text template</t>
+  </si>
+  <si>
+    <t>Template for weather information text. Must contain 2x "%d" placeholder for temperature range. All characters except date formatting have to be enclosed within single quotes (').&lt;br&gt;See &lt;a href="https://docs.oracle.com/javase/7/docs/api/java/text/SimpleDateFormat.html"&gt;https://docs.oracle.com/javase/7/docs/api/java/text/SimpleDateFormat.html&lt;/a&gt; for date format specification.</t>
+  </si>
+  <si>
+    <t>Šablóna textu</t>
+  </si>
+  <si>
+    <t>Textvorlage</t>
+  </si>
+  <si>
+    <t>Vorlage für Wetterinformationstext. Muss 2x Platzhalter "%d" für den Temperaturbereich enthalten. Alle Zeichen außer der Datumsformatierung müssen in einfache Anführungszeichen (') gesetzt werden.&lt;br&gt;Siehe &lt;a href="https://docs.oracle.com/javase/7/docs/api/java/text/SimpleDateFormat.html"&gt;https://docs.oracle.com/javase/7/docs/api/java/text/SimpleDateFormat.html&lt;/a&gt; für die Angabe des Datumsformats.</t>
+  </si>
+  <si>
+    <t>Szablon tekstowy</t>
+  </si>
+  <si>
+    <t>Szablon tekstu informacji o pogodzie. Musi zawierać symbol zastępczy 2x "%d" dla zakresu temperatur. Wszystkie znaki poza formatowaniem daty muszą być ujęte w pojedyncze cudzysłowy ('). &lt;br&gt; Zobacz &lt;a href="https://docs.oracle.com/javase/7/docs/api/java/text/SimpleDateFormat.html"&gt; https://docs.oracle.com/javase/7/docs/api/java/text/SimpleDateFormat.html&lt;/a&gt; w celu uzyskania specyfikacji formatu daty.</t>
+  </si>
+  <si>
+    <t>Modello di testo</t>
+  </si>
+  <si>
+    <t>Modello per il testo delle informazioni meteorologiche. Deve contenere 2x segnaposto "%d" per l'intervallo di temperatura. Tutti i caratteri tranne la formattazione della data devono essere racchiusi tra virgolette singole (').&lt;br&gt;Vedere &lt;a href="https://docs.oracle.com/javase/7/docs/api/java/text/SimpleDateFormat.html"&gt;https://docs.oracle.com/javase/7/docs/api/java/text/SimpleDateFormat.html&lt;/a&gt; per la specifica del formato della data.</t>
+  </si>
+  <si>
+    <t>Šablóna pre informácie o počasí. Musí obsahovať 2x zástupný symbol "%d", ktorý bude nahradený teplotou. Všetky znaky okrem formátovania dátumu musia byť uzavreté v apostofoch ('). Špecifikácia formátu dátumu je dostupná na &lt;a href="https://docs.oracle.com/javase/7/docs/api/java/text/SimpleDateFormat.html"&gt; https://docs.oracle.com/javase/7/docs/api/java/text/SimpleDateFormat.html&lt;/a&gt;.</t>
+  </si>
+  <si>
+    <t>Šablona textu</t>
+  </si>
+  <si>
+    <t>Šablona pro informace o počasí. Musí obsahovat 2x zástupný symbol "%d", který bude nahrazen teplotou. Všechny znaky kromě formátování data musí být uzavřeny v apostofoch ('). Specifikace formátu data je dostupná na &lt;a href="https://docs.oracle.com/javase/7/docs/api/java/text/SimpleDateFormat.html"&gt;https://docs.oracle.com/javase/7/docs/api/java/text/SimpleDateFormat.html&lt;/a&gt;.</t>
+  </si>
+  <si>
+    <t>Zrušiť nastavenie Slideshow ako Launcher aplikácie</t>
+  </si>
+  <si>
+    <t>Deaktivierte Slideshow als Launcher-App</t>
+  </si>
+  <si>
+    <t>Annulla impostazione Slideshow come app di avvio</t>
+  </si>
+  <si>
+    <t>Usuń Slideshow jako aplikację uruchamiającą</t>
+  </si>
+  <si>
+    <t>Zrušit nastavení Slideshow jako Launcher aplikace</t>
+  </si>
+  <si>
+    <t>Odwiedź https://slideshow.digital/documentation, aby uzyskać wskazówki, jak korzystać z większej liczby funkcji Slideshow.</t>
+  </si>
+  <si>
+    <t>Zrušenie Launcher aplikácie bolo úspešné</t>
+  </si>
+  <si>
+    <t>Disinserimento dell'applicazione Launcher è riuscito</t>
+  </si>
+  <si>
+    <t>Rozbrajanie aplikacji Launcher powiodło się</t>
+  </si>
+  <si>
+    <t>Das Deaktivieren der Launcher-Anwendung war erfolgreich</t>
+  </si>
+  <si>
+    <t>Zrušení Launcher aplikace bylo úspěšné</t>
+  </si>
+  <si>
+    <t>android_settings</t>
+  </si>
+  <si>
+    <t>Android settings</t>
+  </si>
+  <si>
+    <t>Nastavenia Androidu</t>
+  </si>
+  <si>
+    <t>Nastavení Androidu</t>
+  </si>
+  <si>
+    <t>Android-Einstellungen</t>
+  </si>
+  <si>
+    <t>Ustawienia Androida</t>
+  </si>
+  <si>
+    <t>Impostazioni Android</t>
+  </si>
+  <si>
+    <t>launcher_clear</t>
+  </si>
+  <si>
+    <t>launcher_clear_success</t>
+  </si>
+  <si>
+    <t>launcher_set</t>
+  </si>
+  <si>
+    <t>launcher_set_help</t>
+  </si>
+  <si>
+    <t>Nastaviť Slideshow ako Launcher aplikáciu</t>
+  </si>
+  <si>
+    <t>Nastavit Slideshow jako Launcher aplikaci</t>
+  </si>
+  <si>
+    <t>Zobrazí seznam aplikací, kde můžete vybrat Slideshow jako Launcher aplikaci tohoto zařízení. Použijte pouze pokud toto zařízení bude určeno převážně pro Slideshow.</t>
+  </si>
+  <si>
+    <t>Imposta Slideshow come applicazione di avvio</t>
+  </si>
+  <si>
+    <t>Apre un elenco di app, in cui è possibile impostare Slideshow come app Launcher di questo dispositivo. Utilizzare solo dispositivi dedicati alla Slideshow.</t>
+  </si>
+  <si>
+    <t>Ustaw Slideshow jako aplikację uruchamiającą</t>
+  </si>
+  <si>
+    <t>Otwiera listę aplikacji, w których możesz ustawić Slideshow jako aplikację uruchamiającą na tym urządzeniu. Używaj tylko urządzeń przeznaczonych do Slideshow.</t>
+  </si>
+  <si>
+    <t>Set Slideshow als Launcher-Anwendung</t>
+  </si>
+  <si>
+    <t>Öffnet eine Liste von Apps, in der Sie die Slideshow als Launcher-App dieses Geräts festlegen können. Verwenden Sie nur Geräte, die für die Slideshow vorgesehen sind.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Opens a dialog with list of apps, where you can set Slideshow as this device's Launcher / Home app. If no dialog is displayed, please change the Home app via Android settings. Use only of devices dedicated to Slideshow. </t>
+  </si>
+  <si>
+    <t>Zobrazí zoznam aplikácií, kde môžete vybrať Slideshow ako Launcher aplikáciu tohto zariadenia. Ak sa nezobrazí zoznam, zmenu môžete spraviť cez nastavenia Androidu. Použite len ak toto zariadenie bude určené prevažne pre Slideshow.</t>
+  </si>
+  <si>
+    <t>Set Slideshow as Launcher / Home application</t>
+  </si>
+  <si>
+    <t>Unsetting Launcher / Home application was successful</t>
+  </si>
+  <si>
+    <t>Unset Slideshow as Launcher / Home application</t>
+  </si>
+  <si>
+    <t>screen_login_required</t>
+  </si>
+  <si>
+    <t>screen_login_required_help</t>
+  </si>
+  <si>
+    <t>Login is required for this action</t>
+  </si>
+  <si>
+    <t>Please enter username and password (the same as for the web interface) or contact your administrator</t>
+  </si>
+  <si>
+    <t>Do wykonania tej czynności wymagane jest logowanie</t>
+  </si>
+  <si>
+    <t>Wprowadź nazwę użytkownika i hasło (takie same jak w przypadku interfejsu internetowego) lub skontaktuj się z administratorem</t>
+  </si>
+  <si>
+    <t>L'accesso è richiesto per questa azione</t>
+  </si>
+  <si>
+    <t>Inserisci nome utente e password (la stessa dell'interfaccia web) o contatta l'amministratore</t>
+  </si>
+  <si>
+    <t>Für diese Aktion ist ein Login erforderlich</t>
+  </si>
+  <si>
+    <t>Bitte geben Sie den Benutzernamen und das Passwort ein (wie für die Weboberfläche) oder wenden Sie sich an Ihren Administrator</t>
+  </si>
+  <si>
+    <t>Pre vykonanie tejto akcie je potrebné prihlásenie</t>
+  </si>
+  <si>
+    <t>Prosím zadajte meno a heslo (rovnaké ako na webové rozhranie), alebo kontaktujte svojho administrátora</t>
+  </si>
+  <si>
+    <t>Pro provedení této akce je třeba přihlášení</t>
+  </si>
+  <si>
+    <t>Prosím zadejte jméno a heslo (stejné jako na webové rozhraní) nebo kontaktujte svého administrátora</t>
+  </si>
+  <si>
+    <t>password_protect_screen</t>
+  </si>
+  <si>
+    <t>password_protect_screen_help</t>
+  </si>
+  <si>
+    <t>Protect screen with password</t>
+  </si>
+  <si>
+    <t>Entering password will be required for any action on the devices's screen (opening on-screen menu, opening settings, etc.). Use the same username and password as for the web interface.</t>
+  </si>
+  <si>
+    <t>Bildschirm mit Passwort schützen</t>
+  </si>
+  <si>
+    <t>Die Eingabe eines Kennworts ist für alle Aktionen auf dem Bildschirm des Geräts erforderlich (Öffnen des Bildschirmmenüs, Öffnen der Einstellungen usw.). Verwenden Sie denselben Benutzernamen und dasselbe Passwort wie für die Weboberfläche.</t>
+  </si>
+  <si>
+    <t>Proteggi lo schermo con una password</t>
+  </si>
+  <si>
+    <t>L'inserimento della password sarà richiesto per qualsiasi azione sullo schermo del dispositivo (apertura del menu su schermo, apertura delle impostazioni, ecc.). Utilizza lo stesso nome utente e password dell'interfaccia web.</t>
+  </si>
+  <si>
+    <t>Chroń ekran hasłem</t>
+  </si>
+  <si>
+    <t>Podanie hasła będzie wymagane przy każdej czynności na ekranie urządzeń (otwieranie menu ekranowego, otwieranie ustawień itp.). Użyj tej samej nazwy użytkownika i hasła, co w przypadku interfejsu internetowego.</t>
+  </si>
+  <si>
+    <t>Zabezpečiť obrazovku heslom</t>
+  </si>
+  <si>
+    <t>Na akciu na obrazovke zariadenia (otvorenie menu, otvorenie nastavení, atď.) bude vyžadované heslo. Použite rovnaké heslo ako do webového rozhrania.</t>
+  </si>
+  <si>
+    <t>Zajistit obrazovku heslem</t>
+  </si>
+  <si>
+    <t>Na akci na obrazovce zařízení (otevření menu, otevření nastavení atd.) dude vyžadováno heslo. Použijte stejné heslo jako do webového rozhraní.</t>
   </si>
 </sst>
 </file>
@@ -12118,11 +12349,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -12437,13 +12669,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G598"/>
+  <dimension ref="A1:G609"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B95" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B582" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B115" sqref="B115"/>
+      <selection pane="bottomRight" activeCell="E606" sqref="E606"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -12549,22 +12781,22 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>3801</v>
+        <v>3800</v>
       </c>
       <c r="C5" t="s">
+        <v>3795</v>
+      </c>
+      <c r="D5" t="s">
+        <v>3797</v>
+      </c>
+      <c r="E5" t="s">
+        <v>3799</v>
+      </c>
+      <c r="F5" t="s">
+        <v>3798</v>
+      </c>
+      <c r="G5" t="s">
         <v>3796</v>
-      </c>
-      <c r="D5" t="s">
-        <v>3798</v>
-      </c>
-      <c r="E5" t="s">
-        <v>3800</v>
-      </c>
-      <c r="F5" t="s">
-        <v>3799</v>
-      </c>
-      <c r="G5" t="s">
-        <v>3797</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -12785,7 +13017,7 @@
         <v>1028</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>3512</v>
+        <v>3511</v>
       </c>
       <c r="E15" t="s">
         <v>1954</v>
@@ -12894,7 +13126,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>3811</v>
+        <v>3810</v>
       </c>
       <c r="C20" t="s">
         <v>1032</v>
@@ -13170,7 +13402,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>3810</v>
+        <v>3809</v>
       </c>
       <c r="C32" t="s">
         <v>1044</v>
@@ -13377,13 +13609,13 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>3809</v>
+        <v>3808</v>
       </c>
       <c r="C41" t="s">
         <v>1052</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>3513</v>
+        <v>3512</v>
       </c>
       <c r="E41" t="s">
         <v>1980</v>
@@ -13544,7 +13776,7 @@
         <v>1059</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>3514</v>
+        <v>3513</v>
       </c>
       <c r="E48" t="s">
         <v>1987</v>
@@ -13567,7 +13799,7 @@
         <v>1060</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>3515</v>
+        <v>3514</v>
       </c>
       <c r="E49" t="s">
         <v>1988</v>
@@ -13584,7 +13816,7 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>3808</v>
+        <v>3807</v>
       </c>
       <c r="C50" t="s">
         <v>1061</v>
@@ -13774,7 +14006,7 @@
         <v>1069</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>3516</v>
+        <v>3515</v>
       </c>
       <c r="E58" t="s">
         <v>1997</v>
@@ -14044,7 +14276,7 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>3807</v>
+        <v>3806</v>
       </c>
       <c r="C70" t="s">
         <v>1081</v>
@@ -14090,7 +14322,7 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>3916</v>
+        <v>3915</v>
       </c>
       <c r="C72" t="s">
         <v>1083</v>
@@ -14136,7 +14368,7 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>3806</v>
+        <v>3805</v>
       </c>
       <c r="C74" t="s">
         <v>1085</v>
@@ -14211,7 +14443,7 @@
         <v>1088</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>3517</v>
+        <v>3516</v>
       </c>
       <c r="E77" t="s">
         <v>2015</v>
@@ -14579,7 +14811,7 @@
         <v>1102</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>3518</v>
+        <v>3517</v>
       </c>
       <c r="E93" t="s">
         <v>2029</v>
@@ -14665,7 +14897,7 @@
         <v>96</v>
       </c>
       <c r="B97" t="s">
-        <v>3805</v>
+        <v>3804</v>
       </c>
       <c r="C97" t="s">
         <v>1106</v>
@@ -15007,7 +15239,7 @@
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>3883</v>
+        <v>3882</v>
       </c>
       <c r="B112" t="s">
         <v>640</v>
@@ -15030,7 +15262,7 @@
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>3884</v>
+        <v>3883</v>
       </c>
       <c r="B113" t="s">
         <v>641</v>
@@ -15053,7 +15285,7 @@
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>3885</v>
+        <v>3884</v>
       </c>
       <c r="B114" t="s">
         <v>642</v>
@@ -15076,7 +15308,7 @@
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>4007</v>
+        <v>4006</v>
       </c>
       <c r="B115" t="s">
         <v>642</v>
@@ -15148,7 +15380,7 @@
         <v>113</v>
       </c>
       <c r="B118" t="s">
-        <v>3812</v>
+        <v>3811</v>
       </c>
       <c r="C118" t="s">
         <v>1125</v>
@@ -15171,7 +15403,7 @@
         <v>114</v>
       </c>
       <c r="B119" t="s">
-        <v>3813</v>
+        <v>3812</v>
       </c>
       <c r="C119" t="s">
         <v>1126</v>
@@ -15269,7 +15501,7 @@
         <v>1130</v>
       </c>
       <c r="D123" s="2" t="s">
-        <v>3519</v>
+        <v>3518</v>
       </c>
       <c r="E123" t="s">
         <v>2056</v>
@@ -15292,7 +15524,7 @@
         <v>1059</v>
       </c>
       <c r="D124" s="2" t="s">
-        <v>3514</v>
+        <v>3513</v>
       </c>
       <c r="E124" t="s">
         <v>1987</v>
@@ -15309,7 +15541,7 @@
         <v>120</v>
       </c>
       <c r="B125" t="s">
-        <v>3803</v>
+        <v>3802</v>
       </c>
       <c r="C125" t="s">
         <v>1131</v>
@@ -15700,7 +15932,7 @@
         <v>137</v>
       </c>
       <c r="B142" t="s">
-        <v>3814</v>
+        <v>3813</v>
       </c>
       <c r="C142" t="s">
         <v>1148</v>
@@ -15746,7 +15978,7 @@
         <v>139</v>
       </c>
       <c r="B144" t="s">
-        <v>3815</v>
+        <v>3814</v>
       </c>
       <c r="C144" t="s">
         <v>3419</v>
@@ -15792,7 +16024,7 @@
         <v>141</v>
       </c>
       <c r="B146" t="s">
-        <v>3816</v>
+        <v>3815</v>
       </c>
       <c r="C146" t="s">
         <v>1151</v>
@@ -15815,7 +16047,7 @@
         <v>142</v>
       </c>
       <c r="B147" t="s">
-        <v>3817</v>
+        <v>3816</v>
       </c>
       <c r="C147" t="s">
         <v>1152</v>
@@ -15982,7 +16214,7 @@
         <v>1159</v>
       </c>
       <c r="D154" s="2" t="s">
-        <v>3520</v>
+        <v>3519</v>
       </c>
       <c r="E154" t="s">
         <v>2085</v>
@@ -16005,7 +16237,7 @@
         <v>1160</v>
       </c>
       <c r="D155" s="3" t="s">
-        <v>3521</v>
+        <v>3520</v>
       </c>
       <c r="E155" t="s">
         <v>2086</v>
@@ -16022,7 +16254,7 @@
         <v>151</v>
       </c>
       <c r="B156" t="s">
-        <v>3818</v>
+        <v>3817</v>
       </c>
       <c r="C156" t="s">
         <v>1161</v>
@@ -16074,7 +16306,7 @@
         <v>1163</v>
       </c>
       <c r="D158" s="2" t="s">
-        <v>3522</v>
+        <v>3521</v>
       </c>
       <c r="E158" t="s">
         <v>2089</v>
@@ -16206,7 +16438,7 @@
         <v>159</v>
       </c>
       <c r="B164" t="s">
-        <v>3802</v>
+        <v>3801</v>
       </c>
       <c r="C164" t="s">
         <v>1169</v>
@@ -16304,7 +16536,7 @@
         <v>1173</v>
       </c>
       <c r="D168" s="2" t="s">
-        <v>3523</v>
+        <v>3522</v>
       </c>
       <c r="E168" t="s">
         <v>2099</v>
@@ -16551,22 +16783,22 @@
         <v>174</v>
       </c>
       <c r="B179" t="s">
-        <v>3898</v>
+        <v>3897</v>
       </c>
       <c r="C179" t="s">
+        <v>3893</v>
+      </c>
+      <c r="D179" s="2" t="s">
+        <v>3896</v>
+      </c>
+      <c r="E179" t="s">
         <v>3894</v>
       </c>
-      <c r="D179" s="2" t="s">
-        <v>3897</v>
-      </c>
-      <c r="E179" t="s">
+      <c r="F179" t="s">
         <v>3895</v>
       </c>
-      <c r="F179" t="s">
-        <v>3896</v>
-      </c>
       <c r="G179" t="s">
-        <v>3893</v>
+        <v>3892</v>
       </c>
     </row>
     <row r="180" spans="1:7" x14ac:dyDescent="0.25">
@@ -16574,10 +16806,10 @@
         <v>175</v>
       </c>
       <c r="B180" t="s">
-        <v>3900</v>
+        <v>3899</v>
       </c>
       <c r="C180" t="s">
-        <v>3899</v>
+        <v>3898</v>
       </c>
       <c r="D180" s="2" t="s">
         <v>1656</v>
@@ -16589,7 +16821,7 @@
         <v>2612</v>
       </c>
       <c r="G180" t="s">
-        <v>3901</v>
+        <v>3900</v>
       </c>
     </row>
     <row r="181" spans="1:7" x14ac:dyDescent="0.25">
@@ -16603,7 +16835,7 @@
         <v>1183</v>
       </c>
       <c r="D181" s="2" t="s">
-        <v>3524</v>
+        <v>3523</v>
       </c>
       <c r="E181" t="s">
         <v>2109</v>
@@ -16626,7 +16858,7 @@
         <v>1184</v>
       </c>
       <c r="D182" s="2" t="s">
-        <v>3525</v>
+        <v>3524</v>
       </c>
       <c r="E182" t="s">
         <v>2110</v>
@@ -16649,10 +16881,10 @@
         <v>1185</v>
       </c>
       <c r="D183" s="2" t="s">
-        <v>3557</v>
+        <v>3556</v>
       </c>
       <c r="E183" t="s">
-        <v>3559</v>
+        <v>3558</v>
       </c>
       <c r="F183" t="s">
         <v>2615</v>
@@ -16689,7 +16921,7 @@
         <v>180</v>
       </c>
       <c r="B185" t="s">
-        <v>3819</v>
+        <v>3818</v>
       </c>
       <c r="C185" t="s">
         <v>1187</v>
@@ -16804,7 +17036,7 @@
         <v>185</v>
       </c>
       <c r="B190" t="s">
-        <v>3820</v>
+        <v>3819</v>
       </c>
       <c r="C190" t="s">
         <v>1192</v>
@@ -16873,7 +17105,7 @@
         <v>188</v>
       </c>
       <c r="B193" t="s">
-        <v>3821</v>
+        <v>3820</v>
       </c>
       <c r="C193" t="s">
         <v>1194</v>
@@ -16942,7 +17174,7 @@
         <v>191</v>
       </c>
       <c r="B196" t="s">
-        <v>3822</v>
+        <v>3821</v>
       </c>
       <c r="C196" t="s">
         <v>1197</v>
@@ -16957,7 +17189,7 @@
         <v>2627</v>
       </c>
       <c r="G196" t="s">
-        <v>3823</v>
+        <v>3822</v>
       </c>
     </row>
     <row r="197" spans="1:7" x14ac:dyDescent="0.25">
@@ -16988,7 +17220,7 @@
         <v>193</v>
       </c>
       <c r="B198" t="s">
-        <v>3824</v>
+        <v>3823</v>
       </c>
       <c r="C198" t="s">
         <v>1199</v>
@@ -17155,7 +17387,7 @@
         <v>1206</v>
       </c>
       <c r="D205" s="2" t="s">
-        <v>3526</v>
+        <v>3525</v>
       </c>
       <c r="E205" t="s">
         <v>2130</v>
@@ -17287,7 +17519,7 @@
         <v>206</v>
       </c>
       <c r="B211" t="s">
-        <v>3825</v>
+        <v>3824</v>
       </c>
       <c r="C211" t="s">
         <v>1212</v>
@@ -17310,7 +17542,7 @@
         <v>207</v>
       </c>
       <c r="B212" t="s">
-        <v>3826</v>
+        <v>3825</v>
       </c>
       <c r="C212" t="s">
         <v>1213</v>
@@ -17494,7 +17726,7 @@
         <v>215</v>
       </c>
       <c r="B220" t="s">
-        <v>3827</v>
+        <v>3826</v>
       </c>
       <c r="C220" t="s">
         <v>1221</v>
@@ -17747,7 +17979,7 @@
         <v>226</v>
       </c>
       <c r="B231" t="s">
-        <v>3828</v>
+        <v>3827</v>
       </c>
       <c r="C231" t="s">
         <v>1232</v>
@@ -17756,7 +17988,7 @@
         <v>1697</v>
       </c>
       <c r="E231" t="s">
-        <v>3560</v>
+        <v>3559</v>
       </c>
       <c r="F231" t="s">
         <v>2662</v>
@@ -18075,7 +18307,7 @@
         <v>1245</v>
       </c>
       <c r="D245" s="2" t="s">
-        <v>3527</v>
+        <v>3526</v>
       </c>
       <c r="E245" t="s">
         <v>2167</v>
@@ -18167,7 +18399,7 @@
         <v>1249</v>
       </c>
       <c r="D249" s="2" t="s">
-        <v>3528</v>
+        <v>3527</v>
       </c>
       <c r="E249" t="s">
         <v>2171</v>
@@ -18506,7 +18738,7 @@
         <v>259</v>
       </c>
       <c r="B264" t="s">
-        <v>3829</v>
+        <v>3828</v>
       </c>
       <c r="C264" t="s">
         <v>1264</v>
@@ -18529,7 +18761,7 @@
         <v>260</v>
       </c>
       <c r="B265" t="s">
-        <v>3830</v>
+        <v>3829</v>
       </c>
       <c r="C265" t="s">
         <v>1265</v>
@@ -18690,45 +18922,45 @@
         <v>267</v>
       </c>
       <c r="B272" t="s">
-        <v>3573</v>
+        <v>3572</v>
       </c>
       <c r="C272" t="s">
+        <v>3567</v>
+      </c>
+      <c r="D272" s="2" t="s">
         <v>3568</v>
       </c>
-      <c r="D272" s="2" t="s">
+      <c r="E272" t="s">
+        <v>3570</v>
+      </c>
+      <c r="F272" t="s">
         <v>3569</v>
       </c>
-      <c r="E272" t="s">
+      <c r="G272" t="s">
         <v>3571</v>
-      </c>
-      <c r="F272" t="s">
-        <v>3570</v>
-      </c>
-      <c r="G272" t="s">
-        <v>3572</v>
       </c>
     </row>
     <row r="273" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
+        <v>3573</v>
+      </c>
+      <c r="B273" t="s">
         <v>3574</v>
       </c>
-      <c r="B273" t="s">
+      <c r="C273" t="s">
         <v>3575</v>
       </c>
-      <c r="C273" t="s">
+      <c r="D273" s="2" t="s">
         <v>3576</v>
       </c>
-      <c r="D273" s="2" t="s">
+      <c r="E273" t="s">
         <v>3577</v>
       </c>
-      <c r="E273" t="s">
+      <c r="F273" t="s">
+        <v>3569</v>
+      </c>
+      <c r="G273" t="s">
         <v>3578</v>
-      </c>
-      <c r="F273" t="s">
-        <v>3570</v>
-      </c>
-      <c r="G273" t="s">
-        <v>3579</v>
       </c>
     </row>
     <row r="274" spans="1:7" x14ac:dyDescent="0.25">
@@ -18897,7 +19129,7 @@
         <v>275</v>
       </c>
       <c r="B281" t="s">
-        <v>3831</v>
+        <v>3830</v>
       </c>
       <c r="C281" t="s">
         <v>1279</v>
@@ -19018,7 +19250,7 @@
         <v>1284</v>
       </c>
       <c r="D286" s="2" t="s">
-        <v>3529</v>
+        <v>3528</v>
       </c>
       <c r="E286" t="s">
         <v>2204</v>
@@ -19064,7 +19296,7 @@
         <v>1286</v>
       </c>
       <c r="D288" s="2" t="s">
-        <v>3530</v>
+        <v>3529</v>
       </c>
       <c r="E288" t="s">
         <v>2206</v>
@@ -19150,7 +19382,7 @@
         <v>286</v>
       </c>
       <c r="B292" t="s">
-        <v>3832</v>
+        <v>3831</v>
       </c>
       <c r="C292" t="s">
         <v>1290</v>
@@ -19219,7 +19451,7 @@
         <v>289</v>
       </c>
       <c r="B295" t="s">
-        <v>3833</v>
+        <v>3832</v>
       </c>
       <c r="C295" t="s">
         <v>1292</v>
@@ -19311,7 +19543,7 @@
         <v>293</v>
       </c>
       <c r="B299" t="s">
-        <v>3834</v>
+        <v>3833</v>
       </c>
       <c r="C299" t="s">
         <v>1295</v>
@@ -19495,7 +19727,7 @@
         <v>301</v>
       </c>
       <c r="B307" t="s">
-        <v>3835</v>
+        <v>3834</v>
       </c>
       <c r="C307" t="s">
         <v>1302</v>
@@ -19564,7 +19796,7 @@
         <v>304</v>
       </c>
       <c r="B310" t="s">
-        <v>3836</v>
+        <v>3835</v>
       </c>
       <c r="C310" t="s">
         <v>1305</v>
@@ -19708,7 +19940,7 @@
         <v>813</v>
       </c>
       <c r="D316" s="2" t="s">
-        <v>3531</v>
+        <v>3530</v>
       </c>
       <c r="E316" t="s">
         <v>2234</v>
@@ -19731,7 +19963,7 @@
         <v>814</v>
       </c>
       <c r="D317" s="2" t="s">
-        <v>3532</v>
+        <v>3531</v>
       </c>
       <c r="E317" t="s">
         <v>2235</v>
@@ -19754,7 +19986,7 @@
         <v>1311</v>
       </c>
       <c r="D318" s="2" t="s">
-        <v>3533</v>
+        <v>3532</v>
       </c>
       <c r="E318" t="s">
         <v>2236</v>
@@ -19777,7 +20009,7 @@
         <v>816</v>
       </c>
       <c r="D319" s="2" t="s">
-        <v>3534</v>
+        <v>3533</v>
       </c>
       <c r="E319" t="s">
         <v>2237</v>
@@ -19840,7 +20072,7 @@
         <v>316</v>
       </c>
       <c r="B322" t="s">
-        <v>3837</v>
+        <v>3836</v>
       </c>
       <c r="C322" t="s">
         <v>1314</v>
@@ -19863,7 +20095,7 @@
         <v>317</v>
       </c>
       <c r="B323" t="s">
-        <v>3838</v>
+        <v>3837</v>
       </c>
       <c r="C323" t="s">
         <v>1315</v>
@@ -19886,22 +20118,22 @@
         <v>318</v>
       </c>
       <c r="B324" t="s">
-        <v>3882</v>
+        <v>3881</v>
       </c>
       <c r="C324" t="s">
+        <v>3877</v>
+      </c>
+      <c r="D324" s="2" t="s">
+        <v>3880</v>
+      </c>
+      <c r="E324" t="s">
         <v>3878</v>
       </c>
-      <c r="D324" s="2" t="s">
-        <v>3881</v>
-      </c>
-      <c r="E324" t="s">
+      <c r="F324" t="s">
         <v>3879</v>
       </c>
-      <c r="F324" t="s">
-        <v>3880</v>
-      </c>
       <c r="G324" t="s">
-        <v>3877</v>
+        <v>3876</v>
       </c>
     </row>
     <row r="325" spans="1:7" x14ac:dyDescent="0.25">
@@ -20185,13 +20417,13 @@
         <v>331</v>
       </c>
       <c r="B337" t="s">
-        <v>3839</v>
+        <v>3838</v>
       </c>
       <c r="C337" t="s">
         <v>1328</v>
       </c>
       <c r="D337" s="2" t="s">
-        <v>3535</v>
+        <v>3534</v>
       </c>
       <c r="E337" t="s">
         <v>2254</v>
@@ -20214,7 +20446,7 @@
         <v>1329</v>
       </c>
       <c r="D338" s="2" t="s">
-        <v>3536</v>
+        <v>3535</v>
       </c>
       <c r="E338" t="s">
         <v>2255</v>
@@ -20251,7 +20483,7 @@
     </row>
     <row r="340" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
-        <v>3758</v>
+        <v>3757</v>
       </c>
       <c r="B340" t="s">
         <v>834</v>
@@ -20260,7 +20492,7 @@
         <v>1331</v>
       </c>
       <c r="D340" s="2" t="s">
-        <v>3537</v>
+        <v>3536</v>
       </c>
       <c r="E340" t="s">
         <v>2257</v>
@@ -20274,10 +20506,10 @@
     </row>
     <row r="341" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
-        <v>3759</v>
+        <v>3758</v>
       </c>
       <c r="B341" t="s">
-        <v>3840</v>
+        <v>3839</v>
       </c>
       <c r="C341" t="s">
         <v>1332</v>
@@ -20467,7 +20699,7 @@
         <v>1340</v>
       </c>
       <c r="D349" s="2" t="s">
-        <v>3538</v>
+        <v>3537</v>
       </c>
       <c r="E349" t="s">
         <v>2266</v>
@@ -20513,7 +20745,7 @@
         <v>1342</v>
       </c>
       <c r="D351" s="2" t="s">
-        <v>3539</v>
+        <v>3538</v>
       </c>
       <c r="E351" t="s">
         <v>2268</v>
@@ -20559,7 +20791,7 @@
         <v>1344</v>
       </c>
       <c r="D353" s="2" t="s">
-        <v>3540</v>
+        <v>3539</v>
       </c>
       <c r="E353" t="s">
         <v>2270</v>
@@ -20582,7 +20814,7 @@
         <v>1345</v>
       </c>
       <c r="D354" s="2" t="s">
-        <v>3541</v>
+        <v>3540</v>
       </c>
       <c r="E354" t="s">
         <v>2271</v>
@@ -20622,7 +20854,7 @@
         <v>348</v>
       </c>
       <c r="B356" t="s">
-        <v>3841</v>
+        <v>3840</v>
       </c>
       <c r="C356" t="s">
         <v>1346</v>
@@ -20651,7 +20883,7 @@
         <v>1347</v>
       </c>
       <c r="D357" s="2" t="s">
-        <v>3542</v>
+        <v>3541</v>
       </c>
       <c r="E357" t="s">
         <v>2274</v>
@@ -20720,7 +20952,7 @@
         <v>1350</v>
       </c>
       <c r="D360" s="2" t="s">
-        <v>3544</v>
+        <v>3543</v>
       </c>
       <c r="E360" t="s">
         <v>2277</v>
@@ -20743,7 +20975,7 @@
         <v>1351</v>
       </c>
       <c r="D361" s="2" t="s">
-        <v>3543</v>
+        <v>3542</v>
       </c>
       <c r="E361" t="s">
         <v>2278</v>
@@ -20921,7 +21153,7 @@
         <v>361</v>
       </c>
       <c r="B369" t="s">
-        <v>3804</v>
+        <v>3803</v>
       </c>
       <c r="C369" t="s">
         <v>1359</v>
@@ -20950,7 +21182,7 @@
         <v>1360</v>
       </c>
       <c r="D370" s="2" t="s">
-        <v>3545</v>
+        <v>3544</v>
       </c>
       <c r="E370" t="s">
         <v>2287</v>
@@ -20967,7 +21199,7 @@
         <v>363</v>
       </c>
       <c r="B371" t="s">
-        <v>3842</v>
+        <v>3841</v>
       </c>
       <c r="C371" t="s">
         <v>1361</v>
@@ -21019,7 +21251,7 @@
         <v>1363</v>
       </c>
       <c r="D373" s="2" t="s">
-        <v>3546</v>
+        <v>3545</v>
       </c>
       <c r="E373" t="s">
         <v>2290</v>
@@ -21059,22 +21291,22 @@
         <v>367</v>
       </c>
       <c r="B375" t="s">
+        <v>3872</v>
+      </c>
+      <c r="C375" t="s">
+        <v>3870</v>
+      </c>
+      <c r="D375" s="2" t="s">
         <v>3873</v>
       </c>
-      <c r="C375" t="s">
+      <c r="E375" t="s">
+        <v>3875</v>
+      </c>
+      <c r="F375" t="s">
+        <v>3874</v>
+      </c>
+      <c r="G375" t="s">
         <v>3871</v>
-      </c>
-      <c r="D375" s="2" t="s">
-        <v>3874</v>
-      </c>
-      <c r="E375" t="s">
-        <v>3876</v>
-      </c>
-      <c r="F375" t="s">
-        <v>3875</v>
-      </c>
-      <c r="G375" t="s">
-        <v>3872</v>
       </c>
     </row>
     <row r="376" spans="1:7" x14ac:dyDescent="0.25">
@@ -21151,22 +21383,22 @@
         <v>371</v>
       </c>
       <c r="B379" t="s">
-        <v>3870</v>
+        <v>3869</v>
       </c>
       <c r="C379" t="s">
+        <v>3864</v>
+      </c>
+      <c r="D379" s="2" t="s">
+        <v>3868</v>
+      </c>
+      <c r="E379" t="s">
+        <v>3866</v>
+      </c>
+      <c r="F379" t="s">
+        <v>3867</v>
+      </c>
+      <c r="G379" t="s">
         <v>3865</v>
-      </c>
-      <c r="D379" s="2" t="s">
-        <v>3869</v>
-      </c>
-      <c r="E379" t="s">
-        <v>3867</v>
-      </c>
-      <c r="F379" t="s">
-        <v>3868</v>
-      </c>
-      <c r="G379" t="s">
-        <v>3866</v>
       </c>
     </row>
     <row r="380" spans="1:7" x14ac:dyDescent="0.25">
@@ -21335,22 +21567,22 @@
         <v>379</v>
       </c>
       <c r="B387" t="s">
+        <v>3910</v>
+      </c>
+      <c r="C387" t="s">
         <v>3911</v>
       </c>
-      <c r="C387" t="s">
+      <c r="D387" s="2" t="s">
         <v>3912</v>
       </c>
-      <c r="D387" s="2" t="s">
+      <c r="E387" t="s">
         <v>3913</v>
       </c>
-      <c r="E387" t="s">
+      <c r="F387" t="s">
         <v>3914</v>
       </c>
-      <c r="F387" t="s">
-        <v>3915</v>
-      </c>
       <c r="G387" t="s">
-        <v>3910</v>
+        <v>3909</v>
       </c>
     </row>
     <row r="388" spans="1:7" x14ac:dyDescent="0.25">
@@ -21473,7 +21705,7 @@
         <v>385</v>
       </c>
       <c r="B393" t="s">
-        <v>3843</v>
+        <v>3842</v>
       </c>
       <c r="C393" t="s">
         <v>1379</v>
@@ -21565,7 +21797,7 @@
         <v>389</v>
       </c>
       <c r="B397" t="s">
-        <v>3844</v>
+        <v>3843</v>
       </c>
       <c r="C397" t="s">
         <v>1383</v>
@@ -21749,7 +21981,7 @@
         <v>397</v>
       </c>
       <c r="B405" t="s">
-        <v>3845</v>
+        <v>3844</v>
       </c>
       <c r="C405" t="s">
         <v>1391</v>
@@ -21795,7 +22027,7 @@
         <v>399</v>
       </c>
       <c r="B407" t="s">
-        <v>3846</v>
+        <v>3845</v>
       </c>
       <c r="C407" t="s">
         <v>1393</v>
@@ -21910,7 +22142,7 @@
         <v>404</v>
       </c>
       <c r="B412" t="s">
-        <v>3847</v>
+        <v>3846</v>
       </c>
       <c r="C412" t="s">
         <v>1398</v>
@@ -22160,25 +22392,25 @@
     </row>
     <row r="423" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A423" t="s">
+        <v>3586</v>
+      </c>
+      <c r="B423" t="s">
+        <v>3589</v>
+      </c>
+      <c r="C423" t="s">
         <v>3587</v>
       </c>
-      <c r="B423" t="s">
+      <c r="D423" s="2" t="s">
         <v>3590</v>
       </c>
-      <c r="C423" t="s">
+      <c r="E423" t="s">
+        <v>3591</v>
+      </c>
+      <c r="F423" t="s">
+        <v>3592</v>
+      </c>
+      <c r="G423" t="s">
         <v>3588</v>
-      </c>
-      <c r="D423" s="2" t="s">
-        <v>3591</v>
-      </c>
-      <c r="E423" t="s">
-        <v>3592</v>
-      </c>
-      <c r="F423" t="s">
-        <v>3593</v>
-      </c>
-      <c r="G423" t="s">
-        <v>3589</v>
       </c>
     </row>
     <row r="424" spans="1:7" x14ac:dyDescent="0.25">
@@ -22186,13 +22418,13 @@
         <v>415</v>
       </c>
       <c r="B424" t="s">
-        <v>3778</v>
+        <v>3777</v>
       </c>
       <c r="C424" t="s">
         <v>1409</v>
       </c>
       <c r="D424" s="2" t="s">
-        <v>3547</v>
+        <v>3546</v>
       </c>
       <c r="E424" t="s">
         <v>2336</v>
@@ -22396,7 +22628,7 @@
         <v>912</v>
       </c>
       <c r="C433" t="s">
-        <v>3909</v>
+        <v>3908</v>
       </c>
       <c r="D433" s="2" t="s">
         <v>1850</v>
@@ -22439,13 +22671,13 @@
         <v>426</v>
       </c>
       <c r="B435" t="s">
-        <v>3779</v>
+        <v>3778</v>
       </c>
       <c r="C435" t="s">
         <v>1419</v>
       </c>
       <c r="D435" s="2" t="s">
-        <v>3548</v>
+        <v>3547</v>
       </c>
       <c r="E435" t="s">
         <v>2346</v>
@@ -22508,13 +22740,13 @@
         <v>429</v>
       </c>
       <c r="B438" t="s">
-        <v>3780</v>
+        <v>3779</v>
       </c>
       <c r="C438" t="s">
         <v>1422</v>
       </c>
       <c r="D438" s="2" t="s">
-        <v>3549</v>
+        <v>3548</v>
       </c>
       <c r="E438" t="s">
         <v>2349</v>
@@ -22623,7 +22855,7 @@
         <v>434</v>
       </c>
       <c r="B443" t="s">
-        <v>3781</v>
+        <v>3780</v>
       </c>
       <c r="C443" t="s">
         <v>1427</v>
@@ -22807,22 +23039,22 @@
         <v>442</v>
       </c>
       <c r="B451" t="s">
-        <v>3511</v>
+        <v>3510</v>
       </c>
       <c r="C451" t="s">
+        <v>3505</v>
+      </c>
+      <c r="D451" s="2" t="s">
+        <v>3509</v>
+      </c>
+      <c r="E451" t="s">
+        <v>3508</v>
+      </c>
+      <c r="F451" t="s">
+        <v>3507</v>
+      </c>
+      <c r="G451" t="s">
         <v>3506</v>
-      </c>
-      <c r="D451" s="2" t="s">
-        <v>3510</v>
-      </c>
-      <c r="E451" t="s">
-        <v>3509</v>
-      </c>
-      <c r="F451" t="s">
-        <v>3508</v>
-      </c>
-      <c r="G451" t="s">
-        <v>3507</v>
       </c>
     </row>
     <row r="452" spans="1:7" x14ac:dyDescent="0.25">
@@ -22853,7 +23085,7 @@
         <v>444</v>
       </c>
       <c r="B453" t="s">
-        <v>3848</v>
+        <v>3847</v>
       </c>
       <c r="C453" t="s">
         <v>1435</v>
@@ -23066,7 +23298,7 @@
         <v>1444</v>
       </c>
       <c r="D462" s="2" t="s">
-        <v>3550</v>
+        <v>3549</v>
       </c>
       <c r="E462" t="s">
         <v>2370</v>
@@ -23520,7 +23752,7 @@
         <v>473</v>
       </c>
       <c r="B482" t="s">
-        <v>3849</v>
+        <v>3848</v>
       </c>
       <c r="C482" t="s">
         <v>1464</v>
@@ -23641,7 +23873,7 @@
         <v>1469</v>
       </c>
       <c r="D487" s="2" t="s">
-        <v>3551</v>
+        <v>3550</v>
       </c>
       <c r="E487" t="s">
         <v>2393</v>
@@ -23658,7 +23890,7 @@
         <v>479</v>
       </c>
       <c r="B488" t="s">
-        <v>3777</v>
+        <v>3776</v>
       </c>
       <c r="C488" t="s">
         <v>1470</v>
@@ -23802,7 +24034,7 @@
         <v>1476</v>
       </c>
       <c r="D494" s="2" t="s">
-        <v>3552</v>
+        <v>3551</v>
       </c>
       <c r="E494" t="s">
         <v>2400</v>
@@ -23825,16 +24057,16 @@
         <v>3481</v>
       </c>
       <c r="D495" s="2" t="s">
-        <v>3558</v>
+        <v>3557</v>
       </c>
       <c r="E495" t="s">
         <v>3482</v>
       </c>
       <c r="F495" t="s">
+        <v>4026</v>
+      </c>
+      <c r="G495" t="s">
         <v>3483</v>
-      </c>
-      <c r="G495" t="s">
-        <v>3484</v>
       </c>
     </row>
     <row r="496" spans="1:7" x14ac:dyDescent="0.25">
@@ -24046,168 +24278,168 @@
     </row>
     <row r="505" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A505" t="s">
+        <v>3980</v>
+      </c>
+      <c r="B505" t="s">
         <v>3981</v>
       </c>
-      <c r="B505" t="s">
+      <c r="C505" t="s">
         <v>3982</v>
       </c>
-      <c r="C505" t="s">
+      <c r="D505" s="2" t="s">
         <v>3983</v>
       </c>
-      <c r="D505" s="2" t="s">
+      <c r="E505" t="s">
         <v>3984</v>
       </c>
-      <c r="E505" t="s">
+      <c r="F505" t="s">
         <v>3985</v>
       </c>
-      <c r="F505" t="s">
+      <c r="G505" t="s">
         <v>3986</v>
-      </c>
-      <c r="G505" t="s">
-        <v>3987</v>
       </c>
     </row>
     <row r="506" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A506" t="s">
-        <v>3980</v>
+        <v>3979</v>
       </c>
       <c r="B506" t="s">
+        <v>3973</v>
+      </c>
+      <c r="C506" t="s">
         <v>3974</v>
       </c>
-      <c r="C506" t="s">
+      <c r="D506" s="2" t="s">
         <v>3975</v>
       </c>
-      <c r="D506" s="2" t="s">
+      <c r="E506" t="s">
         <v>3976</v>
       </c>
-      <c r="E506" t="s">
+      <c r="F506" t="s">
         <v>3977</v>
       </c>
-      <c r="F506" t="s">
+      <c r="G506" t="s">
         <v>3978</v>
-      </c>
-      <c r="G506" t="s">
-        <v>3979</v>
       </c>
     </row>
     <row r="507" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A507" t="s">
+        <v>3945</v>
+      </c>
+      <c r="B507" t="s">
         <v>3946</v>
       </c>
-      <c r="B507" t="s">
+      <c r="C507" t="s">
         <v>3947</v>
       </c>
-      <c r="C507" t="s">
+      <c r="D507" s="2" t="s">
+        <v>3954</v>
+      </c>
+      <c r="E507" t="s">
         <v>3948</v>
       </c>
-      <c r="D507" s="2" t="s">
-        <v>3955</v>
-      </c>
-      <c r="E507" t="s">
+      <c r="F507" t="s">
         <v>3949</v>
       </c>
-      <c r="F507" t="s">
+      <c r="G507" t="s">
         <v>3950</v>
-      </c>
-      <c r="G507" t="s">
-        <v>3951</v>
       </c>
     </row>
     <row r="508" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A508" t="s">
-        <v>3959</v>
+        <v>3958</v>
       </c>
       <c r="B508" t="s">
+        <v>3951</v>
+      </c>
+      <c r="C508" t="s">
         <v>3952</v>
       </c>
-      <c r="C508" t="s">
+      <c r="D508" s="2" t="s">
         <v>3953</v>
       </c>
-      <c r="D508" s="2" t="s">
-        <v>3954</v>
-      </c>
       <c r="E508" t="s">
+        <v>3955</v>
+      </c>
+      <c r="F508" t="s">
         <v>3956</v>
       </c>
-      <c r="F508" t="s">
+      <c r="G508" t="s">
         <v>3957</v>
-      </c>
-      <c r="G508" t="s">
-        <v>3958</v>
       </c>
     </row>
     <row r="509" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A509" t="s">
+        <v>3993</v>
+      </c>
+      <c r="B509" t="s">
         <v>3994</v>
       </c>
-      <c r="B509" t="s">
+      <c r="C509" t="s">
         <v>3995</v>
       </c>
-      <c r="C509" t="s">
+      <c r="D509" s="2" t="s">
         <v>3996</v>
       </c>
-      <c r="D509" s="2" t="s">
+      <c r="E509" t="s">
         <v>3997</v>
       </c>
-      <c r="E509" t="s">
+      <c r="F509" t="s">
         <v>3998</v>
       </c>
-      <c r="F509" t="s">
+      <c r="G509" t="s">
         <v>3999</v>
-      </c>
-      <c r="G509" t="s">
-        <v>4000</v>
       </c>
     </row>
     <row r="510" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A510" t="s">
+        <v>3966</v>
+      </c>
+      <c r="B510" t="s">
         <v>3967</v>
       </c>
-      <c r="B510" t="s">
+      <c r="C510" t="s">
         <v>3968</v>
       </c>
-      <c r="C510" t="s">
+      <c r="D510" s="2" t="s">
         <v>3969</v>
       </c>
-      <c r="D510" s="2" t="s">
+      <c r="E510" t="s">
         <v>3970</v>
       </c>
-      <c r="E510" t="s">
+      <c r="F510" t="s">
         <v>3971</v>
       </c>
-      <c r="F510" t="s">
+      <c r="G510" t="s">
         <v>3972</v>
-      </c>
-      <c r="G510" t="s">
-        <v>3973</v>
       </c>
     </row>
     <row r="511" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A511" t="s">
-        <v>3966</v>
+        <v>3965</v>
       </c>
       <c r="B511" t="s">
+        <v>3959</v>
+      </c>
+      <c r="C511" t="s">
         <v>3960</v>
       </c>
-      <c r="C511" t="s">
+      <c r="D511" s="2" t="s">
         <v>3961</v>
       </c>
-      <c r="D511" s="2" t="s">
+      <c r="E511" t="s">
         <v>3962</v>
       </c>
-      <c r="E511" t="s">
+      <c r="F511" t="s">
         <v>3963</v>
       </c>
-      <c r="F511" t="s">
+      <c r="G511" t="s">
         <v>3964</v>
-      </c>
-      <c r="G511" t="s">
-        <v>3965</v>
       </c>
     </row>
     <row r="512" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A512" t="s">
-        <v>3945</v>
+        <v>3944</v>
       </c>
       <c r="B512" t="s">
         <v>976</v>
@@ -24230,94 +24462,94 @@
     </row>
     <row r="513" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A513" t="s">
+        <v>3937</v>
+      </c>
+      <c r="B513" t="s">
         <v>3938</v>
       </c>
-      <c r="B513" t="s">
+      <c r="C513" t="s">
         <v>3939</v>
       </c>
-      <c r="C513" t="s">
+      <c r="D513" s="2" t="s">
         <v>3940</v>
       </c>
-      <c r="D513" s="2" t="s">
+      <c r="E513" t="s">
         <v>3941</v>
       </c>
-      <c r="E513" t="s">
+      <c r="F513" t="s">
         <v>3942</v>
       </c>
-      <c r="F513" t="s">
+      <c r="G513" t="s">
         <v>3943</v>
-      </c>
-      <c r="G513" t="s">
-        <v>3944</v>
       </c>
     </row>
     <row r="514" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A514" t="s">
+        <v>3930</v>
+      </c>
+      <c r="B514" t="s">
         <v>3931</v>
       </c>
-      <c r="B514" t="s">
+      <c r="C514" t="s">
         <v>3932</v>
       </c>
-      <c r="C514" t="s">
+      <c r="D514" s="2" t="s">
         <v>3933</v>
       </c>
-      <c r="D514" s="2" t="s">
+      <c r="E514" t="s">
         <v>3934</v>
       </c>
-      <c r="E514" t="s">
+      <c r="F514" t="s">
         <v>3935</v>
       </c>
-      <c r="F514" t="s">
+      <c r="G514" t="s">
         <v>3936</v>
-      </c>
-      <c r="G514" t="s">
-        <v>3937</v>
       </c>
     </row>
     <row r="515" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A515" t="s">
-        <v>3930</v>
+        <v>3929</v>
       </c>
       <c r="B515" t="s">
+        <v>3923</v>
+      </c>
+      <c r="C515" t="s">
         <v>3924</v>
       </c>
-      <c r="C515" t="s">
+      <c r="D515" s="2" t="s">
         <v>3925</v>
       </c>
-      <c r="D515" s="2" t="s">
+      <c r="E515" t="s">
         <v>3926</v>
       </c>
-      <c r="E515" t="s">
+      <c r="F515" t="s">
         <v>3927</v>
       </c>
-      <c r="F515" t="s">
+      <c r="G515" t="s">
         <v>3928</v>
-      </c>
-      <c r="G515" t="s">
-        <v>3929</v>
       </c>
     </row>
     <row r="516" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A516" t="s">
+        <v>3916</v>
+      </c>
+      <c r="B516" t="s">
         <v>3917</v>
       </c>
-      <c r="B516" t="s">
+      <c r="C516" t="s">
         <v>3918</v>
       </c>
-      <c r="C516" t="s">
+      <c r="D516" s="2" t="s">
         <v>3919</v>
       </c>
-      <c r="D516" s="2" t="s">
+      <c r="E516" t="s">
         <v>3920</v>
       </c>
-      <c r="E516" t="s">
+      <c r="F516" t="s">
         <v>3921</v>
       </c>
-      <c r="F516" t="s">
+      <c r="G516" t="s">
         <v>3922</v>
-      </c>
-      <c r="G516" t="s">
-        <v>3923</v>
       </c>
     </row>
     <row r="517" spans="1:7" x14ac:dyDescent="0.25">
@@ -24377,7 +24609,7 @@
         <v>1485</v>
       </c>
       <c r="D519" s="2" t="s">
-        <v>3553</v>
+        <v>3552</v>
       </c>
       <c r="E519" t="s">
         <v>2413</v>
@@ -24400,7 +24632,7 @@
         <v>1486</v>
       </c>
       <c r="D520" s="2" t="s">
-        <v>3554</v>
+        <v>3553</v>
       </c>
       <c r="E520" t="s">
         <v>2414</v>
@@ -24423,7 +24655,7 @@
         <v>1487</v>
       </c>
       <c r="D521" s="3" t="s">
-        <v>3555</v>
+        <v>3554</v>
       </c>
       <c r="E521" t="s">
         <v>2415</v>
@@ -24446,7 +24678,7 @@
         <v>1488</v>
       </c>
       <c r="D522" s="2" t="s">
-        <v>3556</v>
+        <v>3555</v>
       </c>
       <c r="E522" t="s">
         <v>2416</v>
@@ -24509,22 +24741,22 @@
         <v>504</v>
       </c>
       <c r="B525" t="s">
+        <v>3987</v>
+      </c>
+      <c r="C525" t="s">
         <v>3988</v>
       </c>
-      <c r="C525" t="s">
+      <c r="D525" s="2" t="s">
         <v>3989</v>
       </c>
-      <c r="D525" s="2" t="s">
+      <c r="E525" t="s">
         <v>3990</v>
       </c>
-      <c r="E525" t="s">
+      <c r="F525" t="s">
         <v>3991</v>
       </c>
-      <c r="F525" t="s">
+      <c r="G525" t="s">
         <v>3992</v>
-      </c>
-      <c r="G525" t="s">
-        <v>3993</v>
       </c>
     </row>
     <row r="526" spans="1:7" x14ac:dyDescent="0.25">
@@ -24670,22 +24902,22 @@
         <v>511</v>
       </c>
       <c r="B532" t="s">
+        <v>4000</v>
+      </c>
+      <c r="C532" t="s">
         <v>4001</v>
       </c>
-      <c r="C532" t="s">
+      <c r="D532" s="2" t="s">
         <v>4002</v>
       </c>
-      <c r="D532" s="2" t="s">
+      <c r="E532" t="s">
         <v>4003</v>
       </c>
-      <c r="E532" t="s">
+      <c r="F532" t="s">
         <v>4004</v>
       </c>
-      <c r="F532" t="s">
+      <c r="G532" t="s">
         <v>4005</v>
-      </c>
-      <c r="G532" t="s">
-        <v>4006</v>
       </c>
     </row>
     <row r="533" spans="1:7" x14ac:dyDescent="0.25">
@@ -25334,367 +25566,367 @@
     </row>
     <row r="561" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A561" t="s">
-        <v>3485</v>
+        <v>3484</v>
       </c>
       <c r="B561" t="s">
-        <v>3494</v>
+        <v>3493</v>
       </c>
       <c r="C561" t="s">
-        <v>3488</v>
+        <v>3487</v>
       </c>
       <c r="D561" t="s">
-        <v>3497</v>
+        <v>3496</v>
       </c>
       <c r="E561" t="s">
-        <v>3500</v>
+        <v>3499</v>
       </c>
       <c r="F561" t="s">
-        <v>3503</v>
+        <v>3502</v>
       </c>
       <c r="G561" t="s">
-        <v>3491</v>
+        <v>3490</v>
       </c>
     </row>
     <row r="562" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A562" t="s">
-        <v>3486</v>
+        <v>3485</v>
       </c>
       <c r="B562" t="s">
-        <v>3495</v>
+        <v>3494</v>
       </c>
       <c r="C562" t="s">
-        <v>3489</v>
+        <v>3488</v>
       </c>
       <c r="D562" t="s">
-        <v>3498</v>
+        <v>3497</v>
       </c>
       <c r="E562" t="s">
-        <v>3501</v>
+        <v>3500</v>
       </c>
       <c r="F562" t="s">
-        <v>3504</v>
+        <v>3503</v>
       </c>
       <c r="G562" t="s">
-        <v>3493</v>
+        <v>3492</v>
       </c>
     </row>
     <row r="563" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A563" t="s">
-        <v>3487</v>
+        <v>3486</v>
       </c>
       <c r="B563" t="s">
-        <v>3496</v>
+        <v>3495</v>
       </c>
       <c r="C563" t="s">
-        <v>3490</v>
+        <v>3489</v>
       </c>
       <c r="D563" t="s">
-        <v>3499</v>
+        <v>3498</v>
       </c>
       <c r="E563" t="s">
-        <v>3502</v>
+        <v>3501</v>
       </c>
       <c r="F563" t="s">
-        <v>3505</v>
+        <v>3504</v>
       </c>
       <c r="G563" t="s">
-        <v>3492</v>
+        <v>3491</v>
       </c>
     </row>
     <row r="564" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A564" t="s">
+        <v>3560</v>
+      </c>
+      <c r="B564" t="s">
+        <v>3566</v>
+      </c>
+      <c r="C564" t="s">
         <v>3561</v>
       </c>
-      <c r="B564" t="s">
-        <v>3567</v>
-      </c>
-      <c r="C564" t="s">
+      <c r="D564" t="s">
+        <v>3564</v>
+      </c>
+      <c r="E564" t="s">
         <v>3562</v>
       </c>
-      <c r="D564" t="s">
+      <c r="F564" t="s">
+        <v>3563</v>
+      </c>
+      <c r="G564" t="s">
         <v>3565</v>
-      </c>
-      <c r="E564" t="s">
-        <v>3563</v>
-      </c>
-      <c r="F564" t="s">
-        <v>3564</v>
-      </c>
-      <c r="G564" t="s">
-        <v>3566</v>
       </c>
     </row>
     <row r="565" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A565" t="s">
+        <v>3579</v>
+      </c>
+      <c r="B565" t="s">
+        <v>3582</v>
+      </c>
+      <c r="C565" t="s">
+        <v>3581</v>
+      </c>
+      <c r="D565" t="s">
+        <v>3585</v>
+      </c>
+      <c r="E565" t="s">
+        <v>3583</v>
+      </c>
+      <c r="F565" t="s">
+        <v>3584</v>
+      </c>
+      <c r="G565" t="s">
         <v>3580</v>
-      </c>
-      <c r="B565" t="s">
-        <v>3583</v>
-      </c>
-      <c r="C565" t="s">
-        <v>3582</v>
-      </c>
-      <c r="D565" t="s">
-        <v>3586</v>
-      </c>
-      <c r="E565" t="s">
-        <v>3584</v>
-      </c>
-      <c r="F565" t="s">
-        <v>3585</v>
-      </c>
-      <c r="G565" t="s">
-        <v>3581</v>
       </c>
     </row>
     <row r="566" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A566" t="s">
-        <v>3594</v>
+        <v>3593</v>
       </c>
       <c r="B566" t="s">
-        <v>3636</v>
+        <v>3635</v>
       </c>
       <c r="C566" t="s">
-        <v>3615</v>
+        <v>3614</v>
       </c>
       <c r="D566" t="s">
-        <v>3687</v>
+        <v>3686</v>
       </c>
       <c r="E566" t="s">
-        <v>3701</v>
+        <v>3700</v>
       </c>
       <c r="F566" t="s">
-        <v>3669</v>
+        <v>3668</v>
       </c>
       <c r="G566" t="s">
-        <v>3636</v>
+        <v>3635</v>
       </c>
     </row>
     <row r="567" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A567" t="s">
-        <v>3595</v>
+        <v>3594</v>
       </c>
       <c r="B567" t="s">
-        <v>3850</v>
+        <v>3849</v>
       </c>
       <c r="C567" t="s">
-        <v>3616</v>
+        <v>3615</v>
       </c>
       <c r="D567" t="s">
-        <v>3688</v>
+        <v>3687</v>
       </c>
       <c r="E567" t="s">
-        <v>3702</v>
+        <v>3701</v>
       </c>
       <c r="F567" t="s">
-        <v>3670</v>
+        <v>3669</v>
       </c>
       <c r="G567" t="s">
-        <v>3773</v>
+        <v>3772</v>
       </c>
     </row>
     <row r="568" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A568" t="s">
-        <v>3596</v>
+        <v>3595</v>
       </c>
       <c r="B568" t="s">
-        <v>3659</v>
+        <v>3658</v>
       </c>
       <c r="C568" t="s">
-        <v>3617</v>
+        <v>3616</v>
       </c>
       <c r="D568" t="s">
-        <v>3689</v>
+        <v>3688</v>
       </c>
       <c r="E568" t="s">
-        <v>3703</v>
+        <v>3702</v>
       </c>
       <c r="F568" t="s">
-        <v>3671</v>
+        <v>3670</v>
       </c>
       <c r="G568" t="s">
-        <v>3637</v>
+        <v>3636</v>
       </c>
     </row>
     <row r="569" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A569" t="s">
-        <v>3597</v>
+        <v>3596</v>
       </c>
       <c r="B569" t="s">
-        <v>3660</v>
+        <v>3659</v>
       </c>
       <c r="C569" t="s">
-        <v>3620</v>
+        <v>3619</v>
       </c>
       <c r="D569" t="s">
-        <v>3690</v>
+        <v>3689</v>
       </c>
       <c r="E569" t="s">
-        <v>3704</v>
+        <v>3703</v>
       </c>
       <c r="F569" t="s">
-        <v>3672</v>
+        <v>3671</v>
       </c>
       <c r="G569" t="s">
-        <v>3638</v>
+        <v>3637</v>
       </c>
     </row>
     <row r="570" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A570" t="s">
-        <v>3598</v>
+        <v>3597</v>
       </c>
       <c r="B570" t="s">
-        <v>3639</v>
+        <v>3638</v>
       </c>
       <c r="C570" t="s">
-        <v>3621</v>
+        <v>3620</v>
       </c>
       <c r="D570" t="s">
-        <v>3691</v>
+        <v>3690</v>
       </c>
       <c r="E570" t="s">
-        <v>3705</v>
+        <v>3704</v>
       </c>
       <c r="F570" t="s">
-        <v>3673</v>
+        <v>3672</v>
       </c>
       <c r="G570" t="s">
-        <v>3639</v>
+        <v>3638</v>
       </c>
     </row>
     <row r="571" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A571" t="s">
-        <v>3599</v>
+        <v>3598</v>
       </c>
       <c r="B571" t="s">
-        <v>3661</v>
+        <v>3660</v>
       </c>
       <c r="C571" t="s">
-        <v>3622</v>
+        <v>3621</v>
       </c>
       <c r="D571" t="s">
-        <v>3692</v>
+        <v>3691</v>
       </c>
       <c r="E571" t="s">
-        <v>3706</v>
+        <v>3705</v>
       </c>
       <c r="F571" t="s">
-        <v>3674</v>
+        <v>3673</v>
       </c>
       <c r="G571" t="s">
-        <v>3640</v>
+        <v>3639</v>
       </c>
     </row>
     <row r="572" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A572" t="s">
-        <v>3600</v>
+        <v>3599</v>
       </c>
       <c r="B572" t="s">
-        <v>3652</v>
+        <v>3651</v>
       </c>
       <c r="C572" t="s">
-        <v>3618</v>
+        <v>3617</v>
       </c>
       <c r="D572" t="s">
-        <v>3693</v>
+        <v>3692</v>
       </c>
       <c r="E572" t="s">
-        <v>3707</v>
+        <v>3706</v>
       </c>
       <c r="F572" t="s">
-        <v>3675</v>
+        <v>3674</v>
       </c>
       <c r="G572" t="s">
-        <v>3645</v>
+        <v>3644</v>
       </c>
     </row>
     <row r="573" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A573" t="s">
-        <v>3601</v>
+        <v>3600</v>
       </c>
       <c r="B573" t="s">
-        <v>3662</v>
+        <v>3661</v>
       </c>
       <c r="C573" t="s">
-        <v>3619</v>
+        <v>3618</v>
       </c>
       <c r="D573" t="s">
-        <v>3694</v>
+        <v>3693</v>
       </c>
       <c r="E573" t="s">
-        <v>3708</v>
+        <v>3707</v>
       </c>
       <c r="F573" t="s">
-        <v>3676</v>
+        <v>3675</v>
       </c>
       <c r="G573" t="s">
-        <v>3641</v>
+        <v>3640</v>
       </c>
     </row>
     <row r="574" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A574" t="s">
-        <v>3602</v>
+        <v>3601</v>
       </c>
       <c r="B574" t="s">
-        <v>3653</v>
+        <v>3652</v>
       </c>
       <c r="C574" t="s">
-        <v>3623</v>
+        <v>3622</v>
       </c>
       <c r="D574" t="s">
-        <v>3695</v>
+        <v>3694</v>
       </c>
       <c r="E574" t="s">
-        <v>3709</v>
+        <v>3708</v>
       </c>
       <c r="F574" t="s">
-        <v>3677</v>
+        <v>3676</v>
       </c>
       <c r="G574" t="s">
-        <v>3648</v>
+        <v>3647</v>
       </c>
     </row>
     <row r="575" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A575" t="s">
-        <v>3603</v>
+        <v>3602</v>
       </c>
       <c r="B575" t="s">
-        <v>3654</v>
+        <v>3653</v>
       </c>
       <c r="C575" t="s">
-        <v>3627</v>
+        <v>3626</v>
       </c>
       <c r="D575" t="s">
-        <v>3696</v>
+        <v>3695</v>
       </c>
       <c r="E575" t="s">
-        <v>3710</v>
+        <v>3709</v>
       </c>
       <c r="F575" t="s">
-        <v>3678</v>
+        <v>3677</v>
       </c>
       <c r="G575" t="s">
-        <v>3649</v>
+        <v>3648</v>
       </c>
     </row>
     <row r="576" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A576" t="s">
-        <v>3604</v>
+        <v>3603</v>
       </c>
       <c r="B576" t="s">
         <v>608</v>
       </c>
       <c r="C576" t="s">
-        <v>3626</v>
+        <v>3625</v>
       </c>
       <c r="D576" t="s">
-        <v>3697</v>
+        <v>3696</v>
       </c>
       <c r="E576" t="s">
-        <v>3711</v>
+        <v>3710</v>
       </c>
       <c r="F576" t="s">
-        <v>3679</v>
+        <v>3678</v>
       </c>
       <c r="G576" t="s">
         <v>3021</v>
@@ -25702,508 +25934,761 @@
     </row>
     <row r="577" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A577" t="s">
-        <v>3605</v>
+        <v>3604</v>
       </c>
       <c r="B577" t="s">
-        <v>3663</v>
+        <v>3662</v>
       </c>
       <c r="C577" t="s">
-        <v>3625</v>
+        <v>3624</v>
       </c>
       <c r="D577" t="s">
-        <v>3625</v>
+        <v>3624</v>
       </c>
       <c r="E577" t="s">
-        <v>3712</v>
+        <v>3711</v>
       </c>
       <c r="F577" t="s">
-        <v>3680</v>
+        <v>3679</v>
       </c>
       <c r="G577" t="s">
-        <v>3646</v>
+        <v>3645</v>
       </c>
     </row>
     <row r="578" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A578" t="s">
-        <v>3606</v>
+        <v>3605</v>
       </c>
       <c r="B578" t="s">
-        <v>3668</v>
+        <v>3667</v>
       </c>
       <c r="C578" t="s">
-        <v>3624</v>
+        <v>3623</v>
       </c>
       <c r="D578" t="s">
-        <v>3624</v>
+        <v>3623</v>
       </c>
       <c r="E578" t="s">
-        <v>3713</v>
+        <v>3712</v>
       </c>
       <c r="F578" t="s">
-        <v>3681</v>
+        <v>3680</v>
       </c>
       <c r="G578" t="s">
-        <v>3647</v>
+        <v>3646</v>
       </c>
     </row>
     <row r="579" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A579" t="s">
-        <v>3607</v>
+        <v>3606</v>
       </c>
       <c r="B579" t="s">
-        <v>3664</v>
+        <v>3663</v>
       </c>
       <c r="C579" t="s">
-        <v>3629</v>
+        <v>3628</v>
       </c>
       <c r="D579" t="s">
-        <v>3721</v>
+        <v>3720</v>
       </c>
       <c r="E579" t="s">
-        <v>3714</v>
+        <v>3713</v>
       </c>
       <c r="F579" t="s">
-        <v>3728</v>
+        <v>3727</v>
       </c>
       <c r="G579" t="s">
-        <v>3642</v>
+        <v>3641</v>
       </c>
     </row>
     <row r="580" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A580" t="s">
-        <v>3608</v>
+        <v>3607</v>
       </c>
       <c r="B580" t="s">
-        <v>3655</v>
+        <v>3654</v>
       </c>
       <c r="C580" t="s">
-        <v>3628</v>
+        <v>3627</v>
       </c>
       <c r="D580" t="s">
-        <v>3698</v>
+        <v>3697</v>
       </c>
       <c r="E580" t="s">
-        <v>3715</v>
+        <v>3714</v>
       </c>
       <c r="F580" t="s">
-        <v>3682</v>
+        <v>3681</v>
       </c>
       <c r="G580" t="s">
-        <v>3774</v>
+        <v>3773</v>
       </c>
     </row>
     <row r="581" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A581" t="s">
-        <v>3609</v>
+        <v>3608</v>
       </c>
       <c r="B581" t="s">
-        <v>3665</v>
+        <v>3664</v>
       </c>
       <c r="C581" t="s">
-        <v>3630</v>
+        <v>3629</v>
       </c>
       <c r="D581" t="s">
-        <v>3722</v>
+        <v>3721</v>
       </c>
       <c r="E581" t="s">
+        <v>3725</v>
+      </c>
+      <c r="F581" t="s">
         <v>3726</v>
       </c>
-      <c r="F581" t="s">
-        <v>3727</v>
-      </c>
       <c r="G581" t="s">
-        <v>3775</v>
+        <v>3774</v>
       </c>
     </row>
     <row r="582" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A582" t="s">
-        <v>3610</v>
+        <v>3609</v>
       </c>
       <c r="B582" t="s">
-        <v>3656</v>
+        <v>3655</v>
       </c>
       <c r="C582" t="s">
-        <v>3633</v>
+        <v>3632</v>
       </c>
       <c r="D582" t="s">
-        <v>3699</v>
+        <v>3698</v>
       </c>
       <c r="E582" t="s">
-        <v>3716</v>
+        <v>3715</v>
       </c>
       <c r="F582" t="s">
-        <v>3683</v>
+        <v>3682</v>
       </c>
       <c r="G582" t="s">
-        <v>3776</v>
+        <v>3775</v>
       </c>
     </row>
     <row r="583" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A583" t="s">
-        <v>3611</v>
+        <v>3610</v>
       </c>
       <c r="B583" t="s">
-        <v>3666</v>
+        <v>3665</v>
       </c>
       <c r="C583" t="s">
-        <v>3631</v>
+        <v>3630</v>
       </c>
       <c r="D583" t="s">
-        <v>3723</v>
+        <v>3722</v>
       </c>
       <c r="E583" t="s">
-        <v>3717</v>
+        <v>3716</v>
       </c>
       <c r="F583" t="s">
-        <v>3684</v>
+        <v>3683</v>
       </c>
       <c r="G583" t="s">
-        <v>3643</v>
+        <v>3642</v>
       </c>
     </row>
     <row r="584" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A584" t="s">
-        <v>3612</v>
+        <v>3611</v>
       </c>
       <c r="B584" t="s">
-        <v>3657</v>
+        <v>3656</v>
       </c>
       <c r="C584" t="s">
-        <v>3634</v>
+        <v>3633</v>
       </c>
       <c r="D584" t="s">
-        <v>3700</v>
+        <v>3699</v>
       </c>
       <c r="E584" t="s">
-        <v>3718</v>
+        <v>3717</v>
       </c>
       <c r="F584" t="s">
-        <v>3685</v>
+        <v>3684</v>
       </c>
       <c r="G584" t="s">
-        <v>3650</v>
+        <v>3649</v>
       </c>
     </row>
     <row r="585" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A585" t="s">
-        <v>3613</v>
+        <v>3612</v>
       </c>
       <c r="B585" t="s">
-        <v>3667</v>
+        <v>3666</v>
       </c>
       <c r="C585" t="s">
-        <v>3632</v>
+        <v>3631</v>
       </c>
       <c r="D585" t="s">
+        <v>3723</v>
+      </c>
+      <c r="E585" t="s">
         <v>3724</v>
       </c>
-      <c r="E585" t="s">
-        <v>3725</v>
-      </c>
       <c r="F585" t="s">
-        <v>3729</v>
+        <v>3728</v>
       </c>
       <c r="G585" t="s">
-        <v>3644</v>
+        <v>3643</v>
       </c>
     </row>
     <row r="586" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A586" t="s">
-        <v>3614</v>
+        <v>3613</v>
       </c>
       <c r="B586" t="s">
-        <v>3658</v>
+        <v>3657</v>
       </c>
       <c r="C586" t="s">
-        <v>3635</v>
+        <v>3634</v>
       </c>
       <c r="D586" t="s">
+        <v>3718</v>
+      </c>
+      <c r="E586" t="s">
         <v>3719</v>
       </c>
-      <c r="E586" t="s">
-        <v>3720</v>
-      </c>
       <c r="F586" t="s">
-        <v>3686</v>
+        <v>3685</v>
       </c>
       <c r="G586" t="s">
-        <v>3651</v>
+        <v>3650</v>
       </c>
     </row>
     <row r="587" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A587" t="s">
-        <v>3731</v>
+        <v>3730</v>
       </c>
       <c r="B587" t="s">
-        <v>3740</v>
+        <v>3739</v>
       </c>
       <c r="C587" t="s">
-        <v>3734</v>
+        <v>3733</v>
       </c>
       <c r="D587" t="s">
-        <v>3750</v>
+        <v>3749</v>
       </c>
       <c r="E587" t="s">
-        <v>3754</v>
+        <v>3753</v>
       </c>
       <c r="F587" t="s">
-        <v>3746</v>
+        <v>3745</v>
       </c>
       <c r="G587" t="s">
-        <v>3738</v>
+        <v>3737</v>
       </c>
     </row>
     <row r="588" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A588" t="s">
-        <v>3732</v>
+        <v>3731</v>
       </c>
       <c r="B588" t="s">
-        <v>3741</v>
+        <v>3740</v>
       </c>
       <c r="C588" t="s">
-        <v>3744</v>
+        <v>3743</v>
       </c>
       <c r="D588" t="s">
-        <v>3751</v>
+        <v>3750</v>
       </c>
       <c r="E588" t="s">
-        <v>3755</v>
+        <v>3754</v>
       </c>
       <c r="F588" t="s">
-        <v>3747</v>
+        <v>3746</v>
       </c>
       <c r="G588" t="s">
-        <v>3737</v>
+        <v>3736</v>
       </c>
     </row>
     <row r="589" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A589" t="s">
-        <v>3730</v>
+        <v>3729</v>
       </c>
       <c r="B589" t="s">
-        <v>3742</v>
+        <v>3741</v>
       </c>
       <c r="C589" t="s">
-        <v>3745</v>
+        <v>3744</v>
       </c>
       <c r="D589" t="s">
-        <v>3752</v>
+        <v>3751</v>
       </c>
       <c r="E589" t="s">
-        <v>3756</v>
+        <v>3755</v>
       </c>
       <c r="F589" t="s">
-        <v>3748</v>
+        <v>3747</v>
       </c>
       <c r="G589" t="s">
-        <v>3739</v>
+        <v>3738</v>
       </c>
     </row>
     <row r="590" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A590" t="s">
-        <v>3733</v>
+        <v>3732</v>
       </c>
       <c r="B590" t="s">
-        <v>3743</v>
+        <v>3742</v>
       </c>
       <c r="C590" t="s">
+        <v>3734</v>
+      </c>
+      <c r="D590" t="s">
+        <v>3752</v>
+      </c>
+      <c r="E590" t="s">
+        <v>3756</v>
+      </c>
+      <c r="F590" t="s">
+        <v>3748</v>
+      </c>
+      <c r="G590" t="s">
         <v>3735</v>
-      </c>
-      <c r="D590" t="s">
-        <v>3753</v>
-      </c>
-      <c r="E590" t="s">
-        <v>3757</v>
-      </c>
-      <c r="F590" t="s">
-        <v>3749</v>
-      </c>
-      <c r="G590" t="s">
-        <v>3736</v>
       </c>
     </row>
     <row r="591" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A591" t="s">
+        <v>3759</v>
+      </c>
+      <c r="B591" t="s">
+        <v>3765</v>
+      </c>
+      <c r="C591" t="s">
+        <v>3761</v>
+      </c>
+      <c r="D591" t="s">
+        <v>3763</v>
+      </c>
+      <c r="E591" t="s">
+        <v>3764</v>
+      </c>
+      <c r="F591" t="s">
+        <v>3762</v>
+      </c>
+      <c r="G591" t="s">
         <v>3760</v>
-      </c>
-      <c r="B591" t="s">
-        <v>3766</v>
-      </c>
-      <c r="C591" t="s">
-        <v>3762</v>
-      </c>
-      <c r="D591" t="s">
-        <v>3764</v>
-      </c>
-      <c r="E591" t="s">
-        <v>3765</v>
-      </c>
-      <c r="F591" t="s">
-        <v>3763</v>
-      </c>
-      <c r="G591" t="s">
-        <v>3761</v>
       </c>
     </row>
     <row r="592" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A592" t="s">
+        <v>3766</v>
+      </c>
+      <c r="B592" t="s">
+        <v>3768</v>
+      </c>
+      <c r="C592" t="s">
         <v>3767</v>
       </c>
-      <c r="B592" t="s">
+      <c r="D592" t="s">
+        <v>3771</v>
+      </c>
+      <c r="E592" t="s">
         <v>3769</v>
       </c>
-      <c r="C592" t="s">
+      <c r="F592" t="s">
+        <v>3770</v>
+      </c>
+      <c r="G592" t="s">
         <v>3768</v>
-      </c>
-      <c r="D592" t="s">
-        <v>3772</v>
-      </c>
-      <c r="E592" t="s">
-        <v>3770</v>
-      </c>
-      <c r="F592" t="s">
-        <v>3771</v>
-      </c>
-      <c r="G592" t="s">
-        <v>3769</v>
       </c>
     </row>
     <row r="593" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A593" t="s">
-        <v>3782</v>
+        <v>3781</v>
       </c>
       <c r="B593" t="s">
-        <v>3794</v>
+        <v>3793</v>
       </c>
       <c r="C593" t="s">
-        <v>3785</v>
+        <v>3784</v>
       </c>
       <c r="D593" t="s">
-        <v>3788</v>
+        <v>3787</v>
       </c>
       <c r="E593" t="s">
-        <v>3792</v>
+        <v>3791</v>
       </c>
       <c r="F593" t="s">
-        <v>3790</v>
+        <v>3789</v>
       </c>
       <c r="G593" t="s">
-        <v>3784</v>
+        <v>3783</v>
       </c>
     </row>
     <row r="594" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A594" t="s">
-        <v>3783</v>
+        <v>3782</v>
       </c>
       <c r="B594" t="s">
-        <v>3795</v>
+        <v>3794</v>
       </c>
       <c r="C594" t="s">
+        <v>3785</v>
+      </c>
+      <c r="D594" t="s">
+        <v>3788</v>
+      </c>
+      <c r="E594" t="s">
+        <v>3792</v>
+      </c>
+      <c r="F594" t="s">
+        <v>3790</v>
+      </c>
+      <c r="G594" t="s">
         <v>3786</v>
-      </c>
-      <c r="D594" t="s">
-        <v>3789</v>
-      </c>
-      <c r="E594" t="s">
-        <v>3793</v>
-      </c>
-      <c r="F594" t="s">
-        <v>3791</v>
-      </c>
-      <c r="G594" t="s">
-        <v>3787</v>
       </c>
     </row>
     <row r="595" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A595" t="s">
+        <v>3850</v>
+      </c>
+      <c r="B595" t="s">
         <v>3851</v>
       </c>
-      <c r="B595" t="s">
+      <c r="C595" t="s">
         <v>3852</v>
       </c>
-      <c r="C595" t="s">
+      <c r="D595" t="s">
+        <v>3858</v>
+      </c>
+      <c r="E595" t="s">
+        <v>3862</v>
+      </c>
+      <c r="F595" t="s">
+        <v>3860</v>
+      </c>
+      <c r="G595" t="s">
         <v>3853</v>
-      </c>
-      <c r="D595" t="s">
-        <v>3859</v>
-      </c>
-      <c r="E595" t="s">
-        <v>3863</v>
-      </c>
-      <c r="F595" t="s">
-        <v>3861</v>
-      </c>
-      <c r="G595" t="s">
-        <v>3854</v>
       </c>
     </row>
     <row r="596" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A596" t="s">
+        <v>3854</v>
+      </c>
+      <c r="B596" t="s">
+        <v>3857</v>
+      </c>
+      <c r="C596" t="s">
         <v>3855</v>
       </c>
-      <c r="B596" t="s">
-        <v>3858</v>
-      </c>
-      <c r="C596" t="s">
+      <c r="D596" t="s">
+        <v>3859</v>
+      </c>
+      <c r="E596" t="s">
+        <v>3863</v>
+      </c>
+      <c r="F596" t="s">
+        <v>3861</v>
+      </c>
+      <c r="G596" t="s">
         <v>3856</v>
-      </c>
-      <c r="D596" t="s">
-        <v>3860</v>
-      </c>
-      <c r="E596" t="s">
-        <v>3864</v>
-      </c>
-      <c r="F596" t="s">
-        <v>3862</v>
-      </c>
-      <c r="G596" t="s">
-        <v>3857</v>
       </c>
     </row>
     <row r="597" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A597" t="s">
+        <v>3885</v>
+      </c>
+      <c r="B597" t="s">
         <v>3886</v>
       </c>
-      <c r="B597" t="s">
+      <c r="C597" t="s">
         <v>3887</v>
       </c>
-      <c r="C597" t="s">
+      <c r="D597" t="s">
+        <v>3889</v>
+      </c>
+      <c r="E597" t="s">
+        <v>3891</v>
+      </c>
+      <c r="F597" t="s">
+        <v>3890</v>
+      </c>
+      <c r="G597" t="s">
         <v>3888</v>
-      </c>
-      <c r="D597" t="s">
-        <v>3890</v>
-      </c>
-      <c r="E597" t="s">
-        <v>3892</v>
-      </c>
-      <c r="F597" t="s">
-        <v>3891</v>
-      </c>
-      <c r="G597" t="s">
-        <v>3889</v>
       </c>
     </row>
     <row r="598" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A598" t="s">
+        <v>3901</v>
+      </c>
+      <c r="B598" t="s">
+        <v>3904</v>
+      </c>
+      <c r="C598" t="s">
+        <v>3903</v>
+      </c>
+      <c r="D598" t="s">
+        <v>3905</v>
+      </c>
+      <c r="E598" t="s">
+        <v>3907</v>
+      </c>
+      <c r="F598" t="s">
+        <v>3906</v>
+      </c>
+      <c r="G598" t="s">
         <v>3902</v>
       </c>
-      <c r="B598" t="s">
-        <v>3905</v>
-      </c>
-      <c r="C598" t="s">
-        <v>3904</v>
-      </c>
-      <c r="D598" t="s">
-        <v>3906</v>
-      </c>
-      <c r="E598" t="s">
-        <v>3908</v>
-      </c>
-      <c r="F598" t="s">
-        <v>3907</v>
-      </c>
-      <c r="G598" t="s">
-        <v>3903</v>
+    </row>
+    <row r="599" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A599" t="s">
+        <v>4007</v>
+      </c>
+      <c r="B599" t="s">
+        <v>4019</v>
+      </c>
+      <c r="C599" t="s">
+        <v>4009</v>
+      </c>
+      <c r="D599" t="s">
+        <v>4012</v>
+      </c>
+      <c r="E599" t="s">
+        <v>4016</v>
+      </c>
+      <c r="F599" t="s">
+        <v>4014</v>
+      </c>
+      <c r="G599" t="s">
+        <v>4011</v>
+      </c>
+    </row>
+    <row r="600" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A600" t="s">
+        <v>4008</v>
+      </c>
+      <c r="B600" t="s">
+        <v>4020</v>
+      </c>
+      <c r="C600" t="s">
+        <v>4010</v>
+      </c>
+      <c r="D600" t="s">
+        <v>4013</v>
+      </c>
+      <c r="E600" t="s">
+        <v>4017</v>
+      </c>
+      <c r="F600" t="s">
+        <v>4015</v>
+      </c>
+      <c r="G600" t="s">
+        <v>4018</v>
+      </c>
+    </row>
+    <row r="601" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A601" t="s">
+        <v>4039</v>
+      </c>
+      <c r="B601" t="s">
+        <v>4025</v>
+      </c>
+      <c r="C601" t="s">
+        <v>4056</v>
+      </c>
+      <c r="D601" t="s">
+        <v>4022</v>
+      </c>
+      <c r="E601" t="s">
+        <v>4023</v>
+      </c>
+      <c r="F601" t="s">
+        <v>4024</v>
+      </c>
+      <c r="G601" t="s">
+        <v>4021</v>
+      </c>
+    </row>
+    <row r="602" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A602" t="s">
+        <v>4040</v>
+      </c>
+      <c r="B602" t="s">
+        <v>4031</v>
+      </c>
+      <c r="C602" t="s">
+        <v>4055</v>
+      </c>
+      <c r="D602" s="4" t="s">
+        <v>4030</v>
+      </c>
+      <c r="E602" t="s">
+        <v>4028</v>
+      </c>
+      <c r="F602" t="s">
+        <v>4029</v>
+      </c>
+      <c r="G602" t="s">
+        <v>4027</v>
+      </c>
+    </row>
+    <row r="603" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A603" t="s">
+        <v>4032</v>
+      </c>
+      <c r="B603" t="s">
+        <v>4035</v>
+      </c>
+      <c r="C603" t="s">
+        <v>4033</v>
+      </c>
+      <c r="D603" s="4" t="s">
+        <v>4036</v>
+      </c>
+      <c r="E603" s="4" t="s">
+        <v>4038</v>
+      </c>
+      <c r="F603" t="s">
+        <v>4037</v>
+      </c>
+      <c r="G603" t="s">
+        <v>4034</v>
+      </c>
+    </row>
+    <row r="604" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A604" t="s">
+        <v>4041</v>
+      </c>
+      <c r="B604" t="s">
+        <v>4044</v>
+      </c>
+      <c r="C604" t="s">
+        <v>4054</v>
+      </c>
+      <c r="D604" t="s">
+        <v>4050</v>
+      </c>
+      <c r="E604" t="s">
+        <v>4046</v>
+      </c>
+      <c r="F604" t="s">
+        <v>4048</v>
+      </c>
+      <c r="G604" t="s">
+        <v>4043</v>
+      </c>
+    </row>
+    <row r="605" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A605" t="s">
+        <v>4042</v>
+      </c>
+      <c r="B605" t="s">
+        <v>4045</v>
+      </c>
+      <c r="C605" t="s">
+        <v>4052</v>
+      </c>
+      <c r="D605" t="s">
+        <v>4051</v>
+      </c>
+      <c r="E605" t="s">
+        <v>4047</v>
+      </c>
+      <c r="F605" t="s">
+        <v>4049</v>
+      </c>
+      <c r="G605" t="s">
+        <v>4053</v>
+      </c>
+    </row>
+    <row r="606" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A606" t="s">
+        <v>4057</v>
+      </c>
+      <c r="B606" t="s">
+        <v>4069</v>
+      </c>
+      <c r="C606" t="s">
+        <v>4059</v>
+      </c>
+      <c r="D606" t="s">
+        <v>4065</v>
+      </c>
+      <c r="E606" t="s">
+        <v>4063</v>
+      </c>
+      <c r="F606" t="s">
+        <v>4061</v>
+      </c>
+      <c r="G606" t="s">
+        <v>4067</v>
+      </c>
+    </row>
+    <row r="607" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A607" t="s">
+        <v>4058</v>
+      </c>
+      <c r="B607" t="s">
+        <v>4070</v>
+      </c>
+      <c r="C607" t="s">
+        <v>4060</v>
+      </c>
+      <c r="D607" t="s">
+        <v>4066</v>
+      </c>
+      <c r="E607" t="s">
+        <v>4064</v>
+      </c>
+      <c r="F607" t="s">
+        <v>4062</v>
+      </c>
+      <c r="G607" t="s">
+        <v>4068</v>
+      </c>
+    </row>
+    <row r="608" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A608" t="s">
+        <v>4071</v>
+      </c>
+      <c r="B608" t="s">
+        <v>4083</v>
+      </c>
+      <c r="C608" t="s">
+        <v>4073</v>
+      </c>
+      <c r="D608" t="s">
+        <v>4075</v>
+      </c>
+      <c r="E608" t="s">
+        <v>4077</v>
+      </c>
+      <c r="F608" t="s">
+        <v>4079</v>
+      </c>
+      <c r="G608" t="s">
+        <v>4081</v>
+      </c>
+    </row>
+    <row r="609" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A609" t="s">
+        <v>4072</v>
+      </c>
+      <c r="B609" t="s">
+        <v>4084</v>
+      </c>
+      <c r="C609" t="s">
+        <v>4074</v>
+      </c>
+      <c r="D609" t="s">
+        <v>4076</v>
+      </c>
+      <c r="E609" t="s">
+        <v>4078</v>
+      </c>
+      <c r="F609" t="s">
+        <v>4080</v>
+      </c>
+      <c r="G609" t="s">
+        <v>4082</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates for Slideshow version 3.17.12
</commit_message>
<xml_diff>
--- a/backend/localization.xlsx
+++ b/backend/localization.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mimac\Documents\NetBeansProjects\slideshow-localization\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{786B8D5A-2B6B-41F7-AE14-39F23B0F8C7E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95DAD6F2-7135-4C3F-BEC5-F79BC45A60C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3208" yWindow="1839" windowWidth="36784" windowHeight="14643" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-114" yWindow="-114" windowWidth="27602" windowHeight="15027" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="properties" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6910" uniqueCount="6630">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6950" uniqueCount="6670">
   <si>
     <t>keys</t>
   </si>
@@ -19938,6 +19938,126 @@
   </si>
   <si>
     <t>Whether the time part should be displayed in bold font.</t>
+  </si>
+  <si>
+    <t>reboot_on_hdmi_plug_in</t>
+  </si>
+  <si>
+    <t>reboot_on_hdmi_plug_in_help</t>
+  </si>
+  <si>
+    <t>Reboot on HDMI plug in</t>
+  </si>
+  <si>
+    <t>After detecting the HDMI cable was plugged in, the app will automatically reboot the device. Usable on some devices with video decoding problems when no HDMI device is plugged in.</t>
+  </si>
+  <si>
+    <t>Reštartovať zariadenie pri pripojení HDMI kábla</t>
+  </si>
+  <si>
+    <t>Po zapojení HDMI kábla sa zariadenie automaticky reštartuje. Vhodné pre niektoré zariadenia s problémami pri dekódovaní videa, ak nie je zapojené žiadne HDMI zariadenie.</t>
+  </si>
+  <si>
+    <t>Restartovat zařízení při připojení HDMI kabelu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Po zapojení kabelu HDMI se zařízení automaticky restartuje. Vhodné pro některá zařízení s problémy při dekódování videa, pokud není zapojeno žádné HDMI zařízení. </t>
+  </si>
+  <si>
+    <t>Reinicie no plug-in HDMI</t>
+  </si>
+  <si>
+    <t>Depois de detectar que o cabo HDMI foi conectado, o aplicativo irá reiniciar automaticamente o dispositivo. Pode ser usado em alguns dispositivos com problemas de decodificação de vídeo quando nenhum dispositivo HDMI está conectado.</t>
+  </si>
+  <si>
+    <t>Ponovo pokrenite na HDMI priključku</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nakon što otkrije da je HDMI kabel priključen, aplikacija će automatski ponovno pokrenuti uređaj. Koristi se na nekim uređajima s problemima dekodiranja videa ako nije priključen HDMI uređaj. </t>
+  </si>
+  <si>
+    <t>Neustart über HDMI-Plug-in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nachdem das HDMI-Kabel eingesteckt wurde, startet die App das Gerät automatisch neu. Verwendbar auf einigen Geräten mit Videodecodierungsproblemen, wenn kein HDMI-Gerät angeschlossen ist. </t>
+  </si>
+  <si>
+    <t>Redémarrer sur prise HDMI</t>
+  </si>
+  <si>
+    <t>Après avoir détecté que le câble HDMI était branché, l'application redémarrera automatiquement l'appareil. Utilisable sur certains appareils ayant des problèmes de décodage vidéo lorsqu'aucun appareil HDMI n'est branché.</t>
+  </si>
+  <si>
+    <t>Riavvia sulla presa HDMI</t>
+  </si>
+  <si>
+    <t>Dopo aver rilevato che il cavo HDMI è stato collegato, l'app riavvierà automaticamente il dispositivo. Utilizzabile su alcuni dispositivi con problemi di decodifica video quando non è collegato alcun dispositivo HDMI.</t>
+  </si>
+  <si>
+    <t>Uruchom ponownie po wtyczce HDMI</t>
+  </si>
+  <si>
+    <t>Po wykryciu, że kabel HDMI został podłączony, aplikacja automatycznie zrestartuje urządzenie. Można używać na niektórych urządzeniach z problemami z dekodowaniem wideo, gdy żadne urządzenie HDMI nie jest podłączone.</t>
+  </si>
+  <si>
+    <t>preload_items_in_playlist</t>
+  </si>
+  <si>
+    <t>preload_items_in_playlist_help</t>
+  </si>
+  <si>
+    <t>Preload items in playlist</t>
+  </si>
+  <si>
+    <t>Prednačítať položky v playliste</t>
+  </si>
+  <si>
+    <t>Allow loading some of the items (e.g. video files) in advance, so the delay between items is shorter.</t>
+  </si>
+  <si>
+    <t>Povoliť načítanie niektorých položiek (napr. video súbory) dopredu, aby bola pauza medzi položkami kratšia.</t>
+  </si>
+  <si>
+    <t>Pré-carregar itens na lista de reprodução</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Permitir o carregamento de alguns dos itens (por exemplo, arquivos de vídeo) com antecedência, para que o atraso entre os itens seja menor. </t>
+  </si>
+  <si>
+    <t>Precarica elementi nella playlist</t>
+  </si>
+  <si>
+    <t>Consenti il caricamento anticipato di alcuni elementi (ad es. file video), in modo che il ritardo tra gli elementi sia più breve.</t>
+  </si>
+  <si>
+    <t>Wstępnie wczytuj elementy z listy odtwarzania</t>
+  </si>
+  <si>
+    <t>Zezwól na wczytanie niektórych elementów (np. plików wideo) z wyprzedzeniem, aby opóźnienie między elementami było krótsze.</t>
+  </si>
+  <si>
+    <t>Elemente in Playlist vorladen</t>
+  </si>
+  <si>
+    <t>Lassen Sie einige der Elemente (z. B. Videodateien) im Voraus laden, damit die Verzögerung zwischen den Elementen kürzer ist.</t>
+  </si>
+  <si>
+    <t>Précharger des éléments dans la liste de lecture</t>
+  </si>
+  <si>
+    <t>Autorisez le chargement de certains éléments (par exemple, des fichiers vidéo) à l'avance, afin que le délai entre les éléments soit plus court.</t>
+  </si>
+  <si>
+    <t>Unaprijed učitajte stavke na popisu za reprodukciju</t>
+  </si>
+  <si>
+    <t>Dopustite unaprijed učitavanje nekih stavki (npr. Video datoteka) kako bi kašnjenje između stavki bilo kraće.</t>
+  </si>
+  <si>
+    <t>Povolit načítání některých položek (např. video soubory) dopředu, aby byla pauza mezi položkami kratší.</t>
+  </si>
+  <si>
+    <t>Prednačítat položky v playlistu</t>
   </si>
 </sst>
 </file>
@@ -20306,13 +20426,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J691"/>
+  <dimension ref="A1:J695"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B676" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D691" sqref="D691"/>
+      <selection pane="bottomRight" activeCell="C695" sqref="C695"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -42441,6 +42561,134 @@
         <v>6614</v>
       </c>
     </row>
+    <row r="692" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A692" t="s">
+        <v>6630</v>
+      </c>
+      <c r="B692" t="s">
+        <v>6640</v>
+      </c>
+      <c r="C692" t="s">
+        <v>6636</v>
+      </c>
+      <c r="D692" t="s">
+        <v>6632</v>
+      </c>
+      <c r="E692" t="s">
+        <v>6644</v>
+      </c>
+      <c r="F692" t="s">
+        <v>6642</v>
+      </c>
+      <c r="G692" t="s">
+        <v>6646</v>
+      </c>
+      <c r="H692" t="s">
+        <v>6648</v>
+      </c>
+      <c r="I692" t="s">
+        <v>6638</v>
+      </c>
+      <c r="J692" s="6" t="s">
+        <v>6634</v>
+      </c>
+    </row>
+    <row r="693" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A693" t="s">
+        <v>6631</v>
+      </c>
+      <c r="B693" t="s">
+        <v>6641</v>
+      </c>
+      <c r="C693" t="s">
+        <v>6637</v>
+      </c>
+      <c r="D693" t="s">
+        <v>6633</v>
+      </c>
+      <c r="E693" t="s">
+        <v>6645</v>
+      </c>
+      <c r="F693" t="s">
+        <v>6643</v>
+      </c>
+      <c r="G693" t="s">
+        <v>6647</v>
+      </c>
+      <c r="H693" t="s">
+        <v>6649</v>
+      </c>
+      <c r="I693" t="s">
+        <v>6639</v>
+      </c>
+      <c r="J693" s="6" t="s">
+        <v>6635</v>
+      </c>
+    </row>
+    <row r="694" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A694" t="s">
+        <v>6650</v>
+      </c>
+      <c r="B694" t="s">
+        <v>6666</v>
+      </c>
+      <c r="C694" t="s">
+        <v>6669</v>
+      </c>
+      <c r="D694" t="s">
+        <v>6652</v>
+      </c>
+      <c r="E694" t="s">
+        <v>6664</v>
+      </c>
+      <c r="F694" t="s">
+        <v>6662</v>
+      </c>
+      <c r="G694" t="s">
+        <v>6658</v>
+      </c>
+      <c r="H694" t="s">
+        <v>6660</v>
+      </c>
+      <c r="I694" t="s">
+        <v>6656</v>
+      </c>
+      <c r="J694" s="6" t="s">
+        <v>6653</v>
+      </c>
+    </row>
+    <row r="695" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A695" t="s">
+        <v>6651</v>
+      </c>
+      <c r="B695" t="s">
+        <v>6667</v>
+      </c>
+      <c r="C695" t="s">
+        <v>6668</v>
+      </c>
+      <c r="D695" t="s">
+        <v>6654</v>
+      </c>
+      <c r="E695" t="s">
+        <v>6665</v>
+      </c>
+      <c r="F695" t="s">
+        <v>6663</v>
+      </c>
+      <c r="G695" t="s">
+        <v>6659</v>
+      </c>
+      <c r="H695" t="s">
+        <v>6661</v>
+      </c>
+      <c r="I695" t="s">
+        <v>6657</v>
+      </c>
+      <c r="J695" s="6" t="s">
+        <v>6655</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updates for Slideshow version 3.19.2
</commit_message>
<xml_diff>
--- a/backend/localization.xlsx
+++ b/backend/localization.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mimac\Documents\NetBeansProjects\slideshow-localization\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{955B1ACC-6F22-4E67-9080-3B3F08A23AA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{963DE67F-2B5E-4E9C-8536-8D4BC1BAD975}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-114" yWindow="-114" windowWidth="49274" windowHeight="20160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="4234" windowWidth="49046" windowHeight="9995" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="properties" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8424" uniqueCount="8090">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8438" uniqueCount="8104">
   <si>
     <t>keys</t>
   </si>
@@ -24290,6 +24290,48 @@
   </si>
   <si>
     <t>Нажмите кнопку выше, чтобы войти в свою учетную запись %s. Браузер откроется на &lt;b&gt;экране устройства&lt;/b&gt; с формой входа (это означает, что вам потребуется прямой доступ к устройству). После входа в систему вернитесь в приложение, чтобы продолжить. Прежде чем продолжить, ознакомьтесь с политикой конфиденциальности на странице &lt;a href="https://slideshow.digital/privacy-policy/" target="_blank"&gt;https://slideshow.digital/privacy-policy&lt;/a&gt;.</t>
+  </si>
+  <si>
+    <t>Can't open settings directly. Please try navigating to Android Settings - Apps - this app - Permissions and allow "Appear on top" or "Display over other apps" permission.</t>
+  </si>
+  <si>
+    <t>permission_start_at_boot_error</t>
+  </si>
+  <si>
+    <t>Не могу открыть настройки напрямую. Попробуйте перейти в Настройки Android - Приложения - Это приложение - Разрешения и разрешите «Отображать поверх других приложений» или «Отображать поверх других приложений».</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nastavení nelze otevřít přímo. Zkuste prosím přejít do Nastavení Androidu – Aplikace – tato aplikace – Oprávnění a povolte oprávnění „Zobrazovat nahoře“ nebo „Zobrazovat přes jiné aplikace“. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nastavenia nie je možné otvoriť priamo. Skúste prejsť do časti Nastavenia systému Android – Aplikácie – táto aplikácia – Povolenia a povoľte „Zobraziť navrchu“ alebo „Zobraziť cez iné aplikácie“. </t>
+  </si>
+  <si>
+    <t>Ne mogu izravno otvoriti postavke. Pokušajte prijeći na Postavke Androida - Aplikacije - ova aplikacija - Dopuštenja i dopustite "Pojavi se na vrhu" ili "Prikaz preko drugih aplikacija".</t>
+  </si>
+  <si>
+    <t>Impossible d'ouvrir les paramètres directement. Veuillez essayer de naviguer vers Paramètres Android - Applications - cette application - Autorisations et autorisez "Apparaître en haut" ou "Afficher sur d'autres applications".</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Einstellungen können nicht direkt geöffnet werden. Bitte versuchen Sie, zu Android-Einstellungen - Apps - Diese App - Berechtigungen zu navigieren und "Oben anzeigen" oder "Über anderen Apps anzeigen" zuzulassen. </t>
+  </si>
+  <si>
+    <t>Impossibile aprire le impostazioni direttamente. Prova a navigare in Impostazioni Android - App - questa app - Autorizzazioni e consenti "Appari in primo piano" o "Visualizza su altre app".</t>
+  </si>
+  <si>
+    <t>Nie można bezpośrednio otworzyć ustawień. Spróbuj przejść do Ustawienia Androida – Aplikacje – ta aplikacja – Uprawnienia i zezwól na „Wyświetlaj na wierzchu” lub „Wyświetlaj nad innymi aplikacjami”.</t>
+  </si>
+  <si>
+    <t>Não é possível abrir as configurações diretamente. Tente navegar para Configurações do Android - Aplicativos - este aplicativo - Permissões e permitir "Aparecer na parte superior" ou "Exibir sobre outros aplicativos".</t>
+  </si>
+  <si>
+    <t>No se puede abrir la configuración directamente. Intente navegar a Configuración de Android - Aplicaciones - esta aplicación - Permisos y permita "Aparecer en la parte superior" o "Mostrar sobre otras aplicaciones".</t>
+  </si>
+  <si>
+    <t>storage_permissions</t>
+  </si>
+  <si>
+    <t>Storage permissions</t>
   </si>
 </sst>
 </file>
@@ -24647,13 +24689,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L702"/>
+  <dimension ref="A1:L704"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B476" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B677" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J503" sqref="J503"/>
+      <selection pane="bottomRight" activeCell="D705" sqref="D705"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -51342,6 +51384,52 @@
         <v>7386</v>
       </c>
     </row>
+    <row r="703" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A703" t="s">
+        <v>8091</v>
+      </c>
+      <c r="B703" t="s">
+        <v>8095</v>
+      </c>
+      <c r="C703" t="s">
+        <v>8093</v>
+      </c>
+      <c r="D703" t="s">
+        <v>8090</v>
+      </c>
+      <c r="E703" t="s">
+        <v>8096</v>
+      </c>
+      <c r="F703" t="s">
+        <v>8097</v>
+      </c>
+      <c r="G703" t="s">
+        <v>8098</v>
+      </c>
+      <c r="H703" t="s">
+        <v>8099</v>
+      </c>
+      <c r="I703" t="s">
+        <v>8100</v>
+      </c>
+      <c r="J703" t="s">
+        <v>8092</v>
+      </c>
+      <c r="K703" t="s">
+        <v>8094</v>
+      </c>
+      <c r="L703" t="s">
+        <v>8101</v>
+      </c>
+    </row>
+    <row r="704" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A704" t="s">
+        <v>8102</v>
+      </c>
+      <c r="D704" t="s">
+        <v>8103</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updates for Slideshow version 3.22.1
</commit_message>
<xml_diff>
--- a/backend/localization.xlsx
+++ b/backend/localization.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mimac\Documents\NetBeansProjects\slideshow-localization\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A000860-C751-47A4-A542-EF78A4D548C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F375FF29-E890-43B8-8D87-F58E503DC7A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-114" yWindow="-114" windowWidth="49274" windowHeight="20160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4149" yWindow="4149" windowWidth="20531" windowHeight="10793" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="properties" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8568" uniqueCount="8241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8664" uniqueCount="8327">
   <si>
     <t>keys</t>
   </si>
@@ -24565,18 +24565,12 @@
     <t>Názov MQTT topicu</t>
   </si>
   <si>
-    <t>Automaticky zasielať informácie o zariadení a štatistiky cez MQTT každé dve minúty. &lt;br&gt;&lt;i&gt;Reštart aplikácie je vyžadovaný pre aplikovanie tohto nastavenia.&lt;/i&gt;</t>
-  </si>
-  <si>
     <t>Ak nie je zadané, použije sa MAC adresa zariadenia (ak je dostupná)&lt;br&gt;&lt;i&gt;Reštart aplikácie je vyžadovaný pre aplikovanie tohto nastavenia.&lt;/i&gt;</t>
   </si>
   <si>
     <t>Relatório de dados por meio do MQTT</t>
   </si>
   <si>
-    <t>Envie automaticamente informações e estatísticas do dispositivo por meio do MQTT a cada 2 minutos.&lt;br&gt;&lt;i&gt;É necessário recarregar para aplicar essa alteração.&lt;/i&gt;</t>
-  </si>
-  <si>
     <t>Nome do tópico MQTT</t>
   </si>
   <si>
@@ -24586,9 +24580,6 @@
     <t>Informar datos a través de MQTT</t>
   </si>
   <si>
-    <t>Envíe automáticamente información y estadísticas del dispositivo a través de MQTT cada 2 minutos.&lt;br&gt;&lt;i&gt;Es necesario volver a cargar para aplicar este cambio.&lt;/i&gt;</t>
-  </si>
-  <si>
     <t>Nombre del tema MQTT</t>
   </si>
   <si>
@@ -24598,9 +24589,6 @@
     <t>Raportuj dane przez MQTT</t>
   </si>
   <si>
-    <t>Automatycznie wysyłaj informacje o urządzeniu i statystyki przez MQTT co 2 minuty.&lt;br&gt;&lt;i&gt;Do zastosowania tej zmiany wymagane jest ponowne załadowanie.&lt;/i&gt;</t>
-  </si>
-  <si>
     <t>Nazwa tematu MQTT</t>
   </si>
   <si>
@@ -24610,9 +24598,6 @@
     <t>Riportare i dati tramite MQTT</t>
   </si>
   <si>
-    <t>Invia automaticamente informazioni e statistiche sul dispositivo tramite MQTT ogni 2 minuti.&lt;br&gt;&lt;i&gt;Per applicare questa modifica è necessario ricaricare.&lt;/i&gt;</t>
-  </si>
-  <si>
     <t>Nome argomento MQTT</t>
   </si>
   <si>
@@ -24622,9 +24607,6 @@
     <t>Rapporter les données via MQTT</t>
   </si>
   <si>
-    <t>Envoyez automatiquement les informations et les statistiques sur l'appareil via MQTT toutes les 2 minutes.&lt;br&gt;&lt;i&gt;Un rechargement est nécessaire pour appliquer cette modification.&lt;/i&gt;</t>
-  </si>
-  <si>
     <t>Nom du sujet MQTT</t>
   </si>
   <si>
@@ -24634,9 +24616,6 @@
     <t>Melden Sie Daten über MQTT</t>
   </si>
   <si>
-    <t>Senden Sie automatisch alle 2 Minuten Geräteinformationen und Statistiken über MQTT.&lt;br&gt;&lt;i&gt;Neu laden ist erforderlich, um diese Änderung zu übernehmen.&lt;/i&gt;</t>
-  </si>
-  <si>
     <t>Name des MQTT-Themas</t>
   </si>
   <si>
@@ -24646,9 +24625,6 @@
     <t>Prijavite podatke putem MQTT-a</t>
   </si>
   <si>
-    <t>Automatski šaljite podatke o uređaju i statistiku putem MQTT svake 2 minute.&lt;br&gt;&lt;i&gt;Za primjenu ove promjene potrebno je ponovno učitavanje.&lt;/i&gt;</t>
-  </si>
-  <si>
     <t>Naziv teme MQTT</t>
   </si>
   <si>
@@ -24658,9 +24634,6 @@
     <t>Сообщать данные через MQTT</t>
   </si>
   <si>
-    <t>Автоматически отправлять информацию об устройстве и статистику через MQTT каждые 2 минуты.&lt;br&gt;&lt;i&gt;Для применения этого изменения требуется перезагрузка.&lt;/i&gt;</t>
-  </si>
-  <si>
     <t>Название темы MQTT</t>
   </si>
   <si>
@@ -24670,9 +24643,6 @@
     <t>Zasílat report přes MQTT</t>
   </si>
   <si>
-    <t>Automaticky zasílat informace o zařízení a statistiky přes MQTT každé dvě minuty. &lt;br&gt;&lt;i&gt;Restart aplikace je vyžadován pro aplikování tohoto nastavení.&lt;/i&gt;</t>
-  </si>
-  <si>
     <t>Název MQTT topicu</t>
   </si>
   <si>
@@ -24685,9 +24655,6 @@
     <t>MQTT topic name</t>
   </si>
   <si>
-    <t>Automatically send device info and statistics through MQTT every 2 minutes.&lt;br&gt;&lt;i&gt;Reload is required for applying this change.&lt;/i&gt;</t>
-  </si>
-  <si>
     <t>If not entered, MAC address of the device will be used (if available).&lt;br&gt;&lt;i&gt;Reload is required for applying this change.&lt;/i&gt;</t>
   </si>
   <si>
@@ -24743,6 +24710,297 @@
   </si>
   <si>
     <t>&lt;p&gt;Slideshow app has been successfully updated to a newer version. There are following new features:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;MQTT: added support for WebSockets, optional automatic statistics sending and custom topic setting&lt;/li&gt;&lt;li&gt;File Manager: added possibility to set particular file length or mute via Properties&lt;/li&gt;&lt;li&gt;Home page: added welcome message (only on first start after update)&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;You can find documentation for features on &lt;a href="https://slideshow.digital/documentation/" target="_blank"&gt;https://slideshow.digital/documentation/&lt;/a&gt;  and watch tutorials on  &lt;a href="https://www.youtube.com/channel/UCJFSXCItojY4PS76JNr_pdQ" target="_blank"&gt;https://www.youtube.com/channel/UCJFSXCItojY4PS76JNr_pdQ&lt;/a&gt;.&lt;/p&gt;&lt;p&gt;If you like Slideshow app, you can support the development by rating the app on &lt;a href="https://play.google.com/store/apps/details?id=sk.mimac.slideshow" target="_blank"&gt;Google Play&lt;/a&gt; or buy us a &lt;a href="https://ko-fi.com/slideshow" target="_blank"&gt;coffee&lt;/a&gt;.&lt;/p&gt;&lt;span style='float:right'&gt;-- The Development team --&lt;/span&gt;</t>
+  </si>
+  <si>
+    <t>mqtt_report_statistics</t>
+  </si>
+  <si>
+    <t>mqtt_report_statistics_help</t>
+  </si>
+  <si>
+    <t>Report statistics through MQTT</t>
+  </si>
+  <si>
+    <t>Statistiques de rapport via MQTT</t>
+  </si>
+  <si>
+    <t>Signaler les statistiques d'affichage des fichiers via MQTT&lt;br&gt;&lt;i&gt;Un rechargement est nécessaire pour appliquer cette modification.&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>Melden Sie Statistiken über MQTT</t>
+  </si>
+  <si>
+    <t>Melden Sie Anzeigestatistiken von Dateien über MQTT&lt;br&gt;&lt;i&gt;Neues Laden ist erforderlich, um diese Änderung zu übernehmen.&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>Segnala le statistiche tramite MQTT</t>
+  </si>
+  <si>
+    <t>Segnala le statistiche di visualizzazione dei file tramite MQTT&lt;br&gt;&lt;i&gt;È necessario ricaricare per applicare questa modifica.&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>Relatório de estatísticas por meio do MQTT</t>
+  </si>
+  <si>
+    <t>Relatório de estatísticas de exibição de arquivos por meio do MQTT&lt;br&gt;&lt;i&gt;Recarregar é necessário para aplicar essa alteração.&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>Raportuj statystyki przez MQTT</t>
+  </si>
+  <si>
+    <t>Raportuj statystyki wyświetlania plików przez MQTT&lt;br&gt;&lt;i&gt;Do zastosowania tej zmiany wymagane jest ponowne wczytanie.&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>Отчет о статистике через MQTT</t>
+  </si>
+  <si>
+    <t>Отчет о статистике отображения файлов через MQTT&lt;br&gt;&lt;i&gt;Для применения этого изменения требуется перезагрузка.&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>Informe de estadísticas a través de MQTT</t>
+  </si>
+  <si>
+    <t>Informe de estadísticas de visualización de archivos a través de MQTT&lt;br&gt;&lt;i&gt;Es necesario volver a cargar para aplicar este cambio.&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>Prijavite statistiku putem MQTT-a</t>
+  </si>
+  <si>
+    <t>Izvještaj o statistici prikaza datoteka putem MQTT-a&lt;br&gt;&lt;i&gt;Za primjenu ove promjene potrebno je ponovno učitavanje.&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>Zasielať štatistiky cez MQTT</t>
+  </si>
+  <si>
+    <t>Automaticky zasielať štatistiky o zobrazených súboroch cez MQTT každé dve minúty.&lt;br&gt;&lt;i&gt;Reštart aplikácie je vyžadovaný pre aplikovanie tohto nastavenia.&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>Zasílat statistiky přes MQTT</t>
+  </si>
+  <si>
+    <t>Automaticky zasílat statistiky o zobrazených souborech přes MQTT každé dvě minuty.&lt;br&gt;&lt;i&gt;Restart aplikace je vyžadován pro aplikování tohoto nastavení.&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>Automatically send device info through MQTT every 2 minutes.&lt;br&gt;&lt;i&gt;Reload is required for applying this change.&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>Automatically report display statistics of files through MQTT every two minutes.&lt;br&gt;&lt;i&gt;Reload is required for applying this change.&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>Envoyez automatiquement les informations sur l'appareil via MQTT toutes les 2 minutes.&lt;br&gt;&lt;i&gt;Un rechargement est nécessaire pour appliquer cette modification.&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>Automatski šaljite podatke o uređaju putem MQTT svake 2 minute.&lt;br&gt;&lt;i&gt;Za primjenu ove promjene potrebno je ponovno učitavanje.&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>Automaticky zasílat informace o zařízení přes MQTT každé dvě minuty. &lt;br&gt;&lt;i&gt;Restart aplikace je vyžadován pro aplikování tohoto nastavení.&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>Senden Sie automatisch alle 2 Minuten Geräteinformationen über MQTT.&lt;br&gt;&lt;i&gt;Neu laden ist erforderlich, um diese Änderung zu übernehmen.&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>Invia automaticamente informazioni sul dispositivo tramite MQTT ogni 2 minuti.&lt;br&gt;&lt;i&gt;Per applicare questa modifica è necessario ricaricare.&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>Automatycznie wysyłaj informacje o urządzeniu przez MQTT co 2 minuty.&lt;br&gt;&lt;i&gt;Do zastosowania tej zmiany wymagane jest ponowne załadowanie.&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>Envie automaticamente informações do dispositivo por meio do MQTT a cada 2 minutos.&lt;br&gt;&lt;i&gt;É necessário recarregar para aplicar essa alteração.&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>Автоматически отправлять информацию об устройстве через MQTT каждые 2 минуты.&lt;br&gt;&lt;i&gt;Для применения этого изменения требуется перезагрузка.&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>Automaticky zasielať informácie o zariadení cez MQTT každé dve minúty. &lt;br&gt;&lt;i&gt;Reštart aplikácie je vyžadovaný pre aplikovanie tohto nastavenia.&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>Envíe automáticamente información del dispositivo a través de MQTT cada 2 minutos.&lt;br&gt;&lt;i&gt;Es necesario volver a cargar para aplicar este cambio.&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>license_key_enter</t>
+  </si>
+  <si>
+    <t>free_trial</t>
+  </si>
+  <si>
+    <t>licence_key_how_to_get</t>
+  </si>
+  <si>
+    <t>license_key_device_id</t>
+  </si>
+  <si>
+    <t>license_key_valid</t>
+  </si>
+  <si>
+    <t>license_key_invalid</t>
+  </si>
+  <si>
+    <t>Free trial</t>
+  </si>
+  <si>
+    <t>Enter license key</t>
+  </si>
+  <si>
+    <t>License key is valid, application will be restarted</t>
+  </si>
+  <si>
+    <t>License key is invalid, please check if it was entered correctly</t>
+  </si>
+  <si>
+    <t>Please contact support to get the license key</t>
+  </si>
+  <si>
+    <t>Zadať licenčný kľúč</t>
+  </si>
+  <si>
+    <t>Licenčný kľúč je správny, aplikácia sa reštartuje</t>
+  </si>
+  <si>
+    <t>Licenčný kľúč nie je správny, prosím skontrolujte preklepy</t>
+  </si>
+  <si>
+    <t>Enter the license key below for the following device ID</t>
+  </si>
+  <si>
+    <t>Zadajte nižšie licenčný kľúč pre nasledujúce ID zariadenia</t>
+  </si>
+  <si>
+    <t>Prosím kontaktujte podporu pre získanie licenčného kľúča</t>
+  </si>
+  <si>
+    <t>Para licenciar favor entrar em contato com o suporte</t>
+  </si>
+  <si>
+    <t>Zadat licenční klíč</t>
+  </si>
+  <si>
+    <t>Prosím kontaktujte podporu pro získání licenčního klíče</t>
+  </si>
+  <si>
+    <t>Zadejte níže licenční klíč pro následující ID zařízení</t>
+  </si>
+  <si>
+    <t>Licenční klíč je správný, aplikace se restartuje</t>
+  </si>
+  <si>
+    <t>Licenční klíč není správný, prosím zkontrolujte překlepy</t>
+  </si>
+  <si>
+    <t>Insira chave da licença</t>
+  </si>
+  <si>
+    <t>Digite a chave de licença abaixo para o seguinte ID do dispositivo</t>
+  </si>
+  <si>
+    <t>A chave de licença é válida, o aplicativo será reiniciado</t>
+  </si>
+  <si>
+    <t>A chave de licença é inválida, verifique se foi digitada corretamente</t>
+  </si>
+  <si>
+    <t>Introduzca la clave de la licencia</t>
+  </si>
+  <si>
+    <t>Póngase en contacto con el soporte para obtener la clave de licencia</t>
+  </si>
+  <si>
+    <t>Ingrese la clave de licencia a continuación para el siguiente ID de dispositivo</t>
+  </si>
+  <si>
+    <t>La clave de licencia es válida, la aplicación se reiniciará</t>
+  </si>
+  <si>
+    <t>La clave de licencia no es válida, verifique si se ingresó correctamente</t>
+  </si>
+  <si>
+    <t>Unesite licencni ključ</t>
+  </si>
+  <si>
+    <t>Kontaktirajte podršku kako biste dobili licencni ključ</t>
+  </si>
+  <si>
+    <t>Unesite licencni ključ ispod za sljedeći ID uređaja</t>
+  </si>
+  <si>
+    <t>Ključ licence je važeći, aplikacija će se ponovno pokrenuti</t>
+  </si>
+  <si>
+    <t>Ključ licence je nevažeći, provjerite je li ispravno unesen</t>
+  </si>
+  <si>
+    <t>Entrez la clé de licence</t>
+  </si>
+  <si>
+    <t>Veuillez contacter le support pour obtenir la clé de licence</t>
+  </si>
+  <si>
+    <t>Entrez la clé de licence ci-dessous pour l'ID d'appareil suivant</t>
+  </si>
+  <si>
+    <t>La clé de licence est valide, l'application va être redémarrée</t>
+  </si>
+  <si>
+    <t>La clé de licence n'est pas valide, veuillez vérifier si elle a été saisie correctement</t>
+  </si>
+  <si>
+    <t>Gebe den Lizenzschlüssel ein</t>
+  </si>
+  <si>
+    <t>Bitte wenden Sie sich an den Support, um den Lizenzschlüssel zu erhalten</t>
+  </si>
+  <si>
+    <t>Geben Sie unten den Lizenzschlüssel für die folgende Geräte-ID ein</t>
+  </si>
+  <si>
+    <t>Der Lizenzschlüssel ist gültig, die Anwendung wird neu gestartet</t>
+  </si>
+  <si>
+    <t>Der Lizenzschlüssel ist ungültig, bitte überprüfen Sie, ob er korrekt eingegeben wurde</t>
+  </si>
+  <si>
+    <t>Inserisci la chiave di licenza</t>
+  </si>
+  <si>
+    <t>Si prega di contattare l'assistenza per ottenere la chiave di licenza</t>
+  </si>
+  <si>
+    <t>Immettere la chiave di licenza di seguito per il seguente ID dispositivo</t>
+  </si>
+  <si>
+    <t>La chiave di licenza è valida, l'applicazione verrà riavviata</t>
+  </si>
+  <si>
+    <t>La chiave di licenza non è valida, controlla se è stata inserita correttamente</t>
+  </si>
+  <si>
+    <t>Wprowadź klucz licencyjny</t>
+  </si>
+  <si>
+    <t>Skontaktuj się z pomocą techniczną, aby uzyskać klucz licencyjny</t>
+  </si>
+  <si>
+    <t>Wprowadź klucz licencyjny poniżej dla następującego identyfikatora urządzenia</t>
+  </si>
+  <si>
+    <t>Klucz licencyjny jest ważny, aplikacja zostanie ponownie uruchomiona</t>
+  </si>
+  <si>
+    <t>Klucz licencyjny jest nieprawidłowy, sprawdź, czy został wprowadzony poprawnie</t>
+  </si>
+  <si>
+    <t>Введите лицензионный ключ</t>
+  </si>
+  <si>
+    <t>Обратитесь в службу поддержки, чтобы получить лицензионный ключ</t>
+  </si>
+  <si>
+    <t>Введите лицензионный ключ ниже для следующего идентификатора устройства</t>
+  </si>
+  <si>
+    <t>Лицензионный ключ действителен, приложение будет перезапущено</t>
+  </si>
+  <si>
+    <t>Лицензионный ключ недействителен, проверьте правильность ввода</t>
   </si>
 </sst>
 </file>
@@ -25102,13 +25360,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L714"/>
+  <dimension ref="A1:L722"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B687" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D709" sqref="D709"/>
+      <selection pane="bottomRight" activeCell="K721" sqref="K721"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -34936,7 +35194,7 @@
         <v>1587</v>
       </c>
       <c r="D259" t="s">
-        <v>8239</v>
+        <v>8228</v>
       </c>
       <c r="E259" t="s">
         <v>2882</v>
@@ -36114,7 +36372,7 @@
         <v>7159</v>
       </c>
       <c r="D290" t="s">
-        <v>8236</v>
+        <v>8225</v>
       </c>
       <c r="E290" t="s">
         <v>7160</v>
@@ -36135,7 +36393,7 @@
         <v>7793</v>
       </c>
       <c r="K290" t="s">
-        <v>8235</v>
+        <v>8224</v>
       </c>
       <c r="L290" t="s">
         <v>7165</v>
@@ -42574,7 +42832,7 @@
         <v>1785</v>
       </c>
       <c r="D460" t="s">
-        <v>8237</v>
+        <v>8226</v>
       </c>
       <c r="E460" t="s">
         <v>3074</v>
@@ -42650,7 +42908,7 @@
         <v>1787</v>
       </c>
       <c r="D462" t="s">
-        <v>8238</v>
+        <v>8227</v>
       </c>
       <c r="E462" t="s">
         <v>3076</v>
@@ -43176,37 +43434,37 @@
         <v>473</v>
       </c>
       <c r="B476" t="s">
-        <v>8224</v>
+        <v>8213</v>
       </c>
       <c r="C476" t="s">
-        <v>8225</v>
+        <v>8214</v>
       </c>
       <c r="D476" t="s">
-        <v>8234</v>
+        <v>8223</v>
       </c>
       <c r="E476" t="s">
-        <v>8226</v>
+        <v>8215</v>
       </c>
       <c r="F476" t="s">
-        <v>8227</v>
+        <v>8216</v>
       </c>
       <c r="G476" t="s">
-        <v>8228</v>
+        <v>8217</v>
       </c>
       <c r="H476" t="s">
-        <v>8229</v>
+        <v>8218</v>
       </c>
       <c r="I476" t="s">
-        <v>8230</v>
+        <v>8219</v>
       </c>
       <c r="J476" t="s">
-        <v>8231</v>
+        <v>8220</v>
       </c>
       <c r="K476" t="s">
-        <v>8232</v>
+        <v>8221</v>
       </c>
       <c r="L476" t="s">
-        <v>8233</v>
+        <v>8222</v>
       </c>
     </row>
     <row r="477" spans="1:12" x14ac:dyDescent="0.25">
@@ -51314,7 +51572,7 @@
         <v>1998</v>
       </c>
       <c r="D690" t="s">
-        <v>8223</v>
+        <v>8212</v>
       </c>
       <c r="E690" t="s">
         <v>3286</v>
@@ -52036,7 +52294,7 @@
         <v>8174</v>
       </c>
       <c r="D709" t="s">
-        <v>8240</v>
+        <v>8229</v>
       </c>
       <c r="E709" t="s">
         <v>8162</v>
@@ -52106,37 +52364,37 @@
         <v>8175</v>
       </c>
       <c r="B711" t="s">
-        <v>8207</v>
+        <v>8200</v>
       </c>
       <c r="C711" t="s">
-        <v>8215</v>
+        <v>8206</v>
       </c>
       <c r="D711" t="s">
-        <v>8219</v>
+        <v>8209</v>
       </c>
       <c r="E711" t="s">
-        <v>8199</v>
+        <v>8194</v>
       </c>
       <c r="F711" t="s">
+        <v>8197</v>
+      </c>
+      <c r="G711" t="s">
+        <v>8191</v>
+      </c>
+      <c r="H711" t="s">
+        <v>8188</v>
+      </c>
+      <c r="I711" t="s">
+        <v>8182</v>
+      </c>
+      <c r="J711" t="s">
         <v>8203</v>
-      </c>
-      <c r="G711" t="s">
-        <v>8195</v>
-      </c>
-      <c r="H711" t="s">
-        <v>8191</v>
-      </c>
-      <c r="I711" t="s">
-        <v>8183</v>
-      </c>
-      <c r="J711" t="s">
-        <v>8211</v>
       </c>
       <c r="K711" t="s">
         <v>8179</v>
       </c>
       <c r="L711" t="s">
-        <v>8187</v>
+        <v>8185</v>
       </c>
     </row>
     <row r="712" spans="1:12" x14ac:dyDescent="0.25">
@@ -52144,37 +52402,37 @@
         <v>8176</v>
       </c>
       <c r="B712" t="s">
-        <v>8208</v>
+        <v>8256</v>
       </c>
       <c r="C712" t="s">
-        <v>8216</v>
+        <v>8257</v>
       </c>
       <c r="D712" t="s">
-        <v>8221</v>
+        <v>8253</v>
       </c>
       <c r="E712" t="s">
-        <v>8200</v>
+        <v>8255</v>
       </c>
       <c r="F712" t="s">
-        <v>8204</v>
+        <v>8258</v>
       </c>
       <c r="G712" t="s">
-        <v>8196</v>
+        <v>8259</v>
       </c>
       <c r="H712" t="s">
-        <v>8192</v>
+        <v>8260</v>
       </c>
       <c r="I712" t="s">
-        <v>8184</v>
+        <v>8261</v>
       </c>
       <c r="J712" t="s">
-        <v>8212</v>
+        <v>8262</v>
       </c>
       <c r="K712" t="s">
-        <v>8181</v>
+        <v>8263</v>
       </c>
       <c r="L712" t="s">
-        <v>8188</v>
+        <v>8264</v>
       </c>
     </row>
     <row r="713" spans="1:12" x14ac:dyDescent="0.25">
@@ -52182,37 +52440,37 @@
         <v>8177</v>
       </c>
       <c r="B713" t="s">
-        <v>8209</v>
+        <v>8201</v>
       </c>
       <c r="C713" t="s">
-        <v>8217</v>
+        <v>8207</v>
       </c>
       <c r="D713" t="s">
-        <v>8220</v>
+        <v>8210</v>
       </c>
       <c r="E713" t="s">
-        <v>8201</v>
+        <v>8195</v>
       </c>
       <c r="F713" t="s">
-        <v>8205</v>
+        <v>8198</v>
       </c>
       <c r="G713" t="s">
-        <v>8197</v>
+        <v>8192</v>
       </c>
       <c r="H713" t="s">
-        <v>8193</v>
+        <v>8189</v>
       </c>
       <c r="I713" t="s">
-        <v>8185</v>
+        <v>8183</v>
       </c>
       <c r="J713" t="s">
-        <v>8213</v>
+        <v>8204</v>
       </c>
       <c r="K713" t="s">
         <v>8180</v>
       </c>
       <c r="L713" t="s">
-        <v>8189</v>
+        <v>8186</v>
       </c>
     </row>
     <row r="714" spans="1:12" x14ac:dyDescent="0.25">
@@ -52220,37 +52478,341 @@
         <v>8178</v>
       </c>
       <c r="B714" t="s">
-        <v>8210</v>
+        <v>8202</v>
       </c>
       <c r="C714" t="s">
-        <v>8218</v>
+        <v>8208</v>
       </c>
       <c r="D714" t="s">
-        <v>8222</v>
+        <v>8211</v>
       </c>
       <c r="E714" t="s">
-        <v>8202</v>
+        <v>8196</v>
       </c>
       <c r="F714" t="s">
-        <v>8206</v>
+        <v>8199</v>
       </c>
       <c r="G714" t="s">
-        <v>8198</v>
+        <v>8193</v>
       </c>
       <c r="H714" t="s">
-        <v>8194</v>
+        <v>8190</v>
       </c>
       <c r="I714" t="s">
-        <v>8186</v>
+        <v>8184</v>
       </c>
       <c r="J714" t="s">
-        <v>8214</v>
+        <v>8205</v>
       </c>
       <c r="K714" t="s">
-        <v>8182</v>
+        <v>8181</v>
       </c>
       <c r="L714" t="s">
-        <v>8190</v>
+        <v>8187</v>
+      </c>
+    </row>
+    <row r="715" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A715" t="s">
+        <v>8230</v>
+      </c>
+      <c r="B715" t="s">
+        <v>8247</v>
+      </c>
+      <c r="C715" t="s">
+        <v>8251</v>
+      </c>
+      <c r="D715" t="s">
+        <v>8232</v>
+      </c>
+      <c r="E715" t="s">
+        <v>8233</v>
+      </c>
+      <c r="F715" t="s">
+        <v>8235</v>
+      </c>
+      <c r="G715" t="s">
+        <v>8237</v>
+      </c>
+      <c r="H715" t="s">
+        <v>8241</v>
+      </c>
+      <c r="I715" t="s">
+        <v>8239</v>
+      </c>
+      <c r="J715" t="s">
+        <v>8243</v>
+      </c>
+      <c r="K715" t="s">
+        <v>8249</v>
+      </c>
+      <c r="L715" t="s">
+        <v>8245</v>
+      </c>
+    </row>
+    <row r="716" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A716" t="s">
+        <v>8231</v>
+      </c>
+      <c r="B716" t="s">
+        <v>8248</v>
+      </c>
+      <c r="C716" t="s">
+        <v>8252</v>
+      </c>
+      <c r="D716" t="s">
+        <v>8254</v>
+      </c>
+      <c r="E716" t="s">
+        <v>8234</v>
+      </c>
+      <c r="F716" t="s">
+        <v>8236</v>
+      </c>
+      <c r="G716" t="s">
+        <v>8238</v>
+      </c>
+      <c r="H716" t="s">
+        <v>8242</v>
+      </c>
+      <c r="I716" t="s">
+        <v>8240</v>
+      </c>
+      <c r="J716" t="s">
+        <v>8244</v>
+      </c>
+      <c r="K716" t="s">
+        <v>8250</v>
+      </c>
+      <c r="L716" t="s">
+        <v>8246</v>
+      </c>
+    </row>
+    <row r="717" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A717" t="s">
+        <v>8265</v>
+      </c>
+      <c r="B717" t="s">
+        <v>8297</v>
+      </c>
+      <c r="C717" t="s">
+        <v>8283</v>
+      </c>
+      <c r="D717" t="s">
+        <v>8272</v>
+      </c>
+      <c r="E717" t="s">
+        <v>8302</v>
+      </c>
+      <c r="F717" t="s">
+        <v>8307</v>
+      </c>
+      <c r="G717" t="s">
+        <v>8312</v>
+      </c>
+      <c r="H717" t="s">
+        <v>8317</v>
+      </c>
+      <c r="I717" t="s">
+        <v>8288</v>
+      </c>
+      <c r="J717" t="s">
+        <v>8322</v>
+      </c>
+      <c r="K717" t="s">
+        <v>8276</v>
+      </c>
+      <c r="L717" t="s">
+        <v>8292</v>
+      </c>
+    </row>
+    <row r="718" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A718" t="s">
+        <v>8266</v>
+      </c>
+      <c r="B718" t="s">
+        <v>8271</v>
+      </c>
+      <c r="C718" t="s">
+        <v>8271</v>
+      </c>
+      <c r="D718" t="s">
+        <v>8271</v>
+      </c>
+      <c r="E718" t="s">
+        <v>8271</v>
+      </c>
+      <c r="F718" t="s">
+        <v>8271</v>
+      </c>
+      <c r="G718" t="s">
+        <v>8271</v>
+      </c>
+      <c r="H718" t="s">
+        <v>8271</v>
+      </c>
+      <c r="I718" t="s">
+        <v>8271</v>
+      </c>
+      <c r="J718" t="s">
+        <v>8271</v>
+      </c>
+      <c r="K718" t="s">
+        <v>8271</v>
+      </c>
+      <c r="L718" t="s">
+        <v>8271</v>
+      </c>
+    </row>
+    <row r="719" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A719" t="s">
+        <v>8267</v>
+      </c>
+      <c r="B719" t="s">
+        <v>8298</v>
+      </c>
+      <c r="C719" t="s">
+        <v>8284</v>
+      </c>
+      <c r="D719" t="s">
+        <v>8275</v>
+      </c>
+      <c r="E719" t="s">
+        <v>8303</v>
+      </c>
+      <c r="F719" t="s">
+        <v>8308</v>
+      </c>
+      <c r="G719" t="s">
+        <v>8313</v>
+      </c>
+      <c r="H719" t="s">
+        <v>8318</v>
+      </c>
+      <c r="I719" t="s">
+        <v>8282</v>
+      </c>
+      <c r="J719" t="s">
+        <v>8323</v>
+      </c>
+      <c r="K719" t="s">
+        <v>8281</v>
+      </c>
+      <c r="L719" t="s">
+        <v>8293</v>
+      </c>
+    </row>
+    <row r="720" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A720" t="s">
+        <v>8268</v>
+      </c>
+      <c r="B720" t="s">
+        <v>8299</v>
+      </c>
+      <c r="C720" t="s">
+        <v>8285</v>
+      </c>
+      <c r="D720" t="s">
+        <v>8279</v>
+      </c>
+      <c r="E720" t="s">
+        <v>8304</v>
+      </c>
+      <c r="F720" t="s">
+        <v>8309</v>
+      </c>
+      <c r="G720" t="s">
+        <v>8314</v>
+      </c>
+      <c r="H720" t="s">
+        <v>8319</v>
+      </c>
+      <c r="I720" t="s">
+        <v>8289</v>
+      </c>
+      <c r="J720" t="s">
+        <v>8324</v>
+      </c>
+      <c r="K720" t="s">
+        <v>8280</v>
+      </c>
+      <c r="L720" t="s">
+        <v>8294</v>
+      </c>
+    </row>
+    <row r="721" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A721" t="s">
+        <v>8269</v>
+      </c>
+      <c r="B721" t="s">
+        <v>8300</v>
+      </c>
+      <c r="C721" t="s">
+        <v>8286</v>
+      </c>
+      <c r="D721" t="s">
+        <v>8273</v>
+      </c>
+      <c r="E721" t="s">
+        <v>8305</v>
+      </c>
+      <c r="F721" t="s">
+        <v>8310</v>
+      </c>
+      <c r="G721" t="s">
+        <v>8315</v>
+      </c>
+      <c r="H721" t="s">
+        <v>8320</v>
+      </c>
+      <c r="I721" t="s">
+        <v>8290</v>
+      </c>
+      <c r="J721" t="s">
+        <v>8325</v>
+      </c>
+      <c r="K721" t="s">
+        <v>8277</v>
+      </c>
+      <c r="L721" t="s">
+        <v>8295</v>
+      </c>
+    </row>
+    <row r="722" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A722" t="s">
+        <v>8270</v>
+      </c>
+      <c r="B722" t="s">
+        <v>8301</v>
+      </c>
+      <c r="C722" t="s">
+        <v>8287</v>
+      </c>
+      <c r="D722" t="s">
+        <v>8274</v>
+      </c>
+      <c r="E722" t="s">
+        <v>8306</v>
+      </c>
+      <c r="F722" t="s">
+        <v>8311</v>
+      </c>
+      <c r="G722" t="s">
+        <v>8316</v>
+      </c>
+      <c r="H722" t="s">
+        <v>8321</v>
+      </c>
+      <c r="I722" t="s">
+        <v>8291</v>
+      </c>
+      <c r="J722" t="s">
+        <v>8326</v>
+      </c>
+      <c r="K722" t="s">
+        <v>8278</v>
+      </c>
+      <c r="L722" t="s">
+        <v>8296</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates for Slideshow version 4.4.4
</commit_message>
<xml_diff>
--- a/backend/localization.xlsx
+++ b/backend/localization.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mimac\Documents\NetBeansProjects\slideshow-localization\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0C1E1B0-F89F-47B5-9015-455500D12A5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B41DCCB-2D59-4D50-A106-B6B04CECBE7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-114" yWindow="-114" windowWidth="49274" windowHeight="20160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38539,7 +38539,7 @@
     <t>&lt;p&gt;슬라이드쇼 앱이 최신 버전으로 성공적으로 업데이트되었습니다.&lt;/p&gt;&lt;p&gt;기능에 대한 설명서는 다음 주소에서 찾을 수 있습니다. &lt;a href="https://slideshow.digital/documentation/" target="_blank"&gt;https://slideshow.digital/documentation/&lt;/a&gt;. 튜터리얼은 다음 주소에서 찾을 수 있습니다.&lt;a href="https://www.youtube.com/channel/UCJFSXCItojY4PS76JNr_pdQ" target="_blank"&gt;https://www.youtube.com/channel/UCJFSXCItojY4PS76JNr_pdQ&lt;/a&gt;.&lt;/p&gt;&lt;p&gt;슬라이드쇼 앱이 마음에 들면 다음에서 앱을 평가하여 개발을 지원할 수 있습니다. &lt;a href="https://play.google.com/store/apps/details?id=sk.mimac.slideshow" target="_blank"&gt;Google Play&lt;/a&gt;. 구매를 원하시면 다음 주소로 연락주세요.&lt;a href="https://ko-fi.com/slideshow" target="_blank"&gt;coffee&lt;/a&gt;.&lt;/p&gt;&lt;span style='float:right'&gt;-- 개발팀 --&lt;/span&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;Slideshow app has been successfully updated to a newer version. There are following changes in this version:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Added Korean localization&lt;/li&gt;&lt;li&gt;Added support for file synchronization from SFTP server (see menu Tools - File synchronization)&lt;/li&gt;&lt;li&gt;Enhanced support for synchronized playback across multiple zones or multiple devices&lt;/li&gt;&lt;li&gt;Added trigger in case there is no user activity (see menu Settings - Triggers - Conditions - Seconds since last user activity)&lt;/li&gt;&lt;li&gt;Added possibility to restrict access to other websites when displaying a URL file&lt;/li&gt;&lt;li&gt;Added possibility to select particular external storage for saving media (see menu Settings - Device settings - Storage for media) &lt;/li&gt;&lt;li&gt;Enhanced visibility of on-screen controls (swipe from the right on the screen)&lt;/li&gt;&lt;li&gt;Removed support for importing time slots from XML configuration created on Slideshow 3.x (use new format introduced in Slideshow 4.0)&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;You can find documentation for features on &lt;a href="https://slideshow.digital/documentation/" target="_blank"&gt;https://slideshow.digital/documentation/&lt;/a&gt;  and watch tutorials on  &lt;a href="https://www.youtube.com/channel/UCJFSXCItojY4PS76JNr_pdQ" target="_blank"&gt;https://www.youtube.com/channel/UCJFSXCItojY4PS76JNr_pdQ&lt;/a&gt;.&lt;/p&gt;&lt;p&gt;If you like Slideshow app, you can support the development by rating the app on &lt;a href="https://play.google.com/store/apps/details?id=sk.mimac.slideshow" target="_blank"&gt;Google Play&lt;/a&gt; or buy us a &lt;a href="https://ko-fi.com/slideshow" target="_blank"&gt;coffee&lt;/a&gt;.&lt;/p&gt;&lt;span style='float:right'&gt;-- The Development team --&lt;/span&gt;</t>
+    <t>&lt;p&gt;Slideshow app has been successfully updated to a newer version. There are following changes in this version:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Added new synchronization commands to other devices (see menu Settings - Other devices)&lt;/li&gt;&lt;li&gt;Fixed displaying PDF if the preloading is turned off&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;You can find documentation for features on &lt;a href="https://slideshow.digital/documentation/" target="_blank"&gt;https://slideshow.digital/documentation/&lt;/a&gt;  and watch tutorials on  &lt;a href="https://www.youtube.com/channel/UCJFSXCItojY4PS76JNr_pdQ" target="_blank"&gt;https://www.youtube.com/channel/UCJFSXCItojY4PS76JNr_pdQ&lt;/a&gt;.&lt;/p&gt;&lt;p&gt;If you like Slideshow app, you can support the development by rating the app on &lt;a href="https://play.google.com/store/apps/details?id=sk.mimac.slideshow" target="_blank"&gt;Google Play&lt;/a&gt; or buy us a &lt;a href="https://ko-fi.com/slideshow" target="_blank"&gt;coffee&lt;/a&gt;.&lt;/p&gt;&lt;span style='float:right'&gt;-- The Development team --&lt;/span&gt;</t>
   </si>
 </sst>
 </file>
@@ -38944,10 +38944,10 @@
   <dimension ref="A1:P834"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B649" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B652" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I657" sqref="I657"/>
+      <selection pane="bottomRight" activeCell="D675" sqref="D675"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3"/>

</xml_diff>

<commit_message>
Updates for Slideshow version 4.8.1
</commit_message>
<xml_diff>
--- a/backend/localization.xlsx
+++ b/backend/localization.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mimac\Documents\NetBeansProjects\slideshow-localization\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0136146-5EE9-4928-AF3A-C7304162460E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D69FEF8D-4B6B-4FC4-971B-88611E669C21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24523" windowHeight="19932" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-114" yWindow="-114" windowWidth="49274" windowHeight="20160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="properties" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14144" uniqueCount="13605">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14480" uniqueCount="13926">
   <si>
     <t>keys</t>
   </si>
@@ -40831,10 +40831,973 @@
     <t>Flash sürücüdeki dosyalar bu uygulamadaki hangi klasöre kopyalanır. Eğik çizgi kök klasör anlamına gelir. Bu yalnızca Flash sürücüden kopyalamaya izin veriliyorsa kullanılır (bkz. Flash sürücü takılırken Eylem ayarı).</t>
   </si>
   <si>
-    <t>&lt;p&gt;Slideshow app has been successfully updated to a newer version. There are following changes in this version:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Added settings internal screensaver layout (see menu Screen layout - Screensaver)&lt;/li&gt;&lt;li&gt;Added Click areas for images (see menu File manager - right click an image - Click areas)&lt;/li&gt;&lt;li&gt;Added new setting Grant web pages permissions (see menu Settings - Device settings)&lt;/li&gt;&lt;li&gt;Added new setting Target folder from Flash drive (see menu Settings - Device settings)&lt;/li&gt;&lt;li&gt;Fixed app update on Android 7&lt;/li&gt;&lt;li&gt;Small fixes &amp; enhancements&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;You can find documentation for features on &lt;a href="https://slideshow.digital/documentation/" target="_blank"&gt;https://slideshow.digital/documentation/&lt;/a&gt;  and watch tutorials on  &lt;a href="https://www.youtube.com/channel/UCJFSXCItojY4PS76JNr_pdQ" target="_blank"&gt;https://www.youtube.com/channel/UCJFSXCItojY4PS76JNr_pdQ&lt;/a&gt;.&lt;/p&gt;&lt;p&gt;If you like Slideshow app, you can support the development by rating the app on &lt;a href="https://play.google.com/store/apps/details?id=sk.mimac.slideshow" target="_blank"&gt;Google Play&lt;/a&gt; or buy us a &lt;a href="https://ko-fi.com/slideshow" target="_blank"&gt;coffee&lt;/a&gt;.&lt;/p&gt;&lt;span style='float:right'&gt;-- The Development team --&lt;/span&gt;</t>
-  </si>
-  <si>
     <t>Clear folder (delete old files)</t>
+  </si>
+  <si>
+    <t>face_detection_preferred_image_width</t>
+  </si>
+  <si>
+    <t>face_detection_preferred_image_width_help</t>
+  </si>
+  <si>
+    <t>face_detection_min_face_size</t>
+  </si>
+  <si>
+    <t>face_detection_min_face_size_help</t>
+  </si>
+  <si>
+    <t>face_detection_min_eyes_opened</t>
+  </si>
+  <si>
+    <t>face_detection_min_eyes_opened_help</t>
+  </si>
+  <si>
+    <t>Preferred camera image width</t>
+  </si>
+  <si>
+    <t>Minimal width of a face (in %)</t>
+  </si>
+  <si>
+    <t>Minimal width of a face in percentage of the total image width, in order for the face to be counted.&lt;br&gt;&lt;i&gt;Reload is required for applying this change.&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>Minimal number of opened eyes</t>
+  </si>
+  <si>
+    <t>Minimálna šírka tváre v percentách z celkovej šírky snímky, aby bola tvár započítaná.&lt;br&gt;&lt;i&gt;Reštart aplikácie je vyžadovaný pre aplikovanie tohto nastavenia.&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>Preferovaná šírka snímky z kamery. Ak kamera nepodporuje danú šírku, použije sa najbližšia väčšia šírka.&lt;br&gt;&lt;i&gt;Reštart aplikácie je vyžadovaný pre aplikovanie tohto nastavenia.&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>Minimálna šírka tváre (v %)</t>
+  </si>
+  <si>
+    <t>Minimálna pravdepodobnosť otvorených očí, aby bola tvár započítaná. Zadajte desatinné číslo medzi 0 a 2.&lt;br&gt;&lt;i&gt;Reštart aplikácie je vyžadovaný pre aplikovanie tohto nastavenia.&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>Minimal probability of opened eyes, in order for the face to be counted. Enter a decimal number between 0 and 2.&lt;br&gt;&lt;i&gt;Reload is required for applying this change.&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>Bevorzugte Bildbreite der Kamera</t>
+  </si>
+  <si>
+    <t>Bevorzugte Breite des von der Kamera aufgenommenen Bildes. Wenn die Kamera diese bestimmte Breite nicht unterstützt, wird die nächstgrößere Breite verwendet.&lt;br&gt;&lt;i&gt;Um diese Änderung anzuwenden, ist ein Neuladen erforderlich.&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>Minimale Breite einer Fläche (in %)</t>
+  </si>
+  <si>
+    <t>Minimale Breite eines Gesichts in Prozent der gesamten Bildbreite, damit das Gesicht gezählt werden kann.&lt;br&gt;&lt;i&gt;Zum Anwenden dieser Änderung ist ein Neuladen erforderlich.&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>Minimale Anzahl geöffneter Augen</t>
+  </si>
+  <si>
+    <t>Minimale Wahrscheinlichkeit geöffneter Augen, damit das Gesicht gezählt werden kann. Geben Sie eine Dezimalzahl zwischen 0 und 2 ein.&lt;br&gt;&lt;i&gt;Zum Anwenden dieser Änderung ist ein Neuladen erforderlich.&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>Largeur d'image de caméra préférée</t>
+  </si>
+  <si>
+    <t>Largeur préférée de l’image prise par la caméra. Si la caméra ne prend pas en charge cette largeur particulière, la largeur la plus grande la plus proche sera utilisée.&lt;br&gt;&lt;i&gt;Un rechargement est nécessaire pour appliquer cette modification.&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>Largeur minimale d'un visage (en %)</t>
+  </si>
+  <si>
+    <t>Largeur minimale d'un visage en pourcentage de la largeur totale de l'image, pour que le visage soit compté.&lt;br&gt;&lt;i&gt;Un rechargement est nécessaire pour appliquer cette modification.&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>Nombre minimal d'yeux ouverts</t>
+  </si>
+  <si>
+    <t>Probabilité minimale d'ouvrir les yeux pour que le visage soit compté. Saisissez un nombre décimal compris entre 0 et 2.&lt;br&gt;&lt;i&gt;Un rechargement est requis pour appliquer cette modification.&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>Željena širina slike kamere</t>
+  </si>
+  <si>
+    <t>Preferirana širina slike snimljene kamerom. Ako kamera ne podržava ovu konkretnu širinu, koristit će se najbliža veća širina.&lt;br&gt;&lt;i&gt;Potrebno je ponovno učitavanje za primjenu ove promjene.&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>Minimalna širina lica (u %)</t>
+  </si>
+  <si>
+    <t>Minimalna širina lica u postotku ukupne širine slike, kako bi se lice moglo računati.&lt;br&gt;&lt;i&gt;Potrebno je ponovno učitavanje za primjenu ove promjene.&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>Minimalan broj otvorenih očiju</t>
+  </si>
+  <si>
+    <t>Minimalna vjerojatnost otvorenih očiju, kako bi se lice moglo prebrojati. Unesite decimalni broj između 0 i 2.&lt;br&gt;&lt;i&gt;Potrebno je ponovno učitavanje za primjenu ove promjene.&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>Larghezza preferita dell'immagine della telecamera</t>
+  </si>
+  <si>
+    <t>Larghezza preferita dell'immagine scattata dalla fotocamera. Se la fotocamera non supporta questa larghezza particolare, verrà utilizzata la larghezza maggiore più vicina.&lt;br&gt;&lt;i&gt;È necessario ricaricare per applicare questa modifica.&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>Larghezza minima di una faccia (in %)</t>
+  </si>
+  <si>
+    <t>Larghezza minima di un volto in percentuale della larghezza totale dell'immagine, affinché il volto possa essere conteggiato.&lt;br&gt;&lt;i&gt;È necessario ricaricare per applicare questa modifica.&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>Numero minimo di occhi aperti</t>
+  </si>
+  <si>
+    <t>Probabilità minima di occhi aperti per poter contare il volto. Inserisci un numero decimale compreso tra 0 e 2.&lt;br&gt;&lt;i&gt;Per applicare questa modifica è necessario ricaricare.&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>推奨されるカメラ画像の幅</t>
+  </si>
+  <si>
+    <t>カメラで撮影した画像の推奨幅。 カメラがこの特定の幅をサポートしていない場合は、最も近い大きい幅が使用されます。&lt;br&gt;&lt;i&gt;この変更を適用するには再読み込みが必要です。&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>顔の最小幅 (%)</t>
+  </si>
+  <si>
+    <t>顔がカウントされるために、画像全体の幅に対するパーセンテージで表した顔の最小幅。&lt;br&gt;&lt;i&gt;この変更を適用するには再読み込みが必要です。&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>開いた目の最小数</t>
+  </si>
+  <si>
+    <t>顔がカウントされるために、目が開いている可能性は最小限です。 0 ～ 2 の 10 進数を入力してください。&lt;br&gt;&lt;i&gt;この変更を適用するには再読み込みが必要です。&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>기본 카메라 이미지 너비</t>
+  </si>
+  <si>
+    <t>카메라로 촬영한 이미지의 기본 너비입니다. 카메라가 이 특정 너비를 지원하지 않는 경우 가장 가까운 더 큰 너비가 사용됩니다.&lt;br&gt;&lt;i&gt;이 변경 사항을 적용하려면 새로고침이 필요합니다.&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>면의 최소 너비(%)</t>
+  </si>
+  <si>
+    <t>얼굴을 계산하기 위한 얼굴의 최소 너비(전체 이미지 너비에 대한 백분율).&lt;br&gt;&lt;i&gt;이 변경 사항을 적용하려면 새로고침이 필요합니다.&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>최소한의 눈을 뜨고</t>
+  </si>
+  <si>
+    <t>얼굴이 계산되기 위해서는 눈을 뜰 확률이 최소화됩니다. 0에서 2 사이의 10진수를 입력하세요.&lt;br&gt;&lt;i&gt;이 변경사항을 적용하려면 새로고침이 필요합니다.&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>Preferowana szerokość obrazu z kamery</t>
+  </si>
+  <si>
+    <t>Preferowana szerokość obrazu rejestrowanego przez kamerę. Jeśli kamera nie obsługuje tej konkretnej szerokości, zostanie użyta najbliższa większa szerokość.&lt;br&gt;&lt;i&gt;Aby zastosować tę zmianę, wymagane jest ponowne załadowanie.&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>Minimalna szerokość twarzy (w %)</t>
+  </si>
+  <si>
+    <t>Minimalna szerokość twarzy jako procent całkowitej szerokości obrazu, aby twarz została policzona.&lt;br&gt;&lt;i&gt;Aby zastosować tę zmianę, wymagane jest ponowne załadowanie.&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>Minimalna liczba otwartych oczu</t>
+  </si>
+  <si>
+    <t>Minimalne prawdopodobieństwo otwarcia oczu, aby można było policzyć twarz. Wprowadź liczbę dziesiętną z zakresu od 0 do 2.&lt;br&gt;&lt;i&gt;Aby zastosować tę zmianę, wymagane jest ponowne załadowanie.&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>Largura preferida da imagem da câmera</t>
+  </si>
+  <si>
+    <t>Largura preferida da imagem tirada pela câmera. Se a câmera não suportar essa largura específica, a largura maior mais próxima será usada.&lt;br&gt;&lt;i&gt;É necessário recarregar para aplicar esta alteração.&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>Largura mínima de uma face (em%)</t>
+  </si>
+  <si>
+    <t>Largura mínima de um rosto em porcentagem da largura total da imagem, para que o rosto seja contado.&lt;br&gt;&lt;i&gt;É necessário recarregar para aplicar esta alteração.&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>Número mínimo de olhos abertos</t>
+  </si>
+  <si>
+    <t>Probabilidade mínima de olhos abertos, para que o rosto seja contado. Insira um número decimal entre 0 e 2.&lt;br&gt;&lt;i&gt;É necessário recarregar para aplicar esta alteração.&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>Предпочтительная ширина изображения камеры</t>
+  </si>
+  <si>
+    <t>Предпочтительная ширина изображения, снятого камерой. Если камера не поддерживает эту конкретную ширину, будет использоваться ближайшая к ней большая ширина.&lt;br&gt;&lt;i&gt;Для применения этого изменения потребуется перезагрузка.&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>Минимальная ширина грани (в %)</t>
+  </si>
+  <si>
+    <t>Минимальная ширина лица в процентах от общей ширины изображения, необходимая для подсчета лица.&lt;br&gt;&lt;i&gt;Для применения этого изменения требуется перезагрузка.&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>Минимальное количество открытых глаз</t>
+  </si>
+  <si>
+    <t>Минимальная вероятность открытия глаз, чтобы лицо можно было засчитать. Введите десятичное число от 0 до 2.&lt;br&gt;&lt;i&gt;Для применения этого изменения потребуется перезагрузка.&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>Želena širina slike kamere</t>
+  </si>
+  <si>
+    <t>Želena širina slike, posnete s kamero. Če kamera ne podpira te določene širine, bo uporabljena najbližja večja širina.&lt;br&gt;&lt;i&gt;Za uveljavitev te spremembe je potrebno ponovno nalaganje.&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>Najmanjša širina obraza (v %)</t>
+  </si>
+  <si>
+    <t>Najmanjša širina obraza v odstotkih skupne širine slike, da se lahko obraz šteje.&lt;br&gt;&lt;i&gt;Za uveljavitev te spremembe je potrebno ponovno nalaganje.&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>Najmanjše število odprtih oči</t>
+  </si>
+  <si>
+    <t>Minimalna verjetnost odprtih oči, da bi lahko prešteli obraz. Vnesite decimalno število med 0 in 2.&lt;br&gt;&lt;i&gt;Za uveljavitev te spremembe je potrebno ponovno nalaganje.&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>Ancho de imagen de cámara preferido</t>
+  </si>
+  <si>
+    <t>Ancho preferido de la imagen tomada por la cámara. Si la cámara no admite este ancho en particular, se utilizará el ancho mayor más cercano.&lt;br&gt;&lt;i&gt;Es necesario volver a cargar para aplicar este cambio.&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>Ancho mínimo de una cara (en %)</t>
+  </si>
+  <si>
+    <t>Ancho mínimo de una cara en porcentaje del ancho total de la imagen, para que la cara se cuente.&lt;br&gt;&lt;i&gt;Es necesario volver a cargar para aplicar este cambio.&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>Número mínimo de ojos abiertos.</t>
+  </si>
+  <si>
+    <t>Probabilidad mínima de ojos abiertos, para que se cuente la cara. Introduce un número decimal entre 0 y 2.&lt;br&gt;&lt;i&gt;Es necesario volver a cargar para aplicar este cambio.&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>Tercih edilen kamera görüntü genişliği</t>
+  </si>
+  <si>
+    <t>Kamera tarafından çekilen görüntünün tercih edilen genişliği. Kamera bu belirli genişliği desteklemiyorsa en yakın geniş genişlik kullanılacaktır.&lt;br&gt;&lt;i&gt;Bu değişikliğin uygulanması için yeniden yükleme gerekiyor.&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>Yüzün minimum genişliği (% olarak)</t>
+  </si>
+  <si>
+    <t>Yüzün sayılabilmesi için toplam resim genişliğinin yüzdesi olarak minimum yüz genişliği.&lt;br&gt;&lt;i&gt;Bu değişikliğin uygulanması için yeniden yükleme gerekir.&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>Minimum sayıda açık göz</t>
+  </si>
+  <si>
+    <t>Yüzün sayılabilmesi için minimum açık göz olasılığı. 0 ile 2 arasında bir ondalık sayı girin.&lt;br&gt;&lt;i&gt;Bu değişikliğin uygulanması için yeniden yükleme gerekiyor.&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>Minimálny počet otvorených očí</t>
+  </si>
+  <si>
+    <t>Preferovaná šírka snímky z kamery</t>
+  </si>
+  <si>
+    <t>Preferovaná šířka snímku z kamery</t>
+  </si>
+  <si>
+    <t>Preferovaná šířka snímku z kamery. Pokud kamera nepodporuje danou šířku, použije se nejbližší větší šířka.&lt;br&gt;&lt;i&gt;Restart aplikace je vyžadován pro aplikování tohoto nastavení.&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>Minimální šířka obličeje (v %)</t>
+  </si>
+  <si>
+    <t>Minimální šířka obličeje v procentech z celkové šířky snímku, aby byla tvář započtena.&lt;br&gt;&lt;i&gt;Restart aplikace je vyžadován pro aplikování tohoto nastavení.&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>Minimální počet otevřených očí</t>
+  </si>
+  <si>
+    <t>Minimální pravděpodobnost otevřených očí, aby byla tvář započtena. Zadejte desetinné číslo mezi 0 a 2.&lt;br&gt;&lt;i&gt;Restart aplikace je vyžadován pro aplikování tohoto nastavení.&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>Preferred width of the image taken by camera. If the camera doesn't support this particular width, the closest larger width will be used. If no value is entered, the maximum available picture size will be chosen.&lt;br&gt;&lt;i&gt;Reload is required for applying this change.&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>watchdog_ping_address</t>
+  </si>
+  <si>
+    <t>watchdog_ping_address_help</t>
+  </si>
+  <si>
+    <t>watchdog_ping_delay_help</t>
+  </si>
+  <si>
+    <t>watchdog_ping_delay</t>
+  </si>
+  <si>
+    <t>watchdog_ping_times</t>
+  </si>
+  <si>
+    <t>watchdog_ping_times_help</t>
+  </si>
+  <si>
+    <t>IP address or hostname of a network device that should be pinged for watchdog. If no address is entered, the network watchdog is turned off.</t>
+  </si>
+  <si>
+    <t>Delay in seconds between consecutive pings.&lt;br&gt;&lt;i&gt;Reload is required for applying this change.&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>Number of consecutive failed pings, after which this  device is rebooted. Works only on rooted devices.</t>
+  </si>
+  <si>
+    <t>Delay between pings (in s)</t>
+  </si>
+  <si>
+    <t>No. of failes pings for reboot</t>
+  </si>
+  <si>
+    <t>IP address for pings</t>
+  </si>
+  <si>
+    <t>IP adresa na ping</t>
+  </si>
+  <si>
+    <t>Počet neúspešných pingov na reštart</t>
+  </si>
+  <si>
+    <t>Počet za sebou idúcich neúspešných pingov, po ktorých sa toto zariadenie reštartuje. Funguje len na rootnutých zariadeniach.</t>
+  </si>
+  <si>
+    <t>IP adresa alebo doménové meno sieťového zariadenia, ktoré bude ping-ované pre watchdog. Ak nie je zadaná žiadna adresa, sieťový watchdog je vypnutý.</t>
+  </si>
+  <si>
+    <t>Oneskorenie medzi pingami (v s)</t>
+  </si>
+  <si>
+    <t>Oneskorenie v sekundách medzi jednotlivými pingami.&lt;br&gt;&lt;i&gt;Reštart aplikácie je vyžadovaný pre aplikovanie tohto nastavenia.&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>핑을 위한 IP 주소</t>
+  </si>
+  <si>
+    <t>감시를 위해 핑을 보내야 하는 네트워크 장치의 IP 주소 또는 호스트 이름입니다. 주소를 입력하지 않으면 네트워크 감시가 꺼집니다.</t>
+  </si>
+  <si>
+    <t>핑 간 지연(초)</t>
+  </si>
+  <si>
+    <t>연속 핑 사이의 지연 시간(초)입니다.&lt;br&gt;&lt;i&gt;이 변경 사항을 적용하려면 새로고침이 필요합니다.&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>재부팅에 대한 핑 실패 횟수</t>
+  </si>
+  <si>
+    <t>이 장치가 재부팅된 후 연속적으로 실패한 ping 횟수입니다. 루팅된 장치에서만 작동합니다.</t>
+  </si>
+  <si>
+    <t>ping 用の IP アドレス</t>
+  </si>
+  <si>
+    <t>ウォッチドッグのために ping を送信する必要があるネットワーク デバイスの IP アドレスまたはホスト名。 アドレスが入力されない場合、ネットワーク ウォッチドッグはオフになります。</t>
+  </si>
+  <si>
+    <t>ping 間の遅延 (秒単位)</t>
+  </si>
+  <si>
+    <t>連続する ping 間の遅延 (秒単位)。&lt;br&gt;&lt;i&gt;この変更を適用するにはリロードが必要です。&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>再起動の失敗した ping の数</t>
+  </si>
+  <si>
+    <t>このデバイスが再起動されるまでに連続して失敗した ping の数。 root化されたデバイスでのみ動作します。</t>
+  </si>
+  <si>
+    <t>Indirizzo IP per i ping</t>
+  </si>
+  <si>
+    <t>Indirizzo IP o nome host di un dispositivo di rete di cui eseguire il ping per il watchdog. Se non viene inserito alcun indirizzo, il watchdog di rete viene disattivato.</t>
+  </si>
+  <si>
+    <t>Ritardo tra i ping (in s)</t>
+  </si>
+  <si>
+    <t>Ritardo in secondi tra ping consecutivi.&lt;br&gt;&lt;i&gt;Per applicare questa modifica è necessario ricaricare.&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>N. di ping non riusciti per il riavvio</t>
+  </si>
+  <si>
+    <t>Numero di ping consecutivi non riusciti, dopo i quali il dispositivo viene riavviato. Funziona solo su dispositivi rooted.</t>
+  </si>
+  <si>
+    <t>IP-Adresse für Pings</t>
+  </si>
+  <si>
+    <t>IP-Adresse oder Hostname eines Netzwerkgeräts, das als Watchdog angepingt werden soll. Wenn keine Adresse eingegeben wird, ist der Netzwerk-Watchdog ausgeschaltet.</t>
+  </si>
+  <si>
+    <t>Verzögerung zwischen Pings (in s)</t>
+  </si>
+  <si>
+    <t>Verzögerung in Sekunden zwischen aufeinanderfolgenden Pings.&lt;br&gt;&lt;i&gt;Zum Anwenden dieser Änderung ist ein Neuladen erforderlich.&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>Anzahl der fehlgeschlagenen Pings für den Neustart</t>
+  </si>
+  <si>
+    <t>Anzahl aufeinanderfolgender fehlgeschlagener Pings, nach denen dieses Gerät neu gestartet wird. Funktioniert nur auf gerooteten Geräten.</t>
+  </si>
+  <si>
+    <t>Adresse IP pour les pings</t>
+  </si>
+  <si>
+    <t>Adresse IP ou nom d'hôte d'un périphérique réseau qui doit faire l'objet d'une requête ping pour le chien de garde. Si aucune adresse n'est saisie, le chien de garde du réseau est désactivé.</t>
+  </si>
+  <si>
+    <t>Délai entre les pings (en s)</t>
+  </si>
+  <si>
+    <t>Délai en secondes entre les pings consécutifs.&lt;br&gt;&lt;i&gt;Un rechargement est requis pour appliquer cette modification.&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>Nombre d'échecs de ping pour le redémarrage</t>
+  </si>
+  <si>
+    <t>Nombre d'échecs ping consécutifs, après quoi cet appareil est redémarré. Fonctionne uniquement sur les appareils rootés.</t>
+  </si>
+  <si>
+    <t>Adres IP dla pingów</t>
+  </si>
+  <si>
+    <t>Adres IP lub nazwa hosta urządzenia sieciowego, które powinno zostać pingowane dla watchdoga. Jeśli nie zostanie wprowadzony żaden adres, funkcja nadzoru sieci zostanie wyłączona.</t>
+  </si>
+  <si>
+    <t>Opóźnienie między pingami (w s)</t>
+  </si>
+  <si>
+    <t>Opóźnienie w sekundach pomiędzy kolejnymi sygnałami.&lt;br&gt;&lt;i&gt;Aby zastosować tę zmianę, wymagane jest ponowne załadowanie.&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>Liczba nieudanych pingów potrzebnych do ponownego uruchomienia</t>
+  </si>
+  <si>
+    <t>Liczba kolejnych nieudanych pingów, po których urządzenie zostanie ponownie uruchomione. Działa tylko na urządzeniach zrootowanych.</t>
+  </si>
+  <si>
+    <t>Endereço IP para pings</t>
+  </si>
+  <si>
+    <t>Endereço IP ou nome de host de um dispositivo de rede que deve receber ping para watchdog. Se nenhum endereço for inserido, o watchdog da rede será desativado.</t>
+  </si>
+  <si>
+    <t>Atraso entre pings (em s)</t>
+  </si>
+  <si>
+    <t>Atraso em segundos entre pings consecutivos.&lt;br&gt;&lt;i&gt;É necessário recarregar para aplicar esta alteração.&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>Nº de falhas em pings para reinicialização</t>
+  </si>
+  <si>
+    <t>Número de pings consecutivos com falha, após os quais este dispositivo é reinicializado. Funciona apenas em dispositivos com acesso root.</t>
+  </si>
+  <si>
+    <t>IP-адрес для пингов</t>
+  </si>
+  <si>
+    <t>IP-адрес или имя хоста сетевого устройства, которое необходимо проверить на наличие сторожевого таймера. Если адрес не введен, сторожевой таймер сети отключается.</t>
+  </si>
+  <si>
+    <t>Задержка между пингами (в с)</t>
+  </si>
+  <si>
+    <t>Задержка в секундах между последовательными пингами.&lt;br&gt;&lt;i&gt;Для применения этого изменения требуется перезагрузка.&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>Количество неудачных пингов для перезагрузки</t>
+  </si>
+  <si>
+    <t>Количество последовательных неудачных попыток проверки связи, после которых устройство перезагружается. Работает только на рутованных устройствах.</t>
+  </si>
+  <si>
+    <t>IP naslov za pinge</t>
+  </si>
+  <si>
+    <t>Naslov IP ali ime gostitelja omrežne naprave, ki jo je treba pingati za čuvaja. Če naslov ni vnesen, je nadzornik omrežja izklopljen.</t>
+  </si>
+  <si>
+    <t>Zakasnitev med pingi (v s)</t>
+  </si>
+  <si>
+    <t>Zakasnitev v sekundah med zaporednimi pingi.&lt;br&gt;&lt;i&gt;Za uveljavitev te spremembe je potrebno ponovno nalaganje.&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>Število neuspešnih pingov za ponovni zagon</t>
+  </si>
+  <si>
+    <t>Število zaporednih neuspelih pingov, po katerih se ta naprava znova zažene. Deluje samo na zakoreninjenih napravah.</t>
+  </si>
+  <si>
+    <t>Dirección IP para pings</t>
+  </si>
+  <si>
+    <t>Dirección IP o nombre de host de un dispositivo de red al que se debe hacer ping para el mecanismo de vigilancia. Si no se ingresa ninguna dirección, el mecanismo de vigilancia de la red se desactiva.</t>
+  </si>
+  <si>
+    <t>Retraso entre pings (en s)</t>
+  </si>
+  <si>
+    <t>Retraso en segundos entre pings consecutivos.&lt;br&gt;&lt;i&gt;Es necesario recargar para aplicar este cambio.&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>No. de pings fallidos para reiniciar</t>
+  </si>
+  <si>
+    <t>Número de pings fallidos consecutivos, después de los cuales se reinicia este dispositivo. Funciona sólo en dispositivos rooteados.</t>
+  </si>
+  <si>
+    <t>Pingler için IP adresi</t>
+  </si>
+  <si>
+    <t>İzleyici için ping atılması gereken bir ağ cihazının IP adresi veya ana bilgisayar adı. Hiçbir adres girilmezse ağ gözlemcisi kapatılır.</t>
+  </si>
+  <si>
+    <t>Pingler arasındaki gecikme (sn)</t>
+  </si>
+  <si>
+    <t>Ardışık ping'ler arasında saniye cinsinden gecikme.&lt;br&gt;&lt;i&gt;Bu değişikliğin uygulanması için yeniden yükleme gerekiyor.&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>Yeniden başlatma için başarısız ping sayısı</t>
+  </si>
+  <si>
+    <t>Bu cihazın yeniden başlatılmasından sonra gerçekleşen ardışık başarısız ping sayısı. Yalnızca root erişimli cihazlarda çalışır.</t>
+  </si>
+  <si>
+    <t>No. of failed pings for reboot</t>
+  </si>
+  <si>
+    <t>face_detection_control_awb_mode</t>
+  </si>
+  <si>
+    <t>face_detection_control_awb_mode_help</t>
+  </si>
+  <si>
+    <t>face_detection_exposure_compensation</t>
+  </si>
+  <si>
+    <t>face_detection_exposure_compensation_help</t>
+  </si>
+  <si>
+    <t>face_detection_detect_eyes</t>
+  </si>
+  <si>
+    <t>face_detection_detect_eyes_help</t>
+  </si>
+  <si>
+    <t>Detect eyes</t>
+  </si>
+  <si>
+    <t>Exposure compensation</t>
+  </si>
+  <si>
+    <t>White balance mode</t>
+  </si>
+  <si>
+    <t>Whether to detect eyes, in addition to faces. If enabled, the face detection process might take longer.</t>
+  </si>
+  <si>
+    <t>White balance mode of camera for taking pictures for face detection.</t>
+  </si>
+  <si>
+    <t>Adjustment to auto-exposure brightness of image for face detection.</t>
+  </si>
+  <si>
+    <t>Režim vyváženia bielej</t>
+  </si>
+  <si>
+    <t>Režim vyváženia bielej fotoaparátu na snímku na detekciu tváre.</t>
+  </si>
+  <si>
+    <t>Kompenzácia expozície</t>
+  </si>
+  <si>
+    <t>Úprava jasu automatickej expozície snímku na detekciu tváre.</t>
+  </si>
+  <si>
+    <t>Detekovať oči</t>
+  </si>
+  <si>
+    <t>Či okrem tvárí detekovať aj oči. Ak je táto možnosť povolená, proces rozpoznávania tváre môže trvať dlhšie.</t>
+  </si>
+  <si>
+    <t>Režim vyvážení bílé</t>
+  </si>
+  <si>
+    <t>Režim vyvážení bílé fotoaparátu na snímek pro detekci obličeje.</t>
+  </si>
+  <si>
+    <t>Kompenzace expozice</t>
+  </si>
+  <si>
+    <t>Úprava jasu automatické expozice snímek pro detekci obličeje.</t>
+  </si>
+  <si>
+    <t>Detekovat oči</t>
+  </si>
+  <si>
+    <t>Zda kromě tváří detekovat i oči. Pokud je tato možnost povolena, proces rozpoznávání obličeje může trvat déle.</t>
+  </si>
+  <si>
+    <t>Način balansa bijele boje</t>
+  </si>
+  <si>
+    <t>Bílá bilance režim fotoaparata za fotografování za detekci tváří.</t>
+  </si>
+  <si>
+    <t>Kompenzacija ekspozicije</t>
+  </si>
+  <si>
+    <t>Adjustment to auto-exposition jasný obraz pro detekci obrazu.</t>
+  </si>
+  <si>
+    <t>Otkrij oči</t>
+  </si>
+  <si>
+    <t>Treba li detektirati oči, osim lica. Pokud je omogućen, proces prepoznavanja lica može trajati duže.</t>
+  </si>
+  <si>
+    <t>Mode balance des blancs</t>
+  </si>
+  <si>
+    <t>La compensation d'exposition</t>
+  </si>
+  <si>
+    <t>Détecter les yeux</t>
+  </si>
+  <si>
+    <t>Weißabgleichmodus</t>
+  </si>
+  <si>
+    <t>Belichtungsausgleich</t>
+  </si>
+  <si>
+    <t>Augen erkennen</t>
+  </si>
+  <si>
+    <t>Modalità bilanciamento del bianco</t>
+  </si>
+  <si>
+    <t>Compensazione dell'esposizione</t>
+  </si>
+  <si>
+    <t>Rileva gli occhi</t>
+  </si>
+  <si>
+    <t>ホワイトバランスモード</t>
+  </si>
+  <si>
+    <t>顔検出用に撮影するカメラのホワイトバランスモード。</t>
+  </si>
+  <si>
+    <t>露出補正</t>
+  </si>
+  <si>
+    <t>顔検出用の画像の自動露出の明るさを調整します。</t>
+  </si>
+  <si>
+    <t>目を検出する</t>
+  </si>
+  <si>
+    <t>顔に加えて目を検出するかどうか。 有効にすると、顔検出プロセスに時間がかかる可能性があります。</t>
+  </si>
+  <si>
+    <t>Modalità di bilanciamento del bianco della fotocamera per scattare foto per il rilevamento dei volti.</t>
+  </si>
+  <si>
+    <t>Regolazione della luminosità dell'esposizione automatica dell'immagine per il rilevamento dei volti.</t>
+  </si>
+  <si>
+    <t>Se rilevare gli occhi, oltre ai volti. Se abilitato, il processo di rilevamento dei volti potrebbe richiedere più tempo.</t>
+  </si>
+  <si>
+    <t>Weißabgleichmodus der Kamera zum Aufnehmen von Bildern zur Gesichtserkennung.</t>
+  </si>
+  <si>
+    <t>Anpassung der automatischen Belichtungshelligkeit des Bildes zur Gesichtserkennung.</t>
+  </si>
+  <si>
+    <t>Ob zusätzlich zu Gesichtern auch Augen erkannt werden sollen. Wenn diese Option aktiviert ist, kann der Gesichtserkennungsprozess länger dauern.</t>
+  </si>
+  <si>
+    <t>Mode balance des blancs de l'appareil photo pour prendre des photos pour la détection des visages.</t>
+  </si>
+  <si>
+    <t>Ajustement de la luminosité de l'exposition automatique de l'image pour la détection des visages.</t>
+  </si>
+  <si>
+    <t>Que ce soit pour détecter les yeux, en plus des visages. S'il est activé, le processus de détection des visages peut prendre plus de temps.</t>
+  </si>
+  <si>
+    <t>Tryb balansu bieli</t>
+  </si>
+  <si>
+    <t>Tryb balansu bieli aparatu do robienia zdjęć w celu wykrywania twarzy.</t>
+  </si>
+  <si>
+    <t>Kompensacja ekspozycji</t>
+  </si>
+  <si>
+    <t>Regulacja jasności obrazu z automatyczną ekspozycją w celu wykrywania twarzy.</t>
+  </si>
+  <si>
+    <t>Wykryj oczy</t>
+  </si>
+  <si>
+    <t>Czy oprócz twarzy wykrywać oczy. Jeśli ta opcja jest włączona, proces wykrywania twarzy może trwać dłużej.</t>
+  </si>
+  <si>
+    <t>화이트 밸런스 모드</t>
+  </si>
+  <si>
+    <t>얼굴 인식을 위한 사진 촬영을 위한 카메라의 화이트 밸런스 모드입니다.</t>
+  </si>
+  <si>
+    <t>노출 보정</t>
+  </si>
+  <si>
+    <t>얼굴 감지를 위한 이미지 자동 노출 밝기 조정.</t>
+  </si>
+  <si>
+    <t>눈 감지</t>
+  </si>
+  <si>
+    <t>얼굴 외에 눈도 감지할지 여부입니다. 활성화하면 얼굴 인식 프로세스가 더 오래 걸릴 수 있습니다.</t>
+  </si>
+  <si>
+    <t>Modo de equilíbrio de branco</t>
+  </si>
+  <si>
+    <t>Modo de equilíbrio de branco da câmera para tirar fotos para detecção de rosto.</t>
+  </si>
+  <si>
+    <t>Compensação de exposição</t>
+  </si>
+  <si>
+    <t>Ajuste do brilho de exposição automática da imagem para detecção de rosto.</t>
+  </si>
+  <si>
+    <t>Detectar olhos</t>
+  </si>
+  <si>
+    <t>Seja para detectar olhos, além de rostos. Se ativado, o processo de detecção de rosto poderá demorar mais.</t>
+  </si>
+  <si>
+    <t>Режим баланса белого</t>
+  </si>
+  <si>
+    <t>Режим баланса белого камеры для съемки с распознаванием лиц.</t>
+  </si>
+  <si>
+    <t>Компенсация экспозиции</t>
+  </si>
+  <si>
+    <t>Регулировка автоэкспозиции яркости изображения для распознавания лиц.</t>
+  </si>
+  <si>
+    <t>Обнаружить глаза</t>
+  </si>
+  <si>
+    <t>Обнаруживать ли глаза помимо лиц. Если этот параметр включен, процесс обнаружения лиц может занять больше времени.</t>
+  </si>
+  <si>
+    <t>Način ravnovesja beline</t>
+  </si>
+  <si>
+    <t>Način ravnovesja beline kamere za fotografiranje za zaznavanje obrazov.</t>
+  </si>
+  <si>
+    <t>Kompenzacija osvetlitve</t>
+  </si>
+  <si>
+    <t>Prilagoditev svetlosti samodejne osvetlitve slike za zaznavanje obraza.</t>
+  </si>
+  <si>
+    <t>Zaznavanje oči</t>
+  </si>
+  <si>
+    <t>Ali naj poleg obrazov zazna tudi oči. Če je omogočeno, lahko postopek zaznavanja obrazov traja dlje.</t>
+  </si>
+  <si>
+    <t>Modo de equilibrio de blancos</t>
+  </si>
+  <si>
+    <t>Modo de balance de blancos de la cámara para tomar fotografías y detectar rostros.</t>
+  </si>
+  <si>
+    <t>Compensación de exposición</t>
+  </si>
+  <si>
+    <t>Ajuste del brillo de exposición automática de la imagen para la detección de rostros.</t>
+  </si>
+  <si>
+    <t>detectar ojos</t>
+  </si>
+  <si>
+    <t>Ya sea para detectar ojos, además de rostros. Si está habilitado, el proceso de detección de rostros puede tardar más.</t>
+  </si>
+  <si>
+    <t>Beyaz dengesi modu</t>
+  </si>
+  <si>
+    <t>Yüz algılama amacıyla fotoğraf çekmek için kameranın beyaz dengesi modu.</t>
+  </si>
+  <si>
+    <t>Pozlama telafisi</t>
+  </si>
+  <si>
+    <t>Yüz algılama için görüntünün otomatik pozlama parlaklığının ayarlanması.</t>
+  </si>
+  <si>
+    <t>Gözleri tespit et</t>
+  </si>
+  <si>
+    <t>Yüzlerin yanı sıra gözlerin de tespit edilip edilmeyeceği. Etkinleştirilirse yüz algılama işlemi daha uzun sürebilir.</t>
+  </si>
+  <si>
+    <t>mirror_image</t>
+  </si>
+  <si>
+    <t>Mirror image</t>
+  </si>
+  <si>
+    <t>Zrkadliť obraz</t>
+  </si>
+  <si>
+    <t>Aynadaki görüntü</t>
+  </si>
+  <si>
+    <t>Imagen de espejo</t>
+  </si>
+  <si>
+    <t>Zrcalna slika</t>
+  </si>
+  <si>
+    <t>Зеркальное изображение</t>
+  </si>
+  <si>
+    <t>Imagem espelhada</t>
+  </si>
+  <si>
+    <t>Odbicie lustrzane</t>
+  </si>
+  <si>
+    <t>미러 이미지</t>
+  </si>
+  <si>
+    <t>鏡像</t>
+  </si>
+  <si>
+    <t>Immagine riflessa</t>
+  </si>
+  <si>
+    <t>Spiegelbild</t>
+  </si>
+  <si>
+    <t>Image miroir</t>
+  </si>
+  <si>
+    <t>watchdog_ping_default_gateway</t>
+  </si>
+  <si>
+    <t>watchdog_ping_default_gateway_help</t>
+  </si>
+  <si>
+    <t>IP address or hostname of a network device that should be pinged for watchdog. If no address is entered, the network watchdog is turned off.&lt;br&gt;&lt;i&gt;Reload is required for applying this change.&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>IP adresa alebo doménové meno sieťového zariadenia, ktoré bude ping-ované pre watchdog. Ak nie je zadaná žiadna adresa, sieťový watchdog je vypnutý.&lt;br&gt;&lt;i&gt;Reštart aplikácie je vyžadovaný pre aplikovanie tohto nastavenia.&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>Ping default gateway</t>
+  </si>
+  <si>
+    <t>Use default gateway for watchdog pings. May be used instead of IP address for pings. Watchdog will be active only if the default gateway is known during the app's startup.&lt;br&gt;&lt;i&gt;Reload is required for applying this change.&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>Pingovať default gateway</t>
+  </si>
+  <si>
+    <t>Použiť default geteway na pingovanie pre watchdog, namiesto IP adresy na ping. Watchdog bude aktívny len ak je default gateway známy počas štartu tejto aplikácie.&lt;br&gt;&lt;i&gt;Reštart aplikácie je vyžadovaný pre aplikovanie tohto nastavenia.&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>Pingovat default gateway</t>
+  </si>
+  <si>
+    <t>Použít default geteway k pingování pro watchdog, místo IP adresy na ping. Watchdog bude aktivní pouze pokud je default gateway znám během startu této aplikace.&lt;br&gt;&lt;i&gt;Restart aplikace je vyžadován pro aplikování tohoto nastavení.&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>Ping-Standard-Gateway</t>
+  </si>
+  <si>
+    <t>Verwenden Sie das Standard-Gateway für Watchdog-Pings. Kann anstelle der IP-Adresse für Pings verwendet werden. Watchdog ist nur aktiv, wenn das Standard-Gateway beim Start der App bekannt ist.&lt;br&gt;&lt;i&gt;Um diese Änderung anzuwenden, ist ein Neuladen erforderlich.&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>Effettua il ping del gateway predefinito</t>
+  </si>
+  <si>
+    <t>Utilizza il gateway predefinito per i ping del watchdog. Può essere utilizzato al posto dell'indirizzo IP per i ping. Il watchdog sarà attivo solo se il gateway predefinito è noto durante l'avvio dell'app.&lt;br&gt;&lt;i&gt;È necessario ricaricare per applicare questa modifica.&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>デフォルトゲートウェイにpingを送信する</t>
+  </si>
+  <si>
+    <t>ウォッチドッグ ping にはデフォルト ゲートウェイを使用します。 ping の IP アドレスの代わりに使用できます。 ウォッチドッグは、アプリの起動時にデフォルト ゲートウェイがわかっている場合にのみアクティブになります。&lt;br&gt;&lt;i&gt;この変更を適用するにはリロードが必要です。&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>Ping 기본 게이트웨이</t>
+  </si>
+  <si>
+    <t>감시 핑에 기본 게이트웨이를 사용합니다. 핑을 위해 IP 주소 대신 사용될 수 있습니다. Watchdog은 앱 시작 중에 기본 게이트웨이가 알려진 경우에만 활성화됩니다.&lt;br&gt;&lt;i&gt;이 변경 사항을 적용하려면 새로고침이 필요합니다.&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>Pinguj bramę domyślną</t>
+  </si>
+  <si>
+    <t>Użyj domyślnej bramy dla pingów watchdoga. Może być używany zamiast adresu IP dla poleceń ping. Watchdog będzie aktywny tylko wtedy, gdy podczas uruchamiania aplikacji znana będzie brama domyślna.&lt;br&gt;&lt;i&gt;Aby zastosować tę zmianę, wymagane jest ponowne załadowanie.&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>Gateway padrão de ping</t>
+  </si>
+  <si>
+    <t>Use o gateway padrão para pings de watchdog. Pode ser usado em vez do endereço IP para pings. O Watchdog estará ativo somente se o gateway padrão for conhecido durante a inicialização do aplicativo.&lt;br&gt;&lt;i&gt;É necessário recarregar para aplicar esta alteração.&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>Ping шлюз по умолчанию</t>
+  </si>
+  <si>
+    <t>Используйте шлюз по умолчанию для проверки связи со сторожевым таймером. Может использоваться вместо IP-адреса для проверки связи. Сторожевой таймер будет активен, только если шлюз по умолчанию известен во время запуска приложения.&lt;br&gt;&lt;i&gt;Для применения этого изменения потребуется перезагрузка.&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>Ping privzeti prehod</t>
+  </si>
+  <si>
+    <t>Uporabi privzeti prehod za nadzorne pinge. Lahko se uporablja namesto naslova IP za pinge. Watchdog bo aktiven samo, če je med zagonom aplikacije znan privzeti prehod.&lt;br&gt;&lt;i&gt;Za uporabo te spremembe je potrebno ponovno nalaganje.&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>Hacer ping a la puerta de enlace predeterminada</t>
+  </si>
+  <si>
+    <t>Utilice la puerta de enlace predeterminada para los pings de vigilancia. Puede usarse en lugar de la dirección IP para pings. El mecanismo de vigilancia estará activo solo si se conoce la puerta de enlace predeterminada durante el inicio de la aplicación.&lt;br&gt;&lt;i&gt;Es necesario volver a cargar para aplicar este cambio.&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>Varsayılan ağ geçidine ping at</t>
+  </si>
+  <si>
+    <t>Watchdog ping'leri için varsayılan ağ geçidini kullanın. Ping'ler için IP adresi yerine kullanılabilir. Watchdog yalnızca uygulamanın başlatılması sırasında varsayılan ağ geçidi biliniyorsa etkin olacaktır.&lt;br&gt;&lt;i&gt;Bu değişikliğin uygulanması için yeniden yükleme gereklidir.&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Slideshow app has been successfully updated to a newer version. There are following changes in this version:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Added possibility to mirror camera image (see Edit content for type Video input)&lt;/li&gt;&lt;li&gt;Added network ping watchdog (see Device settings)&lt;/li&gt;&lt;li&gt;Added new setting Target folder from Flash drive (see menu Settings - Device settings)&lt;/li&gt;&lt;li&gt;Changed screen layout intervals check from every minute to every 10 seconds (screen layout interval can now be decimal number)&lt;/li&gt;&lt;li&gt;Enhanced Face detection with additional settings, status page and MQTT reporting&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;You can find documentation for features on &lt;a href="https://slideshow.digital/documentation/" target="_blank"&gt;https://slideshow.digital/documentation/&lt;/a&gt;  and watch tutorials on  &lt;a href="https://www.youtube.com/channel/UCJFSXCItojY4PS76JNr_pdQ" target="_blank"&gt;https://www.youtube.com/channel/UCJFSXCItojY4PS76JNr_pdQ&lt;/a&gt;.&lt;/p&gt;&lt;p&gt;If you like Slideshow app, you can support the development by rating the app on &lt;a href="https://play.google.com/store/apps/details?id=sk.mimac.slideshow" target="_blank"&gt;Google Play&lt;/a&gt; or buy us a &lt;a href="https://ko-fi.com/slideshow" target="_blank"&gt;coffee&lt;/a&gt;.&lt;/p&gt;&lt;span style='float:right'&gt;-- The Development team --&lt;/span&gt;</t>
   </si>
 </sst>
 </file>
@@ -41237,18 +42200,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P884"/>
+  <dimension ref="A1:P905"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B450" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B650" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D479" sqref="D479"/>
+      <selection pane="bottomRight" activeCell="D676" sqref="D676"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3"/>
   <cols>
-    <col min="1" max="1" width="41.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="49.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.7109375" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" customWidth="1"/>
     <col min="4" max="4" width="32.140625" customWidth="1"/>
@@ -64970,7 +65933,7 @@
         <v>1644</v>
       </c>
       <c r="D475" t="s">
-        <v>13604</v>
+        <v>13603</v>
       </c>
       <c r="E475" t="s">
         <v>2735</v>
@@ -75020,7 +75983,7 @@
         <v>13003</v>
       </c>
       <c r="D676" t="s">
-        <v>13603</v>
+        <v>13925</v>
       </c>
       <c r="E676" t="s">
         <v>12993</v>
@@ -85457,6 +86420,1056 @@
       </c>
       <c r="P884" t="s">
         <v>13602</v>
+      </c>
+    </row>
+    <row r="885" spans="1:16">
+      <c r="A885" t="s">
+        <v>13604</v>
+      </c>
+      <c r="B885" t="s">
+        <v>13631</v>
+      </c>
+      <c r="C885" t="s">
+        <v>13693</v>
+      </c>
+      <c r="D885" t="s">
+        <v>13610</v>
+      </c>
+      <c r="E885" t="s">
+        <v>13625</v>
+      </c>
+      <c r="F885" t="s">
+        <v>13619</v>
+      </c>
+      <c r="G885" t="s">
+        <v>13637</v>
+      </c>
+      <c r="H885" t="s">
+        <v>13643</v>
+      </c>
+      <c r="I885" t="s">
+        <v>13649</v>
+      </c>
+      <c r="J885" t="s">
+        <v>13655</v>
+      </c>
+      <c r="K885" t="s">
+        <v>13661</v>
+      </c>
+      <c r="L885" t="s">
+        <v>13667</v>
+      </c>
+      <c r="M885" t="s">
+        <v>13692</v>
+      </c>
+      <c r="N885" t="s">
+        <v>13673</v>
+      </c>
+      <c r="O885" t="s">
+        <v>13679</v>
+      </c>
+      <c r="P885" t="s">
+        <v>13685</v>
+      </c>
+    </row>
+    <row r="886" spans="1:16">
+      <c r="A886" t="s">
+        <v>13605</v>
+      </c>
+      <c r="B886" t="s">
+        <v>13632</v>
+      </c>
+      <c r="C886" t="s">
+        <v>13694</v>
+      </c>
+      <c r="D886" t="s">
+        <v>13699</v>
+      </c>
+      <c r="E886" t="s">
+        <v>13626</v>
+      </c>
+      <c r="F886" t="s">
+        <v>13620</v>
+      </c>
+      <c r="G886" t="s">
+        <v>13638</v>
+      </c>
+      <c r="H886" t="s">
+        <v>13644</v>
+      </c>
+      <c r="I886" t="s">
+        <v>13650</v>
+      </c>
+      <c r="J886" t="s">
+        <v>13656</v>
+      </c>
+      <c r="K886" t="s">
+        <v>13662</v>
+      </c>
+      <c r="L886" t="s">
+        <v>13668</v>
+      </c>
+      <c r="M886" t="s">
+        <v>13615</v>
+      </c>
+      <c r="N886" t="s">
+        <v>13674</v>
+      </c>
+      <c r="O886" t="s">
+        <v>13680</v>
+      </c>
+      <c r="P886" t="s">
+        <v>13686</v>
+      </c>
+    </row>
+    <row r="887" spans="1:16">
+      <c r="A887" t="s">
+        <v>13606</v>
+      </c>
+      <c r="B887" t="s">
+        <v>13633</v>
+      </c>
+      <c r="C887" t="s">
+        <v>13695</v>
+      </c>
+      <c r="D887" t="s">
+        <v>13611</v>
+      </c>
+      <c r="E887" t="s">
+        <v>13627</v>
+      </c>
+      <c r="F887" t="s">
+        <v>13621</v>
+      </c>
+      <c r="G887" t="s">
+        <v>13639</v>
+      </c>
+      <c r="H887" t="s">
+        <v>13645</v>
+      </c>
+      <c r="I887" t="s">
+        <v>13651</v>
+      </c>
+      <c r="J887" t="s">
+        <v>13657</v>
+      </c>
+      <c r="K887" t="s">
+        <v>13663</v>
+      </c>
+      <c r="L887" t="s">
+        <v>13669</v>
+      </c>
+      <c r="M887" t="s">
+        <v>13616</v>
+      </c>
+      <c r="N887" t="s">
+        <v>13675</v>
+      </c>
+      <c r="O887" t="s">
+        <v>13681</v>
+      </c>
+      <c r="P887" t="s">
+        <v>13687</v>
+      </c>
+    </row>
+    <row r="888" spans="1:16">
+      <c r="A888" t="s">
+        <v>13607</v>
+      </c>
+      <c r="B888" t="s">
+        <v>13634</v>
+      </c>
+      <c r="C888" t="s">
+        <v>13696</v>
+      </c>
+      <c r="D888" t="s">
+        <v>13612</v>
+      </c>
+      <c r="E888" t="s">
+        <v>13628</v>
+      </c>
+      <c r="F888" t="s">
+        <v>13622</v>
+      </c>
+      <c r="G888" t="s">
+        <v>13640</v>
+      </c>
+      <c r="H888" t="s">
+        <v>13646</v>
+      </c>
+      <c r="I888" t="s">
+        <v>13652</v>
+      </c>
+      <c r="J888" t="s">
+        <v>13658</v>
+      </c>
+      <c r="K888" t="s">
+        <v>13664</v>
+      </c>
+      <c r="L888" t="s">
+        <v>13670</v>
+      </c>
+      <c r="M888" t="s">
+        <v>13614</v>
+      </c>
+      <c r="N888" t="s">
+        <v>13676</v>
+      </c>
+      <c r="O888" t="s">
+        <v>13682</v>
+      </c>
+      <c r="P888" t="s">
+        <v>13688</v>
+      </c>
+    </row>
+    <row r="889" spans="1:16">
+      <c r="A889" t="s">
+        <v>13608</v>
+      </c>
+      <c r="B889" t="s">
+        <v>13635</v>
+      </c>
+      <c r="C889" t="s">
+        <v>13697</v>
+      </c>
+      <c r="D889" t="s">
+        <v>13613</v>
+      </c>
+      <c r="E889" t="s">
+        <v>13629</v>
+      </c>
+      <c r="F889" t="s">
+        <v>13623</v>
+      </c>
+      <c r="G889" t="s">
+        <v>13641</v>
+      </c>
+      <c r="H889" t="s">
+        <v>13647</v>
+      </c>
+      <c r="I889" t="s">
+        <v>13653</v>
+      </c>
+      <c r="J889" t="s">
+        <v>13659</v>
+      </c>
+      <c r="K889" t="s">
+        <v>13665</v>
+      </c>
+      <c r="L889" t="s">
+        <v>13671</v>
+      </c>
+      <c r="M889" t="s">
+        <v>13691</v>
+      </c>
+      <c r="N889" t="s">
+        <v>13677</v>
+      </c>
+      <c r="O889" t="s">
+        <v>13683</v>
+      </c>
+      <c r="P889" t="s">
+        <v>13689</v>
+      </c>
+    </row>
+    <row r="890" spans="1:16">
+      <c r="A890" t="s">
+        <v>13609</v>
+      </c>
+      <c r="B890" t="s">
+        <v>13636</v>
+      </c>
+      <c r="C890" t="s">
+        <v>13698</v>
+      </c>
+      <c r="D890" t="s">
+        <v>13618</v>
+      </c>
+      <c r="E890" t="s">
+        <v>13630</v>
+      </c>
+      <c r="F890" t="s">
+        <v>13624</v>
+      </c>
+      <c r="G890" t="s">
+        <v>13642</v>
+      </c>
+      <c r="H890" t="s">
+        <v>13648</v>
+      </c>
+      <c r="I890" t="s">
+        <v>13654</v>
+      </c>
+      <c r="J890" t="s">
+        <v>13660</v>
+      </c>
+      <c r="K890" t="s">
+        <v>13666</v>
+      </c>
+      <c r="L890" t="s">
+        <v>13672</v>
+      </c>
+      <c r="M890" t="s">
+        <v>13617</v>
+      </c>
+      <c r="N890" t="s">
+        <v>13678</v>
+      </c>
+      <c r="O890" t="s">
+        <v>13684</v>
+      </c>
+      <c r="P890" t="s">
+        <v>13690</v>
+      </c>
+    </row>
+    <row r="891" spans="1:16">
+      <c r="A891" t="s">
+        <v>13700</v>
+      </c>
+      <c r="B891" t="s">
+        <v>13711</v>
+      </c>
+      <c r="C891" t="s">
+        <v>13712</v>
+      </c>
+      <c r="D891" t="s">
+        <v>13711</v>
+      </c>
+      <c r="E891" t="s">
+        <v>13742</v>
+      </c>
+      <c r="F891" t="s">
+        <v>13736</v>
+      </c>
+      <c r="G891" t="s">
+        <v>13730</v>
+      </c>
+      <c r="H891" t="s">
+        <v>13724</v>
+      </c>
+      <c r="I891" t="s">
+        <v>13718</v>
+      </c>
+      <c r="J891" t="s">
+        <v>13748</v>
+      </c>
+      <c r="K891" t="s">
+        <v>13754</v>
+      </c>
+      <c r="L891" t="s">
+        <v>13760</v>
+      </c>
+      <c r="M891" t="s">
+        <v>13712</v>
+      </c>
+      <c r="N891" t="s">
+        <v>13766</v>
+      </c>
+      <c r="O891" t="s">
+        <v>13772</v>
+      </c>
+      <c r="P891" t="s">
+        <v>13778</v>
+      </c>
+    </row>
+    <row r="892" spans="1:16">
+      <c r="A892" t="s">
+        <v>13701</v>
+      </c>
+      <c r="B892" t="s">
+        <v>13706</v>
+      </c>
+      <c r="C892" t="s">
+        <v>13715</v>
+      </c>
+      <c r="D892" t="s">
+        <v>13897</v>
+      </c>
+      <c r="E892" t="s">
+        <v>13743</v>
+      </c>
+      <c r="F892" t="s">
+        <v>13737</v>
+      </c>
+      <c r="G892" t="s">
+        <v>13731</v>
+      </c>
+      <c r="H892" t="s">
+        <v>13725</v>
+      </c>
+      <c r="I892" t="s">
+        <v>13719</v>
+      </c>
+      <c r="J892" t="s">
+        <v>13749</v>
+      </c>
+      <c r="K892" t="s">
+        <v>13755</v>
+      </c>
+      <c r="L892" t="s">
+        <v>13761</v>
+      </c>
+      <c r="M892" t="s">
+        <v>13898</v>
+      </c>
+      <c r="N892" t="s">
+        <v>13767</v>
+      </c>
+      <c r="O892" t="s">
+        <v>13773</v>
+      </c>
+      <c r="P892" t="s">
+        <v>13779</v>
+      </c>
+    </row>
+    <row r="893" spans="1:16">
+      <c r="A893" t="s">
+        <v>13703</v>
+      </c>
+      <c r="B893" t="s">
+        <v>13709</v>
+      </c>
+      <c r="C893" t="s">
+        <v>13716</v>
+      </c>
+      <c r="D893" t="s">
+        <v>13709</v>
+      </c>
+      <c r="E893" t="s">
+        <v>13744</v>
+      </c>
+      <c r="F893" t="s">
+        <v>13738</v>
+      </c>
+      <c r="G893" t="s">
+        <v>13732</v>
+      </c>
+      <c r="H893" t="s">
+        <v>13726</v>
+      </c>
+      <c r="I893" t="s">
+        <v>13720</v>
+      </c>
+      <c r="J893" t="s">
+        <v>13750</v>
+      </c>
+      <c r="K893" t="s">
+        <v>13756</v>
+      </c>
+      <c r="L893" t="s">
+        <v>13762</v>
+      </c>
+      <c r="M893" t="s">
+        <v>13716</v>
+      </c>
+      <c r="N893" t="s">
+        <v>13768</v>
+      </c>
+      <c r="O893" t="s">
+        <v>13774</v>
+      </c>
+      <c r="P893" t="s">
+        <v>13780</v>
+      </c>
+    </row>
+    <row r="894" spans="1:16">
+      <c r="A894" t="s">
+        <v>13702</v>
+      </c>
+      <c r="B894" t="s">
+        <v>13707</v>
+      </c>
+      <c r="C894" t="s">
+        <v>13717</v>
+      </c>
+      <c r="D894" t="s">
+        <v>13707</v>
+      </c>
+      <c r="E894" t="s">
+        <v>13745</v>
+      </c>
+      <c r="F894" t="s">
+        <v>13739</v>
+      </c>
+      <c r="G894" t="s">
+        <v>13733</v>
+      </c>
+      <c r="H894" t="s">
+        <v>13727</v>
+      </c>
+      <c r="I894" t="s">
+        <v>13721</v>
+      </c>
+      <c r="J894" t="s">
+        <v>13751</v>
+      </c>
+      <c r="K894" t="s">
+        <v>13757</v>
+      </c>
+      <c r="L894" t="s">
+        <v>13763</v>
+      </c>
+      <c r="M894" t="s">
+        <v>13717</v>
+      </c>
+      <c r="N894" t="s">
+        <v>13769</v>
+      </c>
+      <c r="O894" t="s">
+        <v>13775</v>
+      </c>
+      <c r="P894" t="s">
+        <v>13781</v>
+      </c>
+    </row>
+    <row r="895" spans="1:16">
+      <c r="A895" t="s">
+        <v>13704</v>
+      </c>
+      <c r="B895" t="s">
+        <v>13710</v>
+      </c>
+      <c r="C895" t="s">
+        <v>13713</v>
+      </c>
+      <c r="D895" t="s">
+        <v>13784</v>
+      </c>
+      <c r="E895" t="s">
+        <v>13746</v>
+      </c>
+      <c r="F895" t="s">
+        <v>13740</v>
+      </c>
+      <c r="G895" t="s">
+        <v>13734</v>
+      </c>
+      <c r="H895" t="s">
+        <v>13728</v>
+      </c>
+      <c r="I895" t="s">
+        <v>13722</v>
+      </c>
+      <c r="J895" t="s">
+        <v>13752</v>
+      </c>
+      <c r="K895" t="s">
+        <v>13758</v>
+      </c>
+      <c r="L895" t="s">
+        <v>13764</v>
+      </c>
+      <c r="M895" t="s">
+        <v>13713</v>
+      </c>
+      <c r="N895" t="s">
+        <v>13770</v>
+      </c>
+      <c r="O895" t="s">
+        <v>13776</v>
+      </c>
+      <c r="P895" t="s">
+        <v>13782</v>
+      </c>
+    </row>
+    <row r="896" spans="1:16">
+      <c r="A896" t="s">
+        <v>13705</v>
+      </c>
+      <c r="B896" t="s">
+        <v>13708</v>
+      </c>
+      <c r="C896" t="s">
+        <v>13714</v>
+      </c>
+      <c r="D896" t="s">
+        <v>13708</v>
+      </c>
+      <c r="E896" t="s">
+        <v>13747</v>
+      </c>
+      <c r="F896" t="s">
+        <v>13741</v>
+      </c>
+      <c r="G896" t="s">
+        <v>13735</v>
+      </c>
+      <c r="H896" t="s">
+        <v>13729</v>
+      </c>
+      <c r="I896" t="s">
+        <v>13723</v>
+      </c>
+      <c r="J896" t="s">
+        <v>13753</v>
+      </c>
+      <c r="K896" t="s">
+        <v>13759</v>
+      </c>
+      <c r="L896" t="s">
+        <v>13765</v>
+      </c>
+      <c r="M896" t="s">
+        <v>13714</v>
+      </c>
+      <c r="N896" t="s">
+        <v>13771</v>
+      </c>
+      <c r="O896" t="s">
+        <v>13777</v>
+      </c>
+      <c r="P896" t="s">
+        <v>13783</v>
+      </c>
+    </row>
+    <row r="897" spans="1:16">
+      <c r="A897" t="s">
+        <v>13785</v>
+      </c>
+      <c r="B897" t="s">
+        <v>13809</v>
+      </c>
+      <c r="C897" t="s">
+        <v>13803</v>
+      </c>
+      <c r="D897" t="s">
+        <v>13793</v>
+      </c>
+      <c r="E897" t="s">
+        <v>13815</v>
+      </c>
+      <c r="F897" t="s">
+        <v>13818</v>
+      </c>
+      <c r="G897" t="s">
+        <v>13821</v>
+      </c>
+      <c r="H897" t="s">
+        <v>13824</v>
+      </c>
+      <c r="I897" t="s">
+        <v>13845</v>
+      </c>
+      <c r="J897" t="s">
+        <v>13839</v>
+      </c>
+      <c r="K897" t="s">
+        <v>13851</v>
+      </c>
+      <c r="L897" t="s">
+        <v>13857</v>
+      </c>
+      <c r="M897" t="s">
+        <v>13797</v>
+      </c>
+      <c r="N897" t="s">
+        <v>13863</v>
+      </c>
+      <c r="O897" t="s">
+        <v>13869</v>
+      </c>
+      <c r="P897" t="s">
+        <v>13875</v>
+      </c>
+    </row>
+    <row r="898" spans="1:16">
+      <c r="A898" t="s">
+        <v>13786</v>
+      </c>
+      <c r="B898" t="s">
+        <v>13810</v>
+      </c>
+      <c r="C898" t="s">
+        <v>13804</v>
+      </c>
+      <c r="D898" t="s">
+        <v>13795</v>
+      </c>
+      <c r="E898" t="s">
+        <v>13836</v>
+      </c>
+      <c r="F898" t="s">
+        <v>13833</v>
+      </c>
+      <c r="G898" t="s">
+        <v>13830</v>
+      </c>
+      <c r="H898" t="s">
+        <v>13825</v>
+      </c>
+      <c r="I898" t="s">
+        <v>13846</v>
+      </c>
+      <c r="J898" t="s">
+        <v>13840</v>
+      </c>
+      <c r="K898" t="s">
+        <v>13852</v>
+      </c>
+      <c r="L898" t="s">
+        <v>13858</v>
+      </c>
+      <c r="M898" t="s">
+        <v>13798</v>
+      </c>
+      <c r="N898" t="s">
+        <v>13864</v>
+      </c>
+      <c r="O898" t="s">
+        <v>13870</v>
+      </c>
+      <c r="P898" t="s">
+        <v>13876</v>
+      </c>
+    </row>
+    <row r="899" spans="1:16">
+      <c r="A899" t="s">
+        <v>13787</v>
+      </c>
+      <c r="B899" t="s">
+        <v>13811</v>
+      </c>
+      <c r="C899" t="s">
+        <v>13805</v>
+      </c>
+      <c r="D899" t="s">
+        <v>13792</v>
+      </c>
+      <c r="E899" t="s">
+        <v>13816</v>
+      </c>
+      <c r="F899" t="s">
+        <v>13819</v>
+      </c>
+      <c r="G899" t="s">
+        <v>13822</v>
+      </c>
+      <c r="H899" t="s">
+        <v>13826</v>
+      </c>
+      <c r="I899" t="s">
+        <v>13847</v>
+      </c>
+      <c r="J899" t="s">
+        <v>13841</v>
+      </c>
+      <c r="K899" t="s">
+        <v>13853</v>
+      </c>
+      <c r="L899" t="s">
+        <v>13859</v>
+      </c>
+      <c r="M899" t="s">
+        <v>13799</v>
+      </c>
+      <c r="N899" t="s">
+        <v>13865</v>
+      </c>
+      <c r="O899" t="s">
+        <v>13871</v>
+      </c>
+      <c r="P899" t="s">
+        <v>13877</v>
+      </c>
+    </row>
+    <row r="900" spans="1:16">
+      <c r="A900" t="s">
+        <v>13788</v>
+      </c>
+      <c r="B900" t="s">
+        <v>13812</v>
+      </c>
+      <c r="C900" t="s">
+        <v>13806</v>
+      </c>
+      <c r="D900" t="s">
+        <v>13796</v>
+      </c>
+      <c r="E900" t="s">
+        <v>13837</v>
+      </c>
+      <c r="F900" t="s">
+        <v>13834</v>
+      </c>
+      <c r="G900" t="s">
+        <v>13831</v>
+      </c>
+      <c r="H900" t="s">
+        <v>13827</v>
+      </c>
+      <c r="I900" t="s">
+        <v>13848</v>
+      </c>
+      <c r="J900" t="s">
+        <v>13842</v>
+      </c>
+      <c r="K900" t="s">
+        <v>13854</v>
+      </c>
+      <c r="L900" t="s">
+        <v>13860</v>
+      </c>
+      <c r="M900" t="s">
+        <v>13800</v>
+      </c>
+      <c r="N900" t="s">
+        <v>13866</v>
+      </c>
+      <c r="O900" t="s">
+        <v>13872</v>
+      </c>
+      <c r="P900" t="s">
+        <v>13878</v>
+      </c>
+    </row>
+    <row r="901" spans="1:16">
+      <c r="A901" t="s">
+        <v>13789</v>
+      </c>
+      <c r="B901" t="s">
+        <v>13813</v>
+      </c>
+      <c r="C901" t="s">
+        <v>13807</v>
+      </c>
+      <c r="D901" t="s">
+        <v>13791</v>
+      </c>
+      <c r="E901" t="s">
+        <v>13817</v>
+      </c>
+      <c r="F901" t="s">
+        <v>13820</v>
+      </c>
+      <c r="G901" t="s">
+        <v>13823</v>
+      </c>
+      <c r="H901" t="s">
+        <v>13828</v>
+      </c>
+      <c r="I901" t="s">
+        <v>13849</v>
+      </c>
+      <c r="J901" t="s">
+        <v>13843</v>
+      </c>
+      <c r="K901" t="s">
+        <v>13855</v>
+      </c>
+      <c r="L901" t="s">
+        <v>13861</v>
+      </c>
+      <c r="M901" t="s">
+        <v>13801</v>
+      </c>
+      <c r="N901" t="s">
+        <v>13867</v>
+      </c>
+      <c r="O901" t="s">
+        <v>13873</v>
+      </c>
+      <c r="P901" t="s">
+        <v>13879</v>
+      </c>
+    </row>
+    <row r="902" spans="1:16">
+      <c r="A902" t="s">
+        <v>13790</v>
+      </c>
+      <c r="B902" t="s">
+        <v>13814</v>
+      </c>
+      <c r="C902" t="s">
+        <v>13808</v>
+      </c>
+      <c r="D902" t="s">
+        <v>13794</v>
+      </c>
+      <c r="E902" t="s">
+        <v>13838</v>
+      </c>
+      <c r="F902" t="s">
+        <v>13835</v>
+      </c>
+      <c r="G902" t="s">
+        <v>13832</v>
+      </c>
+      <c r="H902" t="s">
+        <v>13829</v>
+      </c>
+      <c r="I902" t="s">
+        <v>13850</v>
+      </c>
+      <c r="J902" t="s">
+        <v>13844</v>
+      </c>
+      <c r="K902" t="s">
+        <v>13856</v>
+      </c>
+      <c r="L902" t="s">
+        <v>13862</v>
+      </c>
+      <c r="M902" t="s">
+        <v>13802</v>
+      </c>
+      <c r="N902" t="s">
+        <v>13868</v>
+      </c>
+      <c r="O902" t="s">
+        <v>13874</v>
+      </c>
+      <c r="P902" t="s">
+        <v>13880</v>
+      </c>
+    </row>
+    <row r="903" spans="1:16">
+      <c r="A903" t="s">
+        <v>13881</v>
+      </c>
+      <c r="B903" t="s">
+        <v>13886</v>
+      </c>
+      <c r="C903" t="s">
+        <v>13883</v>
+      </c>
+      <c r="D903" t="s">
+        <v>13882</v>
+      </c>
+      <c r="E903" t="s">
+        <v>13894</v>
+      </c>
+      <c r="F903" t="s">
+        <v>13893</v>
+      </c>
+      <c r="G903" t="s">
+        <v>13892</v>
+      </c>
+      <c r="H903" t="s">
+        <v>13891</v>
+      </c>
+      <c r="I903" t="s">
+        <v>13890</v>
+      </c>
+      <c r="J903" t="s">
+        <v>13889</v>
+      </c>
+      <c r="K903" t="s">
+        <v>13888</v>
+      </c>
+      <c r="L903" t="s">
+        <v>13887</v>
+      </c>
+      <c r="M903" t="s">
+        <v>13883</v>
+      </c>
+      <c r="N903" t="s">
+        <v>13886</v>
+      </c>
+      <c r="O903" t="s">
+        <v>13885</v>
+      </c>
+      <c r="P903" t="s">
+        <v>13884</v>
+      </c>
+    </row>
+    <row r="904" spans="1:16">
+      <c r="A904" t="s">
+        <v>13895</v>
+      </c>
+      <c r="B904" t="s">
+        <v>13899</v>
+      </c>
+      <c r="C904" t="s">
+        <v>13903</v>
+      </c>
+      <c r="D904" t="s">
+        <v>13899</v>
+      </c>
+      <c r="E904" t="s">
+        <v>13899</v>
+      </c>
+      <c r="F904" t="s">
+        <v>13905</v>
+      </c>
+      <c r="G904" t="s">
+        <v>13907</v>
+      </c>
+      <c r="H904" t="s">
+        <v>13909</v>
+      </c>
+      <c r="I904" t="s">
+        <v>13911</v>
+      </c>
+      <c r="J904" t="s">
+        <v>13913</v>
+      </c>
+      <c r="K904" t="s">
+        <v>13915</v>
+      </c>
+      <c r="L904" t="s">
+        <v>13917</v>
+      </c>
+      <c r="M904" t="s">
+        <v>13901</v>
+      </c>
+      <c r="N904" t="s">
+        <v>13919</v>
+      </c>
+      <c r="O904" t="s">
+        <v>13921</v>
+      </c>
+      <c r="P904" t="s">
+        <v>13923</v>
+      </c>
+    </row>
+    <row r="905" spans="1:16">
+      <c r="A905" t="s">
+        <v>13896</v>
+      </c>
+      <c r="B905" t="s">
+        <v>13900</v>
+      </c>
+      <c r="C905" t="s">
+        <v>13904</v>
+      </c>
+      <c r="D905" t="s">
+        <v>13900</v>
+      </c>
+      <c r="E905" t="s">
+        <v>13900</v>
+      </c>
+      <c r="F905" t="s">
+        <v>13906</v>
+      </c>
+      <c r="G905" t="s">
+        <v>13908</v>
+      </c>
+      <c r="H905" t="s">
+        <v>13910</v>
+      </c>
+      <c r="I905" t="s">
+        <v>13912</v>
+      </c>
+      <c r="J905" t="s">
+        <v>13914</v>
+      </c>
+      <c r="K905" t="s">
+        <v>13916</v>
+      </c>
+      <c r="L905" t="s">
+        <v>13918</v>
+      </c>
+      <c r="M905" t="s">
+        <v>13902</v>
+      </c>
+      <c r="N905" t="s">
+        <v>13920</v>
+      </c>
+      <c r="O905" t="s">
+        <v>13922</v>
+      </c>
+      <c r="P905" t="s">
+        <v>13924</v>
       </c>
     </row>
   </sheetData>

</xml_diff>